<commit_message>
callbacks file added, feature merge of series from the same day
</commit_message>
<xml_diff>
--- a/time_spacing/words/words_V1.0.0.xlsx
+++ b/time_spacing/words/words_V1.0.0.xlsx
@@ -501,7 +501,7 @@
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D2" t="n">
         <v>2</v>
@@ -531,7 +531,7 @@
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D3" t="n">
         <v>7</v>
@@ -575,7 +575,7 @@
       <c r="G4" t="n">
         <v>1</v>
       </c>
-      <c r="H4" t="b">
+      <c r="H4" t="n">
         <v>1</v>
       </c>
       <c r="I4" t="inlineStr"/>
@@ -593,7 +593,7 @@
         </is>
       </c>
       <c r="C5" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D5" t="n">
         <v>7</v>
@@ -623,7 +623,7 @@
         </is>
       </c>
       <c r="C6" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D6" t="n">
         <v>5</v>
@@ -653,7 +653,7 @@
         </is>
       </c>
       <c r="C7" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D7" t="n">
         <v>4</v>
@@ -683,7 +683,7 @@
         </is>
       </c>
       <c r="C8" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -713,7 +713,7 @@
         </is>
       </c>
       <c r="C9" s="2" t="n">
-        <v>45377</v>
+        <v>45403</v>
       </c>
       <c r="D9" t="n">
         <v>5</v>
@@ -743,7 +743,7 @@
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>45380</v>
+        <v>45403</v>
       </c>
       <c r="D10" t="n">
         <v>8</v>
@@ -773,7 +773,7 @@
         </is>
       </c>
       <c r="C11" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D11" t="n">
         <v>4</v>
@@ -803,10 +803,10 @@
         </is>
       </c>
       <c r="C12" s="2" t="n">
-        <v>45389</v>
+        <v>45418</v>
       </c>
       <c r="D12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
@@ -815,12 +815,14 @@
         <v>1</v>
       </c>
       <c r="G12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12" t="n">
-        <v>1</v>
-      </c>
-      <c r="I12" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1</v>
+      </c>
       <c r="J12" t="inlineStr"/>
     </row>
     <row r="13">
@@ -835,7 +837,7 @@
         </is>
       </c>
       <c r="C13" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D13" t="n">
         <v>4</v>
@@ -865,7 +867,7 @@
         </is>
       </c>
       <c r="C14" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D14" t="n">
         <v>7</v>
@@ -895,7 +897,7 @@
         </is>
       </c>
       <c r="C15" s="2" t="n">
-        <v>45391</v>
+        <v>45403</v>
       </c>
       <c r="D15" t="n">
         <v>5</v>
@@ -927,7 +929,7 @@
         </is>
       </c>
       <c r="C16" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D16" t="n">
         <v>7</v>
@@ -957,7 +959,7 @@
         </is>
       </c>
       <c r="C17" s="2" t="n">
-        <v>45394</v>
+        <v>45403</v>
       </c>
       <c r="D17" t="n">
         <v>8</v>
@@ -989,7 +991,7 @@
         </is>
       </c>
       <c r="C18" s="2" t="n">
-        <v>45389</v>
+        <v>45403</v>
       </c>
       <c r="D18" t="n">
         <v>5</v>
@@ -1021,7 +1023,7 @@
         </is>
       </c>
       <c r="C19" s="2" t="n">
-        <v>45380</v>
+        <v>45403</v>
       </c>
       <c r="D19" t="n">
         <v>8</v>
@@ -1051,7 +1053,7 @@
         </is>
       </c>
       <c r="C20" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D20" t="n">
         <v>4</v>
@@ -1081,7 +1083,7 @@
         </is>
       </c>
       <c r="C21" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D21" t="n">
         <v>4</v>
@@ -1111,7 +1113,7 @@
         </is>
       </c>
       <c r="C22" s="2" t="n">
-        <v>45381</v>
+        <v>45403</v>
       </c>
       <c r="D22" t="n">
         <v>6</v>
@@ -1141,7 +1143,7 @@
         </is>
       </c>
       <c r="C23" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D23" t="n">
         <v>3</v>
@@ -1171,7 +1173,7 @@
         </is>
       </c>
       <c r="C24" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D24" t="n">
         <v>5</v>
@@ -1201,10 +1203,10 @@
         </is>
       </c>
       <c r="C25" s="2" t="n">
-        <v>45375</v>
+        <v>45431</v>
       </c>
       <c r="D25" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E25" t="b">
         <v>0</v>
@@ -1213,9 +1215,11 @@
         <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>0</v>
-      </c>
-      <c r="H25" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
     </row>
@@ -1231,7 +1235,7 @@
         </is>
       </c>
       <c r="C26" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D26" t="n">
         <v>7</v>
@@ -1261,7 +1265,7 @@
         </is>
       </c>
       <c r="C27" s="2" t="n">
-        <v>45394</v>
+        <v>45403</v>
       </c>
       <c r="D27" t="n">
         <v>8</v>
@@ -1293,7 +1297,7 @@
         </is>
       </c>
       <c r="C28" s="2" t="n">
-        <v>45401</v>
+        <v>45403</v>
       </c>
       <c r="D28" t="n">
         <v>5</v>
@@ -1307,7 +1311,7 @@
       <c r="G28" t="n">
         <v>1</v>
       </c>
-      <c r="H28" t="b">
+      <c r="H28" t="n">
         <v>1</v>
       </c>
       <c r="I28" t="inlineStr"/>
@@ -1325,7 +1329,7 @@
         </is>
       </c>
       <c r="C29" s="2" t="n">
-        <v>45401</v>
+        <v>45403</v>
       </c>
       <c r="D29" t="n">
         <v>7</v>
@@ -1355,7 +1359,7 @@
         </is>
       </c>
       <c r="C30" s="2" t="n">
-        <v>45398</v>
+        <v>45403</v>
       </c>
       <c r="D30" t="n">
         <v>8</v>
@@ -1387,7 +1391,7 @@
         </is>
       </c>
       <c r="C31" s="2" t="n">
-        <v>45380</v>
+        <v>45403</v>
       </c>
       <c r="D31" t="n">
         <v>4</v>
@@ -1419,7 +1423,7 @@
         </is>
       </c>
       <c r="C32" s="2" t="n">
-        <v>45384</v>
+        <v>45403</v>
       </c>
       <c r="D32" t="n">
         <v>4</v>
@@ -1451,7 +1455,7 @@
         </is>
       </c>
       <c r="C33" s="2" t="n">
-        <v>45398</v>
+        <v>45403</v>
       </c>
       <c r="D33" t="n">
         <v>8</v>
@@ -1483,7 +1487,7 @@
         </is>
       </c>
       <c r="C34" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D34" t="n">
         <v>4</v>
@@ -1513,21 +1517,23 @@
         </is>
       </c>
       <c r="C35" s="2" t="n">
-        <v>45375</v>
+        <v>45431</v>
       </c>
       <c r="D35" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E35" t="b">
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35" t="n">
-        <v>0</v>
-      </c>
-      <c r="H35" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H35" t="b">
+        <v>1</v>
+      </c>
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr"/>
     </row>
@@ -1543,7 +1549,7 @@
         </is>
       </c>
       <c r="C36" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D36" t="n">
         <v>4</v>
@@ -1573,7 +1579,7 @@
         </is>
       </c>
       <c r="C37" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D37" t="n">
         <v>3</v>
@@ -1603,7 +1609,7 @@
         </is>
       </c>
       <c r="C38" s="2" t="n">
-        <v>45392</v>
+        <v>45403</v>
       </c>
       <c r="D38" t="n">
         <v>8</v>
@@ -1635,7 +1641,7 @@
         </is>
       </c>
       <c r="C39" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D39" t="n">
         <v>7</v>
@@ -1665,7 +1671,7 @@
         </is>
       </c>
       <c r="C40" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D40" t="n">
         <v>4</v>
@@ -1695,7 +1701,7 @@
         </is>
       </c>
       <c r="C41" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D41" t="n">
         <v>2</v>
@@ -1727,10 +1733,10 @@
         </is>
       </c>
       <c r="C42" s="2" t="n">
-        <v>45375</v>
+        <v>45431</v>
       </c>
       <c r="D42" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E42" t="b">
         <v>0</v>
@@ -1739,9 +1745,11 @@
         <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>0</v>
-      </c>
-      <c r="H42" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H42" t="b">
+        <v>0</v>
+      </c>
       <c r="I42" t="inlineStr"/>
       <c r="J42" t="inlineStr"/>
     </row>
@@ -1757,7 +1765,7 @@
         </is>
       </c>
       <c r="C43" s="2" t="n">
-        <v>45389</v>
+        <v>45403</v>
       </c>
       <c r="D43" t="n">
         <v>5</v>
@@ -1789,7 +1797,7 @@
         </is>
       </c>
       <c r="C44" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D44" t="n">
         <v>4</v>
@@ -1819,7 +1827,7 @@
         </is>
       </c>
       <c r="C45" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D45" t="n">
         <v>7</v>
@@ -1849,10 +1857,10 @@
         </is>
       </c>
       <c r="C46" s="2" t="n">
-        <v>45375</v>
+        <v>45431</v>
       </c>
       <c r="D46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E46" t="b">
         <v>0</v>
@@ -1861,9 +1869,11 @@
         <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>0</v>
-      </c>
-      <c r="H46" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0</v>
+      </c>
       <c r="I46" t="inlineStr"/>
       <c r="J46" t="inlineStr"/>
     </row>
@@ -1879,7 +1889,7 @@
         </is>
       </c>
       <c r="C47" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D47" t="n">
         <v>3</v>
@@ -1909,7 +1919,7 @@
         </is>
       </c>
       <c r="C48" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D48" t="n">
         <v>3</v>
@@ -1939,7 +1949,7 @@
         </is>
       </c>
       <c r="C49" s="2" t="n">
-        <v>45377</v>
+        <v>45403</v>
       </c>
       <c r="D49" t="n">
         <v>2</v>
@@ -1953,7 +1963,7 @@
       <c r="G49" t="n">
         <v>1</v>
       </c>
-      <c r="H49" t="b">
+      <c r="H49" t="n">
         <v>0</v>
       </c>
       <c r="I49" t="inlineStr"/>
@@ -1971,10 +1981,10 @@
         </is>
       </c>
       <c r="C50" s="2" t="n">
-        <v>45379</v>
+        <v>45418</v>
       </c>
       <c r="D50" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E50" t="b">
         <v>0</v>
@@ -1983,9 +1993,11 @@
         <v>0</v>
       </c>
       <c r="G50" t="n">
-        <v>0</v>
-      </c>
-      <c r="H50" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H50" t="b">
+        <v>0</v>
+      </c>
       <c r="I50" t="inlineStr"/>
       <c r="J50" t="inlineStr"/>
     </row>
@@ -2001,7 +2013,7 @@
         </is>
       </c>
       <c r="C51" s="2" t="n">
-        <v>45393</v>
+        <v>45403</v>
       </c>
       <c r="D51" t="n">
         <v>5</v>
@@ -2033,7 +2045,7 @@
         </is>
       </c>
       <c r="C52" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D52" t="n">
         <v>3</v>
@@ -2063,7 +2075,7 @@
         </is>
       </c>
       <c r="C53" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D53" t="n">
         <v>3</v>
@@ -2093,7 +2105,7 @@
         </is>
       </c>
       <c r="C54" s="2" t="n">
-        <v>45379</v>
+        <v>45403</v>
       </c>
       <c r="D54" t="n">
         <v>5</v>
@@ -2123,7 +2135,7 @@
         </is>
       </c>
       <c r="C55" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D55" t="n">
         <v>7</v>
@@ -2153,7 +2165,7 @@
         </is>
       </c>
       <c r="C56" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D56" t="n">
         <v>4</v>
@@ -2183,7 +2195,7 @@
         </is>
       </c>
       <c r="C57" s="2" t="n">
-        <v>45392</v>
+        <v>45403</v>
       </c>
       <c r="D57" t="n">
         <v>8</v>
@@ -2215,7 +2227,7 @@
         </is>
       </c>
       <c r="C58" s="2" t="n">
-        <v>45395</v>
+        <v>45403</v>
       </c>
       <c r="D58" t="n">
         <v>7</v>
@@ -2245,7 +2257,7 @@
         </is>
       </c>
       <c r="C59" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D59" t="n">
         <v>7</v>
@@ -2275,7 +2287,7 @@
         </is>
       </c>
       <c r="C60" s="2" t="n">
-        <v>45384</v>
+        <v>45403</v>
       </c>
       <c r="D60" t="n">
         <v>4</v>
@@ -2321,7 +2333,7 @@
       <c r="G61" t="n">
         <v>1</v>
       </c>
-      <c r="H61" t="b">
+      <c r="H61" t="n">
         <v>1</v>
       </c>
       <c r="I61" t="inlineStr"/>
@@ -2339,7 +2351,7 @@
         </is>
       </c>
       <c r="C62" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D62" t="n">
         <v>4</v>
@@ -2369,7 +2381,7 @@
         </is>
       </c>
       <c r="C63" s="2" t="n">
-        <v>45398</v>
+        <v>45403</v>
       </c>
       <c r="D63" t="n">
         <v>7</v>
@@ -2399,7 +2411,7 @@
         </is>
       </c>
       <c r="C64" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D64" t="n">
         <v>4</v>
@@ -2429,7 +2441,7 @@
         </is>
       </c>
       <c r="C65" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D65" t="n">
         <v>7</v>
@@ -2459,7 +2471,7 @@
         </is>
       </c>
       <c r="C66" s="2" t="n">
-        <v>45391</v>
+        <v>45403</v>
       </c>
       <c r="D66" t="n">
         <v>5</v>
@@ -2491,7 +2503,7 @@
         </is>
       </c>
       <c r="C67" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D67" t="n">
         <v>2</v>
@@ -2523,7 +2535,7 @@
         </is>
       </c>
       <c r="C68" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D68" t="n">
         <v>4</v>
@@ -2553,7 +2565,7 @@
         </is>
       </c>
       <c r="C69" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D69" t="n">
         <v>4</v>
@@ -2583,7 +2595,7 @@
         </is>
       </c>
       <c r="C70" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D70" t="n">
         <v>7</v>
@@ -2613,7 +2625,7 @@
         </is>
       </c>
       <c r="C71" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D71" t="n">
         <v>1</v>
@@ -2645,7 +2657,7 @@
         </is>
       </c>
       <c r="C72" s="2" t="n">
-        <v>45401</v>
+        <v>45403</v>
       </c>
       <c r="D72" t="n">
         <v>5</v>
@@ -2659,7 +2671,7 @@
       <c r="G72" t="n">
         <v>1</v>
       </c>
-      <c r="H72" t="b">
+      <c r="H72" t="n">
         <v>1</v>
       </c>
       <c r="I72" t="inlineStr"/>
@@ -2677,7 +2689,7 @@
         </is>
       </c>
       <c r="C73" s="2" t="n">
-        <v>45398</v>
+        <v>45403</v>
       </c>
       <c r="D73" t="n">
         <v>8</v>
@@ -2709,7 +2721,7 @@
         </is>
       </c>
       <c r="C74" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D74" t="n">
         <v>3</v>
@@ -2739,7 +2751,7 @@
         </is>
       </c>
       <c r="C75" s="2" t="n">
-        <v>45380</v>
+        <v>45403</v>
       </c>
       <c r="D75" t="n">
         <v>4</v>
@@ -2771,7 +2783,7 @@
         </is>
       </c>
       <c r="C76" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D76" t="n">
         <v>2</v>
@@ -2801,7 +2813,7 @@
         </is>
       </c>
       <c r="C77" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D77" t="n">
         <v>3</v>
@@ -2831,7 +2843,7 @@
         </is>
       </c>
       <c r="C78" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D78" t="n">
         <v>7</v>
@@ -2861,7 +2873,7 @@
         </is>
       </c>
       <c r="C79" s="2" t="n">
-        <v>45395</v>
+        <v>45403</v>
       </c>
       <c r="D79" t="n">
         <v>5</v>
@@ -2893,7 +2905,7 @@
         </is>
       </c>
       <c r="C80" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D80" t="n">
         <v>7</v>
@@ -2923,7 +2935,7 @@
         </is>
       </c>
       <c r="C81" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D81" t="n">
         <v>7</v>
@@ -2953,7 +2965,7 @@
         </is>
       </c>
       <c r="C82" s="2" t="n">
-        <v>45394</v>
+        <v>45403</v>
       </c>
       <c r="D82" t="n">
         <v>8</v>
@@ -2985,7 +2997,7 @@
         </is>
       </c>
       <c r="C83" s="2" t="n">
-        <v>45378</v>
+        <v>45403</v>
       </c>
       <c r="D83" t="n">
         <v>4</v>
@@ -3017,7 +3029,7 @@
         </is>
       </c>
       <c r="C84" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D84" t="n">
         <v>4</v>
@@ -3047,7 +3059,7 @@
         </is>
       </c>
       <c r="C85" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D85" t="n">
         <v>4</v>
@@ -3077,7 +3089,7 @@
         </is>
       </c>
       <c r="C86" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D86" t="n">
         <v>3</v>
@@ -3107,7 +3119,7 @@
         </is>
       </c>
       <c r="C87" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D87" t="n">
         <v>3</v>
@@ -3137,7 +3149,7 @@
         </is>
       </c>
       <c r="C88" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D88" t="n">
         <v>7</v>
@@ -3167,7 +3179,7 @@
         </is>
       </c>
       <c r="C89" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D89" t="n">
         <v>7</v>
@@ -3197,7 +3209,7 @@
         </is>
       </c>
       <c r="C90" s="2" t="n">
-        <v>45390</v>
+        <v>45403</v>
       </c>
       <c r="D90" t="n">
         <v>4</v>
@@ -3211,7 +3223,7 @@
       <c r="G90" t="n">
         <v>1</v>
       </c>
-      <c r="H90" t="b">
+      <c r="H90" t="n">
         <v>1</v>
       </c>
       <c r="I90" t="inlineStr"/>
@@ -3229,7 +3241,7 @@
         </is>
       </c>
       <c r="C91" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D91" t="n">
         <v>4</v>
@@ -3259,7 +3271,7 @@
         </is>
       </c>
       <c r="C92" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D92" t="n">
         <v>7</v>
@@ -3289,7 +3301,7 @@
         </is>
       </c>
       <c r="C93" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D93" t="n">
         <v>4</v>
@@ -3319,7 +3331,7 @@
         </is>
       </c>
       <c r="C94" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D94" t="n">
         <v>4</v>
@@ -3349,7 +3361,7 @@
         </is>
       </c>
       <c r="C95" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D95" t="n">
         <v>3</v>
@@ -3379,7 +3391,7 @@
         </is>
       </c>
       <c r="C96" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D96" t="n">
         <v>3</v>
@@ -3409,7 +3421,7 @@
         </is>
       </c>
       <c r="C97" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D97" t="n">
         <v>0</v>
@@ -3439,7 +3451,7 @@
         </is>
       </c>
       <c r="C98" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D98" t="n">
         <v>3</v>
@@ -3469,7 +3481,7 @@
         </is>
       </c>
       <c r="C99" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D99" t="n">
         <v>5</v>
@@ -3499,7 +3511,7 @@
         </is>
       </c>
       <c r="C100" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D100" t="n">
         <v>2</v>
@@ -3531,7 +3543,7 @@
         </is>
       </c>
       <c r="C101" s="2" t="n">
-        <v>45377</v>
+        <v>45403</v>
       </c>
       <c r="D101" t="n">
         <v>5</v>
@@ -3561,7 +3573,7 @@
         </is>
       </c>
       <c r="C102" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D102" t="n">
         <v>1</v>
@@ -3591,7 +3603,7 @@
         </is>
       </c>
       <c r="C103" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D103" t="n">
         <v>4</v>
@@ -3621,24 +3633,26 @@
         </is>
       </c>
       <c r="C104" s="2" t="n">
-        <v>45390</v>
+        <v>45429</v>
       </c>
       <c r="D104" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E104" t="b">
         <v>0</v>
       </c>
       <c r="F104" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G104" t="n">
-        <v>1</v>
-      </c>
-      <c r="H104" t="b">
-        <v>1</v>
-      </c>
-      <c r="I104" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="H104" t="n">
+        <v>1</v>
+      </c>
+      <c r="I104" t="n">
+        <v>1</v>
+      </c>
       <c r="J104" t="inlineStr"/>
     </row>
     <row r="105">
@@ -3653,7 +3667,7 @@
         </is>
       </c>
       <c r="C105" s="2" t="n">
-        <v>45401</v>
+        <v>45403</v>
       </c>
       <c r="D105" t="n">
         <v>5</v>
@@ -3667,7 +3681,7 @@
       <c r="G105" t="n">
         <v>1</v>
       </c>
-      <c r="H105" t="b">
+      <c r="H105" t="n">
         <v>1</v>
       </c>
       <c r="I105" t="inlineStr"/>
@@ -3685,7 +3699,7 @@
         </is>
       </c>
       <c r="C106" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D106" t="n">
         <v>3</v>
@@ -3715,7 +3729,7 @@
         </is>
       </c>
       <c r="C107" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D107" t="n">
         <v>5</v>
@@ -3745,7 +3759,7 @@
         </is>
       </c>
       <c r="C108" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D108" t="n">
         <v>8</v>
@@ -3775,7 +3789,7 @@
         </is>
       </c>
       <c r="C109" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D109" t="n">
         <v>3</v>
@@ -3805,7 +3819,7 @@
         </is>
       </c>
       <c r="C110" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D110" t="n">
         <v>1</v>
@@ -3837,7 +3851,7 @@
         </is>
       </c>
       <c r="C111" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D111" t="n">
         <v>1</v>
@@ -3867,7 +3881,7 @@
         </is>
       </c>
       <c r="C112" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D112" t="n">
         <v>2</v>
@@ -3897,7 +3911,7 @@
         </is>
       </c>
       <c r="C113" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D113" t="n">
         <v>5</v>
@@ -3927,7 +3941,7 @@
         </is>
       </c>
       <c r="C114" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D114" t="n">
         <v>3</v>
@@ -3957,7 +3971,7 @@
         </is>
       </c>
       <c r="C115" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D115" t="n">
         <v>4</v>
@@ -3987,7 +4001,7 @@
         </is>
       </c>
       <c r="C116" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D116" t="n">
         <v>4</v>
@@ -4017,7 +4031,7 @@
         </is>
       </c>
       <c r="C117" s="2" t="n">
-        <v>45378</v>
+        <v>45403</v>
       </c>
       <c r="D117" t="n">
         <v>4</v>
@@ -4049,7 +4063,7 @@
         </is>
       </c>
       <c r="C118" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D118" t="n">
         <v>2</v>
@@ -4081,7 +4095,7 @@
         </is>
       </c>
       <c r="C119" s="2" t="n">
-        <v>45395</v>
+        <v>45403</v>
       </c>
       <c r="D119" t="n">
         <v>5</v>
@@ -4113,7 +4127,7 @@
         </is>
       </c>
       <c r="C120" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D120" t="n">
         <v>7</v>
@@ -4143,7 +4157,7 @@
         </is>
       </c>
       <c r="C121" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D121" t="n">
         <v>4</v>
@@ -4173,7 +4187,7 @@
         </is>
       </c>
       <c r="C122" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D122" t="n">
         <v>3</v>
@@ -4203,7 +4217,7 @@
         </is>
       </c>
       <c r="C123" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D123" t="n">
         <v>4</v>
@@ -4233,7 +4247,7 @@
         </is>
       </c>
       <c r="C124" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D124" t="n">
         <v>3</v>
@@ -4263,21 +4277,23 @@
         </is>
       </c>
       <c r="C125" s="2" t="n">
-        <v>45375</v>
+        <v>45405</v>
       </c>
       <c r="D125" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E125" t="b">
         <v>0</v>
       </c>
       <c r="F125" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G125" t="n">
-        <v>0</v>
-      </c>
-      <c r="H125" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H125" t="n">
+        <v>1</v>
+      </c>
       <c r="I125" t="inlineStr"/>
       <c r="J125" t="inlineStr"/>
     </row>
@@ -4293,7 +4309,7 @@
         </is>
       </c>
       <c r="C126" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D126" t="n">
         <v>3</v>
@@ -4323,7 +4339,7 @@
         </is>
       </c>
       <c r="C127" s="2" t="n">
-        <v>45399</v>
+        <v>45403</v>
       </c>
       <c r="D127" t="n">
         <v>7</v>
@@ -4353,7 +4369,7 @@
         </is>
       </c>
       <c r="C128" s="2" t="n">
-        <v>45396</v>
+        <v>45403</v>
       </c>
       <c r="D128" t="n">
         <v>8</v>
@@ -4385,7 +4401,7 @@
         </is>
       </c>
       <c r="C129" s="2" t="n">
-        <v>45389</v>
+        <v>45403</v>
       </c>
       <c r="D129" t="n">
         <v>5</v>
@@ -4417,7 +4433,7 @@
         </is>
       </c>
       <c r="C130" s="2" t="n">
-        <v>45382</v>
+        <v>45403</v>
       </c>
       <c r="D130" t="n">
         <v>4</v>
@@ -4449,7 +4465,7 @@
         </is>
       </c>
       <c r="C131" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D131" t="n">
         <v>7</v>
@@ -4479,7 +4495,7 @@
         </is>
       </c>
       <c r="C132" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D132" t="n">
         <v>4</v>
@@ -4509,7 +4525,7 @@
         </is>
       </c>
       <c r="C133" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D133" t="n">
         <v>4</v>
@@ -4539,7 +4555,7 @@
         </is>
       </c>
       <c r="C134" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D134" t="n">
         <v>2</v>
@@ -4573,7 +4589,7 @@
         </is>
       </c>
       <c r="C135" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D135" t="n">
         <v>3</v>
@@ -4603,24 +4619,26 @@
         </is>
       </c>
       <c r="C136" s="2" t="n">
-        <v>45390</v>
+        <v>45429</v>
       </c>
       <c r="D136" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E136" t="b">
         <v>0</v>
       </c>
       <c r="F136" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G136" t="n">
-        <v>1</v>
-      </c>
-      <c r="H136" t="b">
-        <v>1</v>
-      </c>
-      <c r="I136" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="H136" t="n">
+        <v>1</v>
+      </c>
+      <c r="I136" t="n">
+        <v>1</v>
+      </c>
       <c r="J136" t="inlineStr"/>
     </row>
     <row r="137">
@@ -4638,7 +4656,7 @@
         </is>
       </c>
       <c r="C137" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D137" t="n">
         <v>0</v>
@@ -4670,7 +4688,7 @@
         </is>
       </c>
       <c r="C138" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D138" t="n">
         <v>4</v>
@@ -4700,21 +4718,23 @@
         </is>
       </c>
       <c r="C139" s="2" t="n">
-        <v>45375</v>
+        <v>45418</v>
       </c>
       <c r="D139" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E139" t="b">
         <v>0</v>
       </c>
       <c r="F139" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G139" t="n">
-        <v>0</v>
-      </c>
-      <c r="H139" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H139" t="n">
+        <v>1</v>
+      </c>
       <c r="I139" t="inlineStr"/>
       <c r="J139" t="inlineStr"/>
     </row>
@@ -4730,7 +4750,7 @@
         </is>
       </c>
       <c r="C140" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D140" t="n">
         <v>0</v>
@@ -4761,7 +4781,7 @@
         </is>
       </c>
       <c r="C141" s="2" t="n">
-        <v>45380</v>
+        <v>45403</v>
       </c>
       <c r="D141" t="n">
         <v>4</v>
@@ -4795,7 +4815,7 @@
         </is>
       </c>
       <c r="C142" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D142" t="n">
         <v>3</v>
@@ -4827,7 +4847,7 @@
         </is>
       </c>
       <c r="C143" s="2" t="n">
-        <v>45377</v>
+        <v>45403</v>
       </c>
       <c r="D143" t="n">
         <v>2</v>
@@ -4841,7 +4861,7 @@
       <c r="G143" t="n">
         <v>2</v>
       </c>
-      <c r="H143" t="b">
+      <c r="H143" t="n">
         <v>1</v>
       </c>
       <c r="I143" t="n">
@@ -4863,7 +4883,7 @@
         </is>
       </c>
       <c r="C144" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D144" t="n">
         <v>2</v>
@@ -4899,7 +4919,7 @@
         </is>
       </c>
       <c r="C145" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D145" t="n">
         <v>2</v>
@@ -4929,7 +4949,7 @@
         </is>
       </c>
       <c r="C146" s="2" t="n">
-        <v>45391</v>
+        <v>45403</v>
       </c>
       <c r="D146" t="n">
         <v>5</v>
@@ -4962,7 +4982,7 @@
         </is>
       </c>
       <c r="C147" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D147" t="n">
         <v>0</v>
@@ -4994,7 +5014,7 @@
         </is>
       </c>
       <c r="C148" s="2" t="n">
-        <v>45382</v>
+        <v>45403</v>
       </c>
       <c r="D148" t="n">
         <v>4</v>
@@ -5028,7 +5048,7 @@
         </is>
       </c>
       <c r="C149" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D149" t="n">
         <v>2</v>
@@ -5058,7 +5078,7 @@
         </is>
       </c>
       <c r="C150" s="2" t="n">
-        <v>45379</v>
+        <v>45403</v>
       </c>
       <c r="D150" t="n">
         <v>3</v>
@@ -5072,7 +5092,7 @@
       <c r="G150" t="n">
         <v>1</v>
       </c>
-      <c r="H150" t="b">
+      <c r="H150" t="n">
         <v>1</v>
       </c>
       <c r="I150" t="inlineStr"/>
@@ -5090,7 +5110,7 @@
         </is>
       </c>
       <c r="C151" s="2" t="n">
-        <v>45391</v>
+        <v>45403</v>
       </c>
       <c r="D151" t="n">
         <v>5</v>
@@ -5123,7 +5143,7 @@
         </is>
       </c>
       <c r="C152" s="2" t="n">
-        <v>45382</v>
+        <v>45403</v>
       </c>
       <c r="D152" t="n">
         <v>4</v>
@@ -5156,7 +5176,7 @@
         </is>
       </c>
       <c r="C153" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D153" t="n">
         <v>3</v>
@@ -5187,7 +5207,7 @@
         </is>
       </c>
       <c r="C154" s="2" t="n">
-        <v>45377</v>
+        <v>45403</v>
       </c>
       <c r="D154" t="n">
         <v>2</v>
@@ -5201,7 +5221,7 @@
       <c r="G154" t="n">
         <v>1</v>
       </c>
-      <c r="H154" t="b">
+      <c r="H154" t="n">
         <v>1</v>
       </c>
       <c r="I154" t="inlineStr"/>
@@ -5219,7 +5239,7 @@
         </is>
       </c>
       <c r="C155" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D155" t="n">
         <v>1</v>
@@ -5251,7 +5271,7 @@
         </is>
       </c>
       <c r="C156" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D156" t="n">
         <v>0</v>
@@ -5282,7 +5302,7 @@
         </is>
       </c>
       <c r="C157" s="2" t="n">
-        <v>45382</v>
+        <v>45403</v>
       </c>
       <c r="D157" t="n">
         <v>4</v>
@@ -5314,7 +5334,7 @@
         </is>
       </c>
       <c r="C158" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D158" t="n">
         <v>3</v>
@@ -5345,7 +5365,7 @@
         </is>
       </c>
       <c r="C159" s="2" t="n">
-        <v>45376</v>
+        <v>45403</v>
       </c>
       <c r="D159" t="n">
         <v>0</v>
@@ -5359,7 +5379,7 @@
       <c r="G159" t="n">
         <v>1</v>
       </c>
-      <c r="H159" t="b">
+      <c r="H159" t="n">
         <v>0</v>
       </c>
       <c r="I159" t="inlineStr"/>
@@ -5379,7 +5399,7 @@
         </is>
       </c>
       <c r="C160" s="2" t="n">
-        <v>45401</v>
+        <v>45403</v>
       </c>
       <c r="D160" t="n">
         <v>5</v>
@@ -5393,7 +5413,7 @@
       <c r="G160" t="n">
         <v>1</v>
       </c>
-      <c r="H160" t="b">
+      <c r="H160" t="n">
         <v>1</v>
       </c>
       <c r="I160" t="inlineStr"/>
@@ -5412,7 +5432,7 @@
         </is>
       </c>
       <c r="C161" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D161" t="n">
         <v>2</v>
@@ -5443,7 +5463,7 @@
         </is>
       </c>
       <c r="C162" s="2" t="n">
-        <v>45384</v>
+        <v>45403</v>
       </c>
       <c r="D162" t="n">
         <v>4</v>
@@ -5475,21 +5495,23 @@
         </is>
       </c>
       <c r="C163" s="2" t="n">
-        <v>45375</v>
+        <v>45405</v>
       </c>
       <c r="D163" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E163" t="b">
         <v>0</v>
       </c>
       <c r="F163" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G163" t="n">
-        <v>0</v>
-      </c>
-      <c r="H163" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H163" t="b">
+        <v>1</v>
+      </c>
       <c r="I163" t="inlineStr"/>
       <c r="J163" t="inlineStr"/>
     </row>
@@ -5505,7 +5527,7 @@
         </is>
       </c>
       <c r="C164" s="2" t="n">
-        <v>45380</v>
+        <v>45403</v>
       </c>
       <c r="D164" t="n">
         <v>4</v>
@@ -5537,24 +5559,26 @@
         </is>
       </c>
       <c r="C165" s="2" t="n">
-        <v>45375</v>
+        <v>45407</v>
       </c>
       <c r="D165" t="n">
+        <v>3</v>
+      </c>
+      <c r="E165" t="b">
+        <v>0</v>
+      </c>
+      <c r="F165" t="n">
         <v>2</v>
       </c>
-      <c r="E165" t="b">
-        <v>0</v>
-      </c>
-      <c r="F165" t="n">
-        <v>1</v>
-      </c>
       <c r="G165" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H165" t="n">
         <v>1</v>
       </c>
-      <c r="I165" t="inlineStr"/>
+      <c r="I165" t="n">
+        <v>1</v>
+      </c>
       <c r="J165" t="inlineStr"/>
     </row>
     <row r="166">
@@ -5569,7 +5593,7 @@
         </is>
       </c>
       <c r="C166" s="2" t="n">
-        <v>45376</v>
+        <v>45403</v>
       </c>
       <c r="D166" t="n">
         <v>0</v>
@@ -5583,7 +5607,7 @@
       <c r="G166" t="n">
         <v>1</v>
       </c>
-      <c r="H166" t="b">
+      <c r="H166" t="n">
         <v>0</v>
       </c>
       <c r="I166" t="inlineStr"/>
@@ -5601,7 +5625,7 @@
         </is>
       </c>
       <c r="C167" s="2" t="n">
-        <v>45382</v>
+        <v>45403</v>
       </c>
       <c r="D167" t="n">
         <v>4</v>
@@ -5634,7 +5658,7 @@
         </is>
       </c>
       <c r="C168" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D168" t="n">
         <v>0</v>
@@ -5666,7 +5690,7 @@
         </is>
       </c>
       <c r="C169" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D169" t="n">
         <v>4</v>
@@ -5696,7 +5720,7 @@
         </is>
       </c>
       <c r="C170" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D170" t="n">
         <v>4</v>
@@ -5727,7 +5751,7 @@
         </is>
       </c>
       <c r="C171" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D171" t="n">
         <v>0</v>
@@ -5757,7 +5781,7 @@
         </is>
       </c>
       <c r="C172" s="2" t="n">
-        <v>45376</v>
+        <v>45403</v>
       </c>
       <c r="D172" t="n">
         <v>1</v>
@@ -5771,7 +5795,7 @@
       <c r="G172" t="n">
         <v>1</v>
       </c>
-      <c r="H172" t="b">
+      <c r="H172" t="n">
         <v>1</v>
       </c>
       <c r="I172" t="inlineStr"/>
@@ -5789,7 +5813,7 @@
         </is>
       </c>
       <c r="C173" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D173" t="n">
         <v>1</v>
@@ -5819,7 +5843,7 @@
         </is>
       </c>
       <c r="C174" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D174" t="n">
         <v>4</v>
@@ -5849,7 +5873,7 @@
         </is>
       </c>
       <c r="C175" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D175" t="n">
         <v>4</v>
@@ -5879,7 +5903,7 @@
         </is>
       </c>
       <c r="C176" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D176" t="n">
         <v>3</v>
@@ -5909,7 +5933,7 @@
         </is>
       </c>
       <c r="C177" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D177" t="n">
         <v>3</v>
@@ -5939,10 +5963,10 @@
         </is>
       </c>
       <c r="C178" s="2" t="n">
-        <v>45375</v>
+        <v>45407</v>
       </c>
       <c r="D178" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E178" t="b">
         <v>0</v>
@@ -5951,9 +5975,11 @@
         <v>0</v>
       </c>
       <c r="G178" t="n">
-        <v>0</v>
-      </c>
-      <c r="H178" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H178" t="n">
+        <v>0</v>
+      </c>
       <c r="I178" t="inlineStr"/>
       <c r="J178" t="inlineStr"/>
     </row>
@@ -5969,7 +5995,7 @@
         </is>
       </c>
       <c r="C179" s="2" t="n">
-        <v>45390</v>
+        <v>45403</v>
       </c>
       <c r="D179" t="n">
         <v>4</v>
@@ -5983,7 +6009,7 @@
       <c r="G179" t="n">
         <v>2</v>
       </c>
-      <c r="H179" t="b">
+      <c r="H179" t="n">
         <v>1</v>
       </c>
       <c r="I179" t="n">
@@ -6003,7 +6029,7 @@
         </is>
       </c>
       <c r="C180" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D180" t="n">
         <v>2</v>
@@ -6033,7 +6059,7 @@
         </is>
       </c>
       <c r="C181" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D181" t="n">
         <v>3</v>
@@ -6063,7 +6089,7 @@
         </is>
       </c>
       <c r="C182" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D182" t="n">
         <v>4</v>
@@ -6093,7 +6119,7 @@
         </is>
       </c>
       <c r="C183" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D183" t="n">
         <v>2</v>
@@ -6123,7 +6149,7 @@
         </is>
       </c>
       <c r="C184" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D184" t="n">
         <v>0</v>
@@ -6156,7 +6182,7 @@
         </is>
       </c>
       <c r="C185" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D185" t="n">
         <v>2</v>
@@ -6186,7 +6212,7 @@
         </is>
       </c>
       <c r="C186" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D186" t="n">
         <v>4</v>
@@ -6216,7 +6242,7 @@
         </is>
       </c>
       <c r="C187" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D187" t="n">
         <v>4</v>
@@ -6246,7 +6272,7 @@
         </is>
       </c>
       <c r="C188" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D188" t="n">
         <v>4</v>
@@ -6276,7 +6302,7 @@
         </is>
       </c>
       <c r="C189" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D189" t="n">
         <v>3</v>
@@ -6306,7 +6332,7 @@
         </is>
       </c>
       <c r="C190" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D190" t="n">
         <v>3</v>
@@ -6336,7 +6362,7 @@
         </is>
       </c>
       <c r="C191" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D191" t="n">
         <v>4</v>
@@ -6366,7 +6392,7 @@
         </is>
       </c>
       <c r="C192" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D192" t="n">
         <v>3</v>
@@ -6396,7 +6422,7 @@
         </is>
       </c>
       <c r="C193" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D193" t="n">
         <v>2</v>
@@ -6428,7 +6454,7 @@
         </is>
       </c>
       <c r="C194" s="2" t="n">
-        <v>45384</v>
+        <v>45403</v>
       </c>
       <c r="D194" t="n">
         <v>4</v>
@@ -6461,7 +6487,7 @@
         </is>
       </c>
       <c r="C195" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D195" t="n">
         <v>2</v>
@@ -6491,7 +6517,7 @@
         </is>
       </c>
       <c r="C196" s="2" t="n">
-        <v>45390</v>
+        <v>45403</v>
       </c>
       <c r="D196" t="n">
         <v>4</v>
@@ -6505,7 +6531,7 @@
       <c r="G196" t="n">
         <v>1</v>
       </c>
-      <c r="H196" t="b">
+      <c r="H196" t="n">
         <v>1</v>
       </c>
       <c r="I196" t="inlineStr"/>
@@ -6523,21 +6549,23 @@
         </is>
       </c>
       <c r="C197" s="2" t="n">
-        <v>45375</v>
+        <v>45407</v>
       </c>
       <c r="D197" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E197" t="b">
         <v>0</v>
       </c>
       <c r="F197" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G197" t="n">
-        <v>0</v>
-      </c>
-      <c r="H197" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H197" t="n">
+        <v>1</v>
+      </c>
       <c r="I197" t="inlineStr"/>
       <c r="J197" t="inlineStr"/>
     </row>
@@ -6553,7 +6581,7 @@
         </is>
       </c>
       <c r="C198" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D198" t="n">
         <v>4</v>
@@ -6583,7 +6611,7 @@
         </is>
       </c>
       <c r="C199" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D199" t="n">
         <v>3</v>
@@ -6613,7 +6641,7 @@
         </is>
       </c>
       <c r="C200" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D200" t="n">
         <v>2</v>
@@ -6643,7 +6671,7 @@
         </is>
       </c>
       <c r="C201" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D201" t="n">
         <v>1</v>
@@ -6675,21 +6703,23 @@
         </is>
       </c>
       <c r="C202" s="2" t="n">
-        <v>45375</v>
+        <v>45429</v>
       </c>
       <c r="D202" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E202" t="b">
         <v>0</v>
       </c>
       <c r="F202" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G202" t="n">
-        <v>0</v>
-      </c>
-      <c r="H202" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H202" t="n">
+        <v>1</v>
+      </c>
       <c r="I202" t="inlineStr"/>
       <c r="J202" t="inlineStr"/>
     </row>
@@ -6705,7 +6735,7 @@
         </is>
       </c>
       <c r="C203" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D203" t="n">
         <v>3</v>
@@ -6735,7 +6765,7 @@
         </is>
       </c>
       <c r="C204" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D204" t="n">
         <v>0</v>
@@ -6765,7 +6795,7 @@
         </is>
       </c>
       <c r="C205" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D205" t="n">
         <v>0</v>
@@ -6797,7 +6827,7 @@
         </is>
       </c>
       <c r="C206" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D206" t="n">
         <v>2</v>
@@ -6831,7 +6861,7 @@
         </is>
       </c>
       <c r="C207" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D207" t="n">
         <v>0</v>
@@ -6861,7 +6891,7 @@
         </is>
       </c>
       <c r="C208" s="2" t="n">
-        <v>45376</v>
+        <v>45403</v>
       </c>
       <c r="D208" t="n">
         <v>1</v>
@@ -6875,7 +6905,7 @@
       <c r="G208" t="n">
         <v>1</v>
       </c>
-      <c r="H208" t="b">
+      <c r="H208" t="n">
         <v>1</v>
       </c>
       <c r="I208" t="inlineStr"/>
@@ -6893,7 +6923,7 @@
         </is>
       </c>
       <c r="C209" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D209" t="n">
         <v>0</v>
@@ -6925,7 +6955,7 @@
         </is>
       </c>
       <c r="C210" s="2" t="n">
-        <v>45391</v>
+        <v>45403</v>
       </c>
       <c r="D210" t="n">
         <v>5</v>
@@ -6957,7 +6987,7 @@
         </is>
       </c>
       <c r="C211" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D211" t="n">
         <v>2</v>
@@ -6987,7 +7017,7 @@
         </is>
       </c>
       <c r="C212" s="2" t="n">
-        <v>45393</v>
+        <v>45403</v>
       </c>
       <c r="D212" t="n">
         <v>5</v>
@@ -7019,21 +7049,23 @@
         </is>
       </c>
       <c r="C213" s="2" t="n">
-        <v>45375</v>
+        <v>45429</v>
       </c>
       <c r="D213" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E213" t="b">
         <v>0</v>
       </c>
       <c r="F213" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G213" t="n">
-        <v>0</v>
-      </c>
-      <c r="H213" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H213" t="n">
+        <v>1</v>
+      </c>
       <c r="I213" t="inlineStr"/>
       <c r="J213" t="inlineStr"/>
     </row>
@@ -7049,7 +7081,7 @@
         </is>
       </c>
       <c r="C214" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D214" t="n">
         <v>2</v>
@@ -7079,10 +7111,10 @@
         </is>
       </c>
       <c r="C215" s="2" t="n">
-        <v>45375</v>
+        <v>45405</v>
       </c>
       <c r="D215" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E215" t="b">
         <v>0</v>
@@ -7091,12 +7123,14 @@
         <v>1</v>
       </c>
       <c r="G215" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H215" t="n">
-        <v>1</v>
-      </c>
-      <c r="I215" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="I215" t="n">
+        <v>1</v>
+      </c>
       <c r="J215" t="inlineStr"/>
     </row>
     <row r="216">
@@ -7111,7 +7145,7 @@
         </is>
       </c>
       <c r="C216" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D216" t="n">
         <v>2</v>
@@ -7141,7 +7175,7 @@
         </is>
       </c>
       <c r="C217" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D217" t="n">
         <v>1</v>
@@ -7173,7 +7207,7 @@
         </is>
       </c>
       <c r="C218" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D218" t="n">
         <v>1</v>
@@ -7207,7 +7241,7 @@
         </is>
       </c>
       <c r="C219" s="2" t="n">
-        <v>45401</v>
+        <v>45403</v>
       </c>
       <c r="D219" t="n">
         <v>5</v>
@@ -7221,7 +7255,7 @@
       <c r="G219" t="n">
         <v>1</v>
       </c>
-      <c r="H219" t="b">
+      <c r="H219" t="n">
         <v>1</v>
       </c>
       <c r="I219" t="inlineStr"/>
@@ -7239,7 +7273,7 @@
         </is>
       </c>
       <c r="C220" s="2" t="n">
-        <v>45389</v>
+        <v>45403</v>
       </c>
       <c r="D220" t="n">
         <v>5</v>
@@ -7271,7 +7305,7 @@
         </is>
       </c>
       <c r="C221" s="2" t="n">
-        <v>45376</v>
+        <v>45403</v>
       </c>
       <c r="D221" t="n">
         <v>1</v>
@@ -7285,7 +7319,7 @@
       <c r="G221" t="n">
         <v>2</v>
       </c>
-      <c r="H221" t="b">
+      <c r="H221" t="n">
         <v>1</v>
       </c>
       <c r="I221" t="n">
@@ -7305,7 +7339,7 @@
         </is>
       </c>
       <c r="C222" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D222" t="n">
         <v>3</v>
@@ -7336,7 +7370,7 @@
         </is>
       </c>
       <c r="C223" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D223" t="n">
         <v>1</v>
@@ -7368,7 +7402,7 @@
         </is>
       </c>
       <c r="C224" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D224" t="n">
         <v>0</v>
@@ -7398,7 +7432,7 @@
         </is>
       </c>
       <c r="C225" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D225" t="n">
         <v>2</v>
@@ -7431,7 +7465,7 @@
         </is>
       </c>
       <c r="C226" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D226" t="n">
         <v>2</v>
@@ -7461,7 +7495,7 @@
         </is>
       </c>
       <c r="C227" s="2" t="n">
-        <v>45382</v>
+        <v>45403</v>
       </c>
       <c r="D227" t="n">
         <v>4</v>
@@ -7495,7 +7529,7 @@
         </is>
       </c>
       <c r="C228" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D228" t="n">
         <v>4</v>
@@ -7525,7 +7559,7 @@
         </is>
       </c>
       <c r="C229" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D229" t="n">
         <v>4</v>
@@ -7555,7 +7589,7 @@
         </is>
       </c>
       <c r="C230" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D230" t="n">
         <v>3</v>
@@ -7585,21 +7619,23 @@
         </is>
       </c>
       <c r="C231" s="2" t="n">
-        <v>45375</v>
+        <v>45418</v>
       </c>
       <c r="D231" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E231" t="b">
         <v>0</v>
       </c>
       <c r="F231" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G231" t="n">
-        <v>0</v>
-      </c>
-      <c r="H231" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H231" t="b">
+        <v>1</v>
+      </c>
       <c r="I231" t="inlineStr"/>
       <c r="J231" t="inlineStr"/>
     </row>
@@ -7618,7 +7654,7 @@
         </is>
       </c>
       <c r="C232" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D232" t="n">
         <v>0</v>
@@ -7648,7 +7684,7 @@
         </is>
       </c>
       <c r="C233" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D233" t="n">
         <v>2</v>
@@ -7680,7 +7716,7 @@
         </is>
       </c>
       <c r="C234" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D234" t="n">
         <v>3</v>
@@ -7712,7 +7748,7 @@
         </is>
       </c>
       <c r="C235" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D235" t="n">
         <v>2</v>
@@ -7743,7 +7779,7 @@
         </is>
       </c>
       <c r="C236" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D236" t="n">
         <v>3</v>
@@ -7773,7 +7809,7 @@
         </is>
       </c>
       <c r="C237" s="2" t="n">
-        <v>45380</v>
+        <v>45403</v>
       </c>
       <c r="D237" t="n">
         <v>4</v>
@@ -7805,7 +7841,7 @@
         </is>
       </c>
       <c r="C238" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D238" t="n">
         <v>1</v>
@@ -7835,7 +7871,7 @@
         </is>
       </c>
       <c r="C239" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D239" t="n">
         <v>2</v>
@@ -7865,7 +7901,7 @@
         </is>
       </c>
       <c r="C240" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D240" t="n">
         <v>1</v>
@@ -7895,7 +7931,7 @@
         </is>
       </c>
       <c r="C241" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D241" t="n">
         <v>3</v>
@@ -7925,7 +7961,7 @@
         </is>
       </c>
       <c r="C242" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D242" t="n">
         <v>2</v>
@@ -7955,7 +7991,7 @@
         </is>
       </c>
       <c r="C243" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D243" t="n">
         <v>2</v>
@@ -7985,7 +8021,7 @@
         </is>
       </c>
       <c r="C244" s="2" t="n">
-        <v>45380</v>
+        <v>45403</v>
       </c>
       <c r="D244" t="n">
         <v>4</v>
@@ -8018,7 +8054,7 @@
         </is>
       </c>
       <c r="C245" s="2" t="n">
-        <v>45376</v>
+        <v>45403</v>
       </c>
       <c r="D245" t="n">
         <v>1</v>
@@ -8032,7 +8068,7 @@
       <c r="G245" t="n">
         <v>2</v>
       </c>
-      <c r="H245" t="b">
+      <c r="H245" t="n">
         <v>1</v>
       </c>
       <c r="I245" t="n">
@@ -8052,7 +8088,7 @@
         </is>
       </c>
       <c r="C246" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D246" t="n">
         <v>0</v>
@@ -8082,7 +8118,7 @@
         </is>
       </c>
       <c r="C247" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D247" t="n">
         <v>3</v>
@@ -8114,7 +8150,7 @@
         </is>
       </c>
       <c r="C248" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D248" t="n">
         <v>0</v>
@@ -8146,7 +8182,7 @@
         </is>
       </c>
       <c r="C249" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D249" t="n">
         <v>3</v>
@@ -8176,7 +8212,7 @@
         </is>
       </c>
       <c r="C250" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D250" t="n">
         <v>0</v>
@@ -8206,21 +8242,23 @@
         </is>
       </c>
       <c r="C251" s="2" t="n">
-        <v>45375</v>
+        <v>45404</v>
       </c>
       <c r="D251" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E251" t="b">
         <v>0</v>
       </c>
       <c r="F251" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G251" t="n">
-        <v>0</v>
-      </c>
-      <c r="H251" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H251" t="n">
+        <v>1</v>
+      </c>
       <c r="I251" t="inlineStr"/>
       <c r="J251" t="inlineStr"/>
     </row>
@@ -8236,7 +8274,7 @@
         </is>
       </c>
       <c r="C252" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D252" t="n">
         <v>3</v>
@@ -8269,7 +8307,7 @@
         </is>
       </c>
       <c r="C253" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D253" t="n">
         <v>0</v>
@@ -8303,7 +8341,7 @@
         </is>
       </c>
       <c r="C254" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D254" t="n">
         <v>2</v>
@@ -8333,7 +8371,7 @@
         </is>
       </c>
       <c r="C255" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D255" t="n">
         <v>0</v>
@@ -8363,7 +8401,7 @@
         </is>
       </c>
       <c r="C256" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D256" t="n">
         <v>3</v>
@@ -8393,10 +8431,10 @@
         </is>
       </c>
       <c r="C257" s="2" t="n">
-        <v>45375</v>
+        <v>45407</v>
       </c>
       <c r="D257" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E257" t="b">
         <v>0</v>
@@ -8405,9 +8443,11 @@
         <v>0</v>
       </c>
       <c r="G257" t="n">
-        <v>0</v>
-      </c>
-      <c r="H257" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H257" t="n">
+        <v>0</v>
+      </c>
       <c r="I257" t="inlineStr"/>
       <c r="J257" t="inlineStr"/>
     </row>
@@ -8423,7 +8463,7 @@
         </is>
       </c>
       <c r="C258" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D258" t="n">
         <v>1</v>
@@ -8455,7 +8495,7 @@
         </is>
       </c>
       <c r="C259" s="2" t="n">
-        <v>45379</v>
+        <v>45403</v>
       </c>
       <c r="D259" t="n">
         <v>3</v>
@@ -8469,7 +8509,7 @@
       <c r="G259" t="n">
         <v>2</v>
       </c>
-      <c r="H259" t="b">
+      <c r="H259" t="n">
         <v>1</v>
       </c>
       <c r="I259" t="n">
@@ -8489,7 +8529,7 @@
         </is>
       </c>
       <c r="C260" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D260" t="n">
         <v>3</v>
@@ -8521,7 +8561,7 @@
         </is>
       </c>
       <c r="C261" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D261" t="n">
         <v>2</v>
@@ -8551,7 +8591,7 @@
         </is>
       </c>
       <c r="C262" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D262" t="n">
         <v>2</v>
@@ -8581,7 +8621,7 @@
         </is>
       </c>
       <c r="C263" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D263" t="n">
         <v>0</v>
@@ -8611,7 +8651,7 @@
         </is>
       </c>
       <c r="C264" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D264" t="n">
         <v>1</v>
@@ -8641,7 +8681,7 @@
         </is>
       </c>
       <c r="C265" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D265" t="n">
         <v>0</v>
@@ -8673,7 +8713,7 @@
         </is>
       </c>
       <c r="C266" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D266" t="n">
         <v>3</v>
@@ -8703,7 +8743,7 @@
         </is>
       </c>
       <c r="C267" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D267" t="n">
         <v>4</v>
@@ -8733,7 +8773,7 @@
         </is>
       </c>
       <c r="C268" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D268" t="n">
         <v>3</v>
@@ -8765,7 +8805,7 @@
         </is>
       </c>
       <c r="C269" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D269" t="n">
         <v>4</v>
@@ -8795,7 +8835,7 @@
         </is>
       </c>
       <c r="C270" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D270" t="n">
         <v>2</v>
@@ -8826,7 +8866,7 @@
         </is>
       </c>
       <c r="C271" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D271" t="n">
         <v>4</v>
@@ -8856,7 +8896,7 @@
         </is>
       </c>
       <c r="C272" s="2" t="n">
-        <v>45384</v>
+        <v>45403</v>
       </c>
       <c r="D272" t="n">
         <v>4</v>
@@ -8888,7 +8928,7 @@
         </is>
       </c>
       <c r="C273" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D273" t="n">
         <v>0</v>
@@ -8920,7 +8960,7 @@
         </is>
       </c>
       <c r="C274" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D274" t="n">
         <v>0</v>
@@ -8950,7 +8990,7 @@
         </is>
       </c>
       <c r="C275" s="2" t="n">
-        <v>45376</v>
+        <v>45403</v>
       </c>
       <c r="D275" t="n">
         <v>0</v>
@@ -8964,7 +9004,7 @@
       <c r="G275" t="n">
         <v>1</v>
       </c>
-      <c r="H275" t="b">
+      <c r="H275" t="n">
         <v>0</v>
       </c>
       <c r="I275" t="inlineStr"/>
@@ -8982,7 +9022,7 @@
         </is>
       </c>
       <c r="C276" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D276" t="n">
         <v>0</v>
@@ -9012,7 +9052,7 @@
         </is>
       </c>
       <c r="C277" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D277" t="n">
         <v>2</v>
@@ -9045,7 +9085,7 @@
         </is>
       </c>
       <c r="C278" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D278" t="n">
         <v>0</v>
@@ -9078,7 +9118,7 @@
         </is>
       </c>
       <c r="C279" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D279" t="n">
         <v>2</v>
@@ -9111,7 +9151,7 @@
         </is>
       </c>
       <c r="C280" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D280" t="n">
         <v>0</v>
@@ -9141,7 +9181,7 @@
         </is>
       </c>
       <c r="C281" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D281" t="n">
         <v>2</v>
@@ -9171,7 +9211,7 @@
         </is>
       </c>
       <c r="C282" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D282" t="n">
         <v>0</v>
@@ -9201,7 +9241,7 @@
         </is>
       </c>
       <c r="C283" s="2" t="n">
-        <v>45376</v>
+        <v>45403</v>
       </c>
       <c r="D283" t="n">
         <v>0</v>
@@ -9215,7 +9255,7 @@
       <c r="G283" t="n">
         <v>1</v>
       </c>
-      <c r="H283" t="b">
+      <c r="H283" t="n">
         <v>0</v>
       </c>
       <c r="I283" t="inlineStr"/>
@@ -9234,7 +9274,7 @@
         </is>
       </c>
       <c r="C284" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D284" t="n">
         <v>0</v>
@@ -9267,7 +9307,7 @@
         </is>
       </c>
       <c r="C285" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D285" t="n">
         <v>3</v>
@@ -9299,7 +9339,7 @@
         </is>
       </c>
       <c r="C286" s="2" t="n">
-        <v>45378</v>
+        <v>45403</v>
       </c>
       <c r="D286" t="n">
         <v>4</v>
@@ -9333,7 +9373,7 @@
         </is>
       </c>
       <c r="C287" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D287" t="n">
         <v>0</v>
@@ -9365,7 +9405,7 @@
         </is>
       </c>
       <c r="C288" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D288" t="n">
         <v>1</v>
@@ -9396,7 +9436,7 @@
         </is>
       </c>
       <c r="C289" s="2" t="n">
-        <v>45393</v>
+        <v>45403</v>
       </c>
       <c r="D289" t="n">
         <v>5</v>
@@ -9428,7 +9468,7 @@
         </is>
       </c>
       <c r="C290" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D290" t="n">
         <v>0</v>
@@ -9458,7 +9498,7 @@
         </is>
       </c>
       <c r="C291" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D291" t="n">
         <v>1</v>
@@ -9488,7 +9528,7 @@
         </is>
       </c>
       <c r="C292" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D292" t="n">
         <v>0</v>
@@ -9519,7 +9559,7 @@
         </is>
       </c>
       <c r="C293" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D293" t="n">
         <v>0</v>
@@ -9550,7 +9590,7 @@
         </is>
       </c>
       <c r="C294" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D294" t="n">
         <v>3</v>
@@ -9583,7 +9623,7 @@
         </is>
       </c>
       <c r="C295" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D295" t="n">
         <v>0</v>
@@ -9613,7 +9653,7 @@
         </is>
       </c>
       <c r="C296" s="2" t="n">
-        <v>45375</v>
+        <v>45404</v>
       </c>
       <c r="D296" t="n">
         <v>0</v>
@@ -9625,12 +9665,14 @@
         <v>0</v>
       </c>
       <c r="G296" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H296" t="n">
         <v>0</v>
       </c>
-      <c r="I296" t="inlineStr"/>
+      <c r="I296" t="n">
+        <v>0</v>
+      </c>
       <c r="J296" t="inlineStr"/>
     </row>
     <row r="297">
@@ -9645,7 +9687,7 @@
         </is>
       </c>
       <c r="C297" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D297" t="n">
         <v>0</v>
@@ -9677,7 +9719,7 @@
         </is>
       </c>
       <c r="C298" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D298" t="n">
         <v>3</v>
@@ -9707,7 +9749,7 @@
         </is>
       </c>
       <c r="C299" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D299" t="n">
         <v>3</v>
@@ -9738,7 +9780,7 @@
         </is>
       </c>
       <c r="C300" s="2" t="n">
-        <v>45382</v>
+        <v>45403</v>
       </c>
       <c r="D300" t="n">
         <v>4</v>
@@ -9771,7 +9813,7 @@
         </is>
       </c>
       <c r="C301" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D301" t="n">
         <v>2</v>
@@ -9805,24 +9847,26 @@
         </is>
       </c>
       <c r="C302" s="2" t="n">
-        <v>45375</v>
+        <v>45405</v>
       </c>
       <c r="D302" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E302" t="b">
         <v>0</v>
       </c>
       <c r="F302" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G302" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H302" t="n">
         <v>1</v>
       </c>
-      <c r="I302" t="inlineStr"/>
+      <c r="I302" t="n">
+        <v>1</v>
+      </c>
       <c r="J302" t="inlineStr"/>
     </row>
     <row r="303">
@@ -9837,7 +9881,7 @@
         </is>
       </c>
       <c r="C303" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D303" t="n">
         <v>1</v>
@@ -9868,7 +9912,7 @@
         </is>
       </c>
       <c r="C304" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D304" t="n">
         <v>4</v>
@@ -9899,7 +9943,7 @@
         </is>
       </c>
       <c r="C305" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D305" t="n">
         <v>0</v>
@@ -9932,7 +9976,7 @@
         </is>
       </c>
       <c r="C306" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D306" t="n">
         <v>0</v>
@@ -9962,7 +10006,7 @@
         </is>
       </c>
       <c r="C307" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D307" t="n">
         <v>2</v>
@@ -9996,7 +10040,7 @@
         </is>
       </c>
       <c r="C308" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D308" t="n">
         <v>0</v>
@@ -10026,7 +10070,7 @@
         </is>
       </c>
       <c r="C309" s="2" t="n">
-        <v>45376</v>
+        <v>45403</v>
       </c>
       <c r="D309" t="n">
         <v>1</v>
@@ -10040,7 +10084,7 @@
       <c r="G309" t="n">
         <v>2</v>
       </c>
-      <c r="H309" t="b">
+      <c r="H309" t="n">
         <v>1</v>
       </c>
       <c r="I309" t="n">
@@ -10061,7 +10105,7 @@
         </is>
       </c>
       <c r="C310" s="2" t="n">
-        <v>45378</v>
+        <v>45403</v>
       </c>
       <c r="D310" t="n">
         <v>4</v>
@@ -10093,7 +10137,7 @@
         </is>
       </c>
       <c r="C311" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D311" t="n">
         <v>1</v>
@@ -10127,7 +10171,7 @@
         </is>
       </c>
       <c r="C312" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D312" t="n">
         <v>0</v>
@@ -10159,7 +10203,7 @@
         </is>
       </c>
       <c r="C313" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D313" t="n">
         <v>3</v>
@@ -10190,7 +10234,7 @@
         </is>
       </c>
       <c r="C314" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D314" t="n">
         <v>2</v>
@@ -10223,7 +10267,7 @@
         </is>
       </c>
       <c r="C315" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D315" t="n">
         <v>4</v>
@@ -10255,21 +10299,23 @@
         </is>
       </c>
       <c r="C316" s="2" t="n">
-        <v>45375</v>
+        <v>45418</v>
       </c>
       <c r="D316" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E316" t="b">
         <v>0</v>
       </c>
       <c r="F316" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G316" t="n">
-        <v>0</v>
-      </c>
-      <c r="H316" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H316" t="b">
+        <v>1</v>
+      </c>
       <c r="I316" t="inlineStr"/>
       <c r="J316" t="inlineStr"/>
     </row>
@@ -10286,7 +10332,7 @@
         </is>
       </c>
       <c r="C317" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D317" t="n">
         <v>2</v>
@@ -10316,7 +10362,7 @@
         </is>
       </c>
       <c r="C318" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D318" t="n">
         <v>0</v>
@@ -10348,7 +10394,7 @@
         </is>
       </c>
       <c r="C319" s="2" t="n">
-        <v>45376</v>
+        <v>45403</v>
       </c>
       <c r="D319" t="n">
         <v>0</v>
@@ -10362,7 +10408,7 @@
       <c r="G319" t="n">
         <v>2</v>
       </c>
-      <c r="H319" t="b">
+      <c r="H319" t="n">
         <v>0</v>
       </c>
       <c r="I319" t="n">
@@ -10383,24 +10429,26 @@
         </is>
       </c>
       <c r="C320" s="2" t="n">
-        <v>45375</v>
+        <v>45404</v>
       </c>
       <c r="D320" t="n">
+        <v>1</v>
+      </c>
+      <c r="E320" t="b">
+        <v>0</v>
+      </c>
+      <c r="F320" t="n">
+        <v>0</v>
+      </c>
+      <c r="G320" t="n">
         <v>2</v>
       </c>
-      <c r="E320" t="b">
-        <v>0</v>
-      </c>
-      <c r="F320" t="n">
-        <v>0</v>
-      </c>
-      <c r="G320" t="n">
-        <v>1</v>
-      </c>
       <c r="H320" t="n">
         <v>0</v>
       </c>
-      <c r="I320" t="inlineStr"/>
+      <c r="I320" t="n">
+        <v>0</v>
+      </c>
       <c r="J320" t="inlineStr"/>
     </row>
     <row r="321">
@@ -10417,7 +10465,7 @@
         </is>
       </c>
       <c r="C321" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D321" t="n">
         <v>1</v>
@@ -10451,7 +10499,7 @@
         </is>
       </c>
       <c r="C322" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D322" t="n">
         <v>4</v>
@@ -10482,7 +10530,7 @@
         </is>
       </c>
       <c r="C323" s="2" t="n">
-        <v>45377</v>
+        <v>45403</v>
       </c>
       <c r="D323" t="n">
         <v>2</v>
@@ -10496,7 +10544,7 @@
       <c r="G323" t="n">
         <v>3</v>
       </c>
-      <c r="H323" t="b">
+      <c r="H323" t="n">
         <v>1</v>
       </c>
       <c r="I323" t="n">
@@ -10518,7 +10566,7 @@
         </is>
       </c>
       <c r="C324" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D324" t="n">
         <v>1</v>
@@ -10552,21 +10600,23 @@
         </is>
       </c>
       <c r="C325" s="2" t="n">
-        <v>45375</v>
+        <v>45407</v>
       </c>
       <c r="D325" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E325" t="b">
         <v>0</v>
       </c>
       <c r="F325" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G325" t="n">
-        <v>0</v>
-      </c>
-      <c r="H325" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H325" t="b">
+        <v>1</v>
+      </c>
       <c r="I325" t="inlineStr"/>
       <c r="J325" t="inlineStr"/>
     </row>
@@ -10583,7 +10633,7 @@
         </is>
       </c>
       <c r="C326" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D326" t="n">
         <v>1</v>
@@ -10616,7 +10666,7 @@
         </is>
       </c>
       <c r="C327" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D327" t="n">
         <v>3</v>
@@ -10651,7 +10701,7 @@
         </is>
       </c>
       <c r="C328" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D328" t="n">
         <v>0</v>
@@ -10681,7 +10731,7 @@
         </is>
       </c>
       <c r="C329" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D329" t="n">
         <v>0</v>
@@ -10711,7 +10761,7 @@
         </is>
       </c>
       <c r="C330" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D330" t="n">
         <v>2</v>
@@ -10746,7 +10796,7 @@
         </is>
       </c>
       <c r="C331" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D331" t="n">
         <v>0</v>
@@ -10778,7 +10828,7 @@
         </is>
       </c>
       <c r="C332" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D332" t="n">
         <v>2</v>
@@ -10813,7 +10863,7 @@
         </is>
       </c>
       <c r="C333" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D333" t="n">
         <v>0</v>
@@ -10843,7 +10893,7 @@
         </is>
       </c>
       <c r="C334" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D334" t="n">
         <v>3</v>
@@ -10874,7 +10924,7 @@
         </is>
       </c>
       <c r="C335" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D335" t="n">
         <v>0</v>
@@ -10904,7 +10954,7 @@
         </is>
       </c>
       <c r="C336" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D336" t="n">
         <v>0</v>
@@ -10934,7 +10984,7 @@
         </is>
       </c>
       <c r="C337" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D337" t="n">
         <v>2</v>
@@ -10966,7 +11016,7 @@
         </is>
       </c>
       <c r="C338" s="2" t="n">
-        <v>45375</v>
+        <v>45404</v>
       </c>
       <c r="D338" t="n">
         <v>0</v>
@@ -10978,9 +11028,11 @@
         <v>0</v>
       </c>
       <c r="G338" t="n">
-        <v>0</v>
-      </c>
-      <c r="H338" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H338" t="n">
+        <v>0</v>
+      </c>
       <c r="I338" t="inlineStr"/>
       <c r="J338" t="inlineStr"/>
     </row>
@@ -10996,7 +11048,7 @@
         </is>
       </c>
       <c r="C339" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D339" t="n">
         <v>0</v>
@@ -11026,7 +11078,7 @@
         </is>
       </c>
       <c r="C340" s="2" t="n">
-        <v>45378</v>
+        <v>45403</v>
       </c>
       <c r="D340" t="n">
         <v>4</v>
@@ -11058,7 +11110,7 @@
         </is>
       </c>
       <c r="C341" s="2" t="n">
-        <v>45390</v>
+        <v>45403</v>
       </c>
       <c r="D341" t="n">
         <v>4</v>
@@ -11072,7 +11124,7 @@
       <c r="G341" t="n">
         <v>1</v>
       </c>
-      <c r="H341" t="b">
+      <c r="H341" t="n">
         <v>1</v>
       </c>
       <c r="I341" t="inlineStr"/>
@@ -11090,7 +11142,7 @@
         </is>
       </c>
       <c r="C342" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D342" t="n">
         <v>4</v>
@@ -11120,7 +11172,7 @@
         </is>
       </c>
       <c r="C343" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D343" t="n">
         <v>3</v>
@@ -11150,7 +11202,7 @@
         </is>
       </c>
       <c r="C344" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D344" t="n">
         <v>4</v>
@@ -11183,7 +11235,7 @@
         </is>
       </c>
       <c r="C345" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D345" t="n">
         <v>2</v>
@@ -11216,7 +11268,7 @@
         </is>
       </c>
       <c r="C346" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D346" t="n">
         <v>3</v>
@@ -11250,24 +11302,26 @@
         </is>
       </c>
       <c r="C347" s="2" t="n">
-        <v>45375</v>
+        <v>45404</v>
       </c>
       <c r="D347" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E347" t="b">
         <v>0</v>
       </c>
       <c r="F347" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G347" t="n">
-        <v>1</v>
-      </c>
-      <c r="H347" t="n">
-        <v>0</v>
-      </c>
-      <c r="I347" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="H347" t="b">
+        <v>1</v>
+      </c>
+      <c r="I347" t="n">
+        <v>0</v>
+      </c>
       <c r="J347" t="inlineStr"/>
     </row>
     <row r="348">
@@ -11285,7 +11339,7 @@
         </is>
       </c>
       <c r="C348" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D348" t="n">
         <v>0</v>
@@ -11315,7 +11369,7 @@
         </is>
       </c>
       <c r="C349" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D349" t="n">
         <v>2</v>
@@ -11345,7 +11399,7 @@
         </is>
       </c>
       <c r="C350" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D350" t="n">
         <v>0</v>
@@ -11377,7 +11431,7 @@
         </is>
       </c>
       <c r="C351" s="2" t="n">
-        <v>45401</v>
+        <v>45403</v>
       </c>
       <c r="D351" t="n">
         <v>5</v>
@@ -11391,7 +11445,7 @@
       <c r="G351" t="n">
         <v>1</v>
       </c>
-      <c r="H351" t="b">
+      <c r="H351" t="n">
         <v>1</v>
       </c>
       <c r="I351" t="inlineStr"/>
@@ -11409,7 +11463,7 @@
         </is>
       </c>
       <c r="C352" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D352" t="n">
         <v>0</v>
@@ -11441,7 +11495,7 @@
         </is>
       </c>
       <c r="C353" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D353" t="n">
         <v>3</v>
@@ -11471,7 +11525,7 @@
         </is>
       </c>
       <c r="C354" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D354" t="n">
         <v>2</v>
@@ -11501,7 +11555,7 @@
         </is>
       </c>
       <c r="C355" s="2" t="n">
-        <v>45384</v>
+        <v>45403</v>
       </c>
       <c r="D355" t="n">
         <v>4</v>
@@ -11535,7 +11589,7 @@
         </is>
       </c>
       <c r="C356" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D356" t="n">
         <v>1</v>
@@ -11568,7 +11622,7 @@
         </is>
       </c>
       <c r="C357" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D357" t="n">
         <v>4</v>
@@ -11598,7 +11652,7 @@
         </is>
       </c>
       <c r="C358" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D358" t="n">
         <v>0</v>
@@ -11630,7 +11684,7 @@
         </is>
       </c>
       <c r="C359" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D359" t="n">
         <v>4</v>
@@ -11661,7 +11715,7 @@
         </is>
       </c>
       <c r="C360" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D360" t="n">
         <v>0</v>
@@ -11693,7 +11747,7 @@
         </is>
       </c>
       <c r="C361" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D361" t="n">
         <v>4</v>
@@ -11723,7 +11777,7 @@
         </is>
       </c>
       <c r="C362" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D362" t="n">
         <v>0</v>
@@ -11755,7 +11809,7 @@
         </is>
       </c>
       <c r="C363" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D363" t="n">
         <v>3</v>
@@ -11787,7 +11841,7 @@
         </is>
       </c>
       <c r="C364" s="2" t="n">
-        <v>45375</v>
+        <v>45404</v>
       </c>
       <c r="D364" t="n">
         <v>0</v>
@@ -11799,9 +11853,11 @@
         <v>0</v>
       </c>
       <c r="G364" t="n">
-        <v>0</v>
-      </c>
-      <c r="H364" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H364" t="n">
+        <v>0</v>
+      </c>
       <c r="I364" t="inlineStr"/>
       <c r="J364" t="inlineStr"/>
     </row>
@@ -11820,7 +11876,7 @@
         </is>
       </c>
       <c r="C365" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D365" t="n">
         <v>2</v>
@@ -11852,7 +11908,7 @@
         </is>
       </c>
       <c r="C366" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D366" t="n">
         <v>0</v>
@@ -11884,7 +11940,7 @@
         </is>
       </c>
       <c r="C367" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D367" t="n">
         <v>0</v>
@@ -11915,7 +11971,7 @@
         </is>
       </c>
       <c r="C368" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D368" t="n">
         <v>3</v>
@@ -11945,10 +12001,10 @@
         </is>
       </c>
       <c r="C369" s="2" t="n">
-        <v>45375</v>
+        <v>45404</v>
       </c>
       <c r="D369" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E369" t="b">
         <v>0</v>
@@ -11957,9 +12013,11 @@
         <v>0</v>
       </c>
       <c r="G369" t="n">
-        <v>0</v>
-      </c>
-      <c r="H369" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H369" t="b">
+        <v>0</v>
+      </c>
       <c r="I369" t="inlineStr"/>
       <c r="J369" t="inlineStr"/>
     </row>
@@ -11977,7 +12035,7 @@
         </is>
       </c>
       <c r="C370" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D370" t="n">
         <v>3</v>
@@ -12009,21 +12067,23 @@
         </is>
       </c>
       <c r="C371" s="2" t="n">
-        <v>45375</v>
+        <v>45404</v>
       </c>
       <c r="D371" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E371" t="b">
         <v>0</v>
       </c>
       <c r="F371" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G371" t="n">
-        <v>0</v>
-      </c>
-      <c r="H371" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H371" t="b">
+        <v>1</v>
+      </c>
       <c r="I371" t="inlineStr"/>
       <c r="J371" t="inlineStr"/>
     </row>
@@ -12040,7 +12100,7 @@
         </is>
       </c>
       <c r="C372" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D372" t="n">
         <v>0</v>
@@ -12072,7 +12132,7 @@
         </is>
       </c>
       <c r="C373" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D373" t="n">
         <v>1</v>
@@ -12102,7 +12162,7 @@
         </is>
       </c>
       <c r="C374" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D374" t="n">
         <v>3</v>
@@ -12132,7 +12192,7 @@
         </is>
       </c>
       <c r="C375" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D375" t="n">
         <v>3</v>
@@ -12163,7 +12223,7 @@
         </is>
       </c>
       <c r="C376" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D376" t="n">
         <v>0</v>
@@ -12193,7 +12253,7 @@
         </is>
       </c>
       <c r="C377" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D377" t="n">
         <v>1</v>
@@ -12225,7 +12285,7 @@
         </is>
       </c>
       <c r="C378" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D378" t="n">
         <v>0</v>
@@ -12257,7 +12317,7 @@
         </is>
       </c>
       <c r="C379" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D379" t="n">
         <v>3</v>
@@ -12288,7 +12348,7 @@
         </is>
       </c>
       <c r="C380" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D380" t="n">
         <v>1</v>
@@ -12318,7 +12378,7 @@
         </is>
       </c>
       <c r="C381" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D381" t="n">
         <v>0</v>
@@ -12348,7 +12408,7 @@
         </is>
       </c>
       <c r="C382" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D382" t="n">
         <v>0</v>
@@ -12378,7 +12438,7 @@
         </is>
       </c>
       <c r="C383" s="2" t="n">
-        <v>45375</v>
+        <v>45403</v>
       </c>
       <c r="D383" t="n">
         <v>4</v>

</xml_diff>

<commit_message>
checklist french to english added and working
</commit_message>
<xml_diff>
--- a/time_spacing/words/words_V1.0.0.xlsx
+++ b/time_spacing/words/words_V1.0.0.xlsx
@@ -501,7 +501,7 @@
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D2" t="n">
         <v>2</v>
@@ -531,7 +531,7 @@
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D3" t="n">
         <v>7</v>
@@ -561,7 +561,7 @@
         </is>
       </c>
       <c r="C4" s="2" t="n">
-        <v>45404</v>
+        <v>45406</v>
       </c>
       <c r="D4" t="n">
         <v>8</v>
@@ -593,7 +593,7 @@
         </is>
       </c>
       <c r="C5" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D5" t="n">
         <v>7</v>
@@ -623,21 +623,23 @@
         </is>
       </c>
       <c r="C6" s="2" t="n">
-        <v>45403</v>
+        <v>45434</v>
       </c>
       <c r="D6" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
     </row>
@@ -653,7 +655,7 @@
         </is>
       </c>
       <c r="C7" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D7" t="n">
         <v>4</v>
@@ -683,7 +685,7 @@
         </is>
       </c>
       <c r="C8" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -713,7 +715,7 @@
         </is>
       </c>
       <c r="C9" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D9" t="n">
         <v>5</v>
@@ -743,7 +745,7 @@
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D10" t="n">
         <v>8</v>
@@ -773,7 +775,7 @@
         </is>
       </c>
       <c r="C11" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D11" t="n">
         <v>4</v>
@@ -837,7 +839,7 @@
         </is>
       </c>
       <c r="C13" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D13" t="n">
         <v>4</v>
@@ -867,21 +869,23 @@
         </is>
       </c>
       <c r="C14" s="2" t="n">
-        <v>45403</v>
+        <v>45435</v>
       </c>
       <c r="D14" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
     </row>
@@ -897,7 +901,7 @@
         </is>
       </c>
       <c r="C15" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D15" t="n">
         <v>5</v>
@@ -929,7 +933,7 @@
         </is>
       </c>
       <c r="C16" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D16" t="n">
         <v>7</v>
@@ -959,7 +963,7 @@
         </is>
       </c>
       <c r="C17" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D17" t="n">
         <v>8</v>
@@ -991,7 +995,7 @@
         </is>
       </c>
       <c r="C18" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D18" t="n">
         <v>5</v>
@@ -1023,7 +1027,7 @@
         </is>
       </c>
       <c r="C19" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D19" t="n">
         <v>8</v>
@@ -1053,7 +1057,7 @@
         </is>
       </c>
       <c r="C20" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D20" t="n">
         <v>4</v>
@@ -1083,7 +1087,7 @@
         </is>
       </c>
       <c r="C21" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D21" t="n">
         <v>4</v>
@@ -1113,7 +1117,7 @@
         </is>
       </c>
       <c r="C22" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D22" t="n">
         <v>6</v>
@@ -1143,7 +1147,7 @@
         </is>
       </c>
       <c r="C23" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D23" t="n">
         <v>3</v>
@@ -1173,7 +1177,7 @@
         </is>
       </c>
       <c r="C24" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D24" t="n">
         <v>5</v>
@@ -1235,7 +1239,7 @@
         </is>
       </c>
       <c r="C26" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D26" t="n">
         <v>7</v>
@@ -1265,7 +1269,7 @@
         </is>
       </c>
       <c r="C27" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D27" t="n">
         <v>8</v>
@@ -1297,7 +1301,7 @@
         </is>
       </c>
       <c r="C28" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D28" t="n">
         <v>5</v>
@@ -1329,7 +1333,7 @@
         </is>
       </c>
       <c r="C29" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D29" t="n">
         <v>7</v>
@@ -1359,7 +1363,7 @@
         </is>
       </c>
       <c r="C30" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D30" t="n">
         <v>8</v>
@@ -1391,7 +1395,7 @@
         </is>
       </c>
       <c r="C31" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D31" t="n">
         <v>4</v>
@@ -1423,7 +1427,7 @@
         </is>
       </c>
       <c r="C32" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D32" t="n">
         <v>4</v>
@@ -1455,7 +1459,7 @@
         </is>
       </c>
       <c r="C33" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D33" t="n">
         <v>8</v>
@@ -1487,7 +1491,7 @@
         </is>
       </c>
       <c r="C34" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D34" t="n">
         <v>4</v>
@@ -1531,7 +1535,7 @@
       <c r="G35" t="n">
         <v>1</v>
       </c>
-      <c r="H35" t="b">
+      <c r="H35" t="n">
         <v>1</v>
       </c>
       <c r="I35" t="inlineStr"/>
@@ -1549,7 +1553,7 @@
         </is>
       </c>
       <c r="C36" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D36" t="n">
         <v>4</v>
@@ -1579,7 +1583,7 @@
         </is>
       </c>
       <c r="C37" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D37" t="n">
         <v>3</v>
@@ -1609,7 +1613,7 @@
         </is>
       </c>
       <c r="C38" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D38" t="n">
         <v>8</v>
@@ -1641,7 +1645,7 @@
         </is>
       </c>
       <c r="C39" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D39" t="n">
         <v>7</v>
@@ -1671,7 +1675,7 @@
         </is>
       </c>
       <c r="C40" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D40" t="n">
         <v>4</v>
@@ -1701,7 +1705,7 @@
         </is>
       </c>
       <c r="C41" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D41" t="n">
         <v>2</v>
@@ -1747,7 +1751,7 @@
       <c r="G42" t="n">
         <v>1</v>
       </c>
-      <c r="H42" t="b">
+      <c r="H42" t="n">
         <v>0</v>
       </c>
       <c r="I42" t="inlineStr"/>
@@ -1765,7 +1769,7 @@
         </is>
       </c>
       <c r="C43" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D43" t="n">
         <v>5</v>
@@ -1797,7 +1801,7 @@
         </is>
       </c>
       <c r="C44" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D44" t="n">
         <v>4</v>
@@ -1827,7 +1831,7 @@
         </is>
       </c>
       <c r="C45" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D45" t="n">
         <v>7</v>
@@ -1889,7 +1893,7 @@
         </is>
       </c>
       <c r="C47" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D47" t="n">
         <v>3</v>
@@ -1919,7 +1923,7 @@
         </is>
       </c>
       <c r="C48" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D48" t="n">
         <v>3</v>
@@ -1949,7 +1953,7 @@
         </is>
       </c>
       <c r="C49" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D49" t="n">
         <v>2</v>
@@ -1995,7 +1999,7 @@
       <c r="G50" t="n">
         <v>1</v>
       </c>
-      <c r="H50" t="b">
+      <c r="H50" t="n">
         <v>0</v>
       </c>
       <c r="I50" t="inlineStr"/>
@@ -2013,7 +2017,7 @@
         </is>
       </c>
       <c r="C51" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D51" t="n">
         <v>5</v>
@@ -2045,7 +2049,7 @@
         </is>
       </c>
       <c r="C52" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D52" t="n">
         <v>3</v>
@@ -2075,7 +2079,7 @@
         </is>
       </c>
       <c r="C53" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D53" t="n">
         <v>3</v>
@@ -2105,7 +2109,7 @@
         </is>
       </c>
       <c r="C54" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D54" t="n">
         <v>5</v>
@@ -2135,7 +2139,7 @@
         </is>
       </c>
       <c r="C55" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D55" t="n">
         <v>7</v>
@@ -2165,7 +2169,7 @@
         </is>
       </c>
       <c r="C56" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D56" t="n">
         <v>4</v>
@@ -2195,7 +2199,7 @@
         </is>
       </c>
       <c r="C57" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D57" t="n">
         <v>8</v>
@@ -2227,7 +2231,7 @@
         </is>
       </c>
       <c r="C58" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D58" t="n">
         <v>7</v>
@@ -2257,7 +2261,7 @@
         </is>
       </c>
       <c r="C59" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D59" t="n">
         <v>7</v>
@@ -2287,7 +2291,7 @@
         </is>
       </c>
       <c r="C60" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D60" t="n">
         <v>4</v>
@@ -2319,10 +2323,10 @@
         </is>
       </c>
       <c r="C61" s="2" t="n">
-        <v>45404</v>
+        <v>45435</v>
       </c>
       <c r="D61" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E61" t="b">
         <v>0</v>
@@ -2331,12 +2335,14 @@
         <v>1</v>
       </c>
       <c r="G61" t="n">
-        <v>1</v>
-      </c>
-      <c r="H61" t="n">
-        <v>1</v>
-      </c>
-      <c r="I61" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="H61" t="b">
+        <v>0</v>
+      </c>
+      <c r="I61" t="n">
+        <v>1</v>
+      </c>
       <c r="J61" t="inlineStr"/>
     </row>
     <row r="62">
@@ -2351,7 +2357,7 @@
         </is>
       </c>
       <c r="C62" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D62" t="n">
         <v>4</v>
@@ -2381,21 +2387,23 @@
         </is>
       </c>
       <c r="C63" s="2" t="n">
-        <v>45403</v>
+        <v>45435</v>
       </c>
       <c r="D63" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E63" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F63" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G63" t="n">
-        <v>0</v>
-      </c>
-      <c r="H63" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H63" t="b">
+        <v>1</v>
+      </c>
       <c r="I63" t="inlineStr"/>
       <c r="J63" t="inlineStr"/>
     </row>
@@ -2411,7 +2419,7 @@
         </is>
       </c>
       <c r="C64" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D64" t="n">
         <v>4</v>
@@ -2441,7 +2449,7 @@
         </is>
       </c>
       <c r="C65" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D65" t="n">
         <v>7</v>
@@ -2471,7 +2479,7 @@
         </is>
       </c>
       <c r="C66" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D66" t="n">
         <v>5</v>
@@ -2503,7 +2511,7 @@
         </is>
       </c>
       <c r="C67" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D67" t="n">
         <v>2</v>
@@ -2535,7 +2543,7 @@
         </is>
       </c>
       <c r="C68" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D68" t="n">
         <v>4</v>
@@ -2565,7 +2573,7 @@
         </is>
       </c>
       <c r="C69" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D69" t="n">
         <v>4</v>
@@ -2595,7 +2603,7 @@
         </is>
       </c>
       <c r="C70" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D70" t="n">
         <v>7</v>
@@ -2625,7 +2633,7 @@
         </is>
       </c>
       <c r="C71" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D71" t="n">
         <v>1</v>
@@ -2657,7 +2665,7 @@
         </is>
       </c>
       <c r="C72" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D72" t="n">
         <v>5</v>
@@ -2689,7 +2697,7 @@
         </is>
       </c>
       <c r="C73" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D73" t="n">
         <v>8</v>
@@ -2721,7 +2729,7 @@
         </is>
       </c>
       <c r="C74" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D74" t="n">
         <v>3</v>
@@ -2751,7 +2759,7 @@
         </is>
       </c>
       <c r="C75" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D75" t="n">
         <v>4</v>
@@ -2783,7 +2791,7 @@
         </is>
       </c>
       <c r="C76" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D76" t="n">
         <v>2</v>
@@ -2813,7 +2821,7 @@
         </is>
       </c>
       <c r="C77" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D77" t="n">
         <v>3</v>
@@ -2843,7 +2851,7 @@
         </is>
       </c>
       <c r="C78" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D78" t="n">
         <v>7</v>
@@ -2873,7 +2881,7 @@
         </is>
       </c>
       <c r="C79" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D79" t="n">
         <v>5</v>
@@ -2905,7 +2913,7 @@
         </is>
       </c>
       <c r="C80" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D80" t="n">
         <v>7</v>
@@ -2935,7 +2943,7 @@
         </is>
       </c>
       <c r="C81" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D81" t="n">
         <v>7</v>
@@ -2965,7 +2973,7 @@
         </is>
       </c>
       <c r="C82" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D82" t="n">
         <v>8</v>
@@ -2997,7 +3005,7 @@
         </is>
       </c>
       <c r="C83" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D83" t="n">
         <v>4</v>
@@ -3029,7 +3037,7 @@
         </is>
       </c>
       <c r="C84" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D84" t="n">
         <v>4</v>
@@ -3059,7 +3067,7 @@
         </is>
       </c>
       <c r="C85" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D85" t="n">
         <v>4</v>
@@ -3089,7 +3097,7 @@
         </is>
       </c>
       <c r="C86" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D86" t="n">
         <v>3</v>
@@ -3119,7 +3127,7 @@
         </is>
       </c>
       <c r="C87" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D87" t="n">
         <v>3</v>
@@ -3149,7 +3157,7 @@
         </is>
       </c>
       <c r="C88" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D88" t="n">
         <v>7</v>
@@ -3179,7 +3187,7 @@
         </is>
       </c>
       <c r="C89" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D89" t="n">
         <v>7</v>
@@ -3209,7 +3217,7 @@
         </is>
       </c>
       <c r="C90" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D90" t="n">
         <v>4</v>
@@ -3241,7 +3249,7 @@
         </is>
       </c>
       <c r="C91" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D91" t="n">
         <v>4</v>
@@ -3271,7 +3279,7 @@
         </is>
       </c>
       <c r="C92" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D92" t="n">
         <v>7</v>
@@ -3301,7 +3309,7 @@
         </is>
       </c>
       <c r="C93" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D93" t="n">
         <v>4</v>
@@ -3331,7 +3339,7 @@
         </is>
       </c>
       <c r="C94" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D94" t="n">
         <v>4</v>
@@ -3361,7 +3369,7 @@
         </is>
       </c>
       <c r="C95" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D95" t="n">
         <v>3</v>
@@ -3391,7 +3399,7 @@
         </is>
       </c>
       <c r="C96" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D96" t="n">
         <v>3</v>
@@ -3421,7 +3429,7 @@
         </is>
       </c>
       <c r="C97" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D97" t="n">
         <v>0</v>
@@ -3451,7 +3459,7 @@
         </is>
       </c>
       <c r="C98" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D98" t="n">
         <v>3</v>
@@ -3481,7 +3489,7 @@
         </is>
       </c>
       <c r="C99" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D99" t="n">
         <v>5</v>
@@ -3511,7 +3519,7 @@
         </is>
       </c>
       <c r="C100" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D100" t="n">
         <v>2</v>
@@ -3543,7 +3551,7 @@
         </is>
       </c>
       <c r="C101" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D101" t="n">
         <v>5</v>
@@ -3573,7 +3581,7 @@
         </is>
       </c>
       <c r="C102" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D102" t="n">
         <v>1</v>
@@ -3603,7 +3611,7 @@
         </is>
       </c>
       <c r="C103" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D103" t="n">
         <v>4</v>
@@ -3667,7 +3675,7 @@
         </is>
       </c>
       <c r="C105" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D105" t="n">
         <v>5</v>
@@ -3699,7 +3707,7 @@
         </is>
       </c>
       <c r="C106" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D106" t="n">
         <v>3</v>
@@ -3729,7 +3737,7 @@
         </is>
       </c>
       <c r="C107" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D107" t="n">
         <v>5</v>
@@ -3759,7 +3767,7 @@
         </is>
       </c>
       <c r="C108" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D108" t="n">
         <v>8</v>
@@ -3789,7 +3797,7 @@
         </is>
       </c>
       <c r="C109" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D109" t="n">
         <v>3</v>
@@ -3819,7 +3827,7 @@
         </is>
       </c>
       <c r="C110" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D110" t="n">
         <v>1</v>
@@ -3851,7 +3859,7 @@
         </is>
       </c>
       <c r="C111" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D111" t="n">
         <v>1</v>
@@ -3881,7 +3889,7 @@
         </is>
       </c>
       <c r="C112" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D112" t="n">
         <v>2</v>
@@ -3911,7 +3919,7 @@
         </is>
       </c>
       <c r="C113" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D113" t="n">
         <v>5</v>
@@ -3941,7 +3949,7 @@
         </is>
       </c>
       <c r="C114" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D114" t="n">
         <v>3</v>
@@ -3971,7 +3979,7 @@
         </is>
       </c>
       <c r="C115" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D115" t="n">
         <v>4</v>
@@ -4001,7 +4009,7 @@
         </is>
       </c>
       <c r="C116" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D116" t="n">
         <v>4</v>
@@ -4031,7 +4039,7 @@
         </is>
       </c>
       <c r="C117" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D117" t="n">
         <v>4</v>
@@ -4063,7 +4071,7 @@
         </is>
       </c>
       <c r="C118" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D118" t="n">
         <v>2</v>
@@ -4095,7 +4103,7 @@
         </is>
       </c>
       <c r="C119" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D119" t="n">
         <v>5</v>
@@ -4127,7 +4135,7 @@
         </is>
       </c>
       <c r="C120" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D120" t="n">
         <v>7</v>
@@ -4157,7 +4165,7 @@
         </is>
       </c>
       <c r="C121" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D121" t="n">
         <v>4</v>
@@ -4187,7 +4195,7 @@
         </is>
       </c>
       <c r="C122" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D122" t="n">
         <v>3</v>
@@ -4217,7 +4225,7 @@
         </is>
       </c>
       <c r="C123" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D123" t="n">
         <v>4</v>
@@ -4247,7 +4255,7 @@
         </is>
       </c>
       <c r="C124" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D124" t="n">
         <v>3</v>
@@ -4277,7 +4285,7 @@
         </is>
       </c>
       <c r="C125" s="2" t="n">
-        <v>45405</v>
+        <v>45406</v>
       </c>
       <c r="D125" t="n">
         <v>2</v>
@@ -4309,7 +4317,7 @@
         </is>
       </c>
       <c r="C126" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D126" t="n">
         <v>3</v>
@@ -4339,7 +4347,7 @@
         </is>
       </c>
       <c r="C127" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D127" t="n">
         <v>7</v>
@@ -4369,7 +4377,7 @@
         </is>
       </c>
       <c r="C128" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D128" t="n">
         <v>8</v>
@@ -4401,7 +4409,7 @@
         </is>
       </c>
       <c r="C129" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D129" t="n">
         <v>5</v>
@@ -4433,7 +4441,7 @@
         </is>
       </c>
       <c r="C130" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D130" t="n">
         <v>4</v>
@@ -4465,7 +4473,7 @@
         </is>
       </c>
       <c r="C131" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D131" t="n">
         <v>7</v>
@@ -4495,7 +4503,7 @@
         </is>
       </c>
       <c r="C132" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D132" t="n">
         <v>4</v>
@@ -4525,7 +4533,7 @@
         </is>
       </c>
       <c r="C133" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D133" t="n">
         <v>4</v>
@@ -4555,27 +4563,29 @@
         </is>
       </c>
       <c r="C134" s="2" t="n">
-        <v>45403</v>
+        <v>45410</v>
       </c>
       <c r="D134" t="n">
+        <v>3</v>
+      </c>
+      <c r="E134" t="b">
+        <v>0</v>
+      </c>
+      <c r="F134" t="n">
         <v>2</v>
       </c>
-      <c r="E134" t="b">
-        <v>0</v>
-      </c>
-      <c r="F134" t="n">
-        <v>1</v>
-      </c>
       <c r="G134" t="n">
-        <v>2</v>
-      </c>
-      <c r="H134" t="n">
+        <v>3</v>
+      </c>
+      <c r="H134" t="b">
         <v>1</v>
       </c>
       <c r="I134" t="n">
-        <v>0</v>
-      </c>
-      <c r="J134" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="J134" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -4589,7 +4599,7 @@
         </is>
       </c>
       <c r="C135" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D135" t="n">
         <v>3</v>
@@ -4656,7 +4666,7 @@
         </is>
       </c>
       <c r="C137" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D137" t="n">
         <v>0</v>
@@ -4688,7 +4698,7 @@
         </is>
       </c>
       <c r="C138" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D138" t="n">
         <v>4</v>
@@ -4750,7 +4760,7 @@
         </is>
       </c>
       <c r="C140" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D140" t="n">
         <v>0</v>
@@ -4781,7 +4791,7 @@
         </is>
       </c>
       <c r="C141" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D141" t="n">
         <v>4</v>
@@ -4815,7 +4825,7 @@
         </is>
       </c>
       <c r="C142" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D142" t="n">
         <v>3</v>
@@ -4847,7 +4857,7 @@
         </is>
       </c>
       <c r="C143" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D143" t="n">
         <v>2</v>
@@ -4883,7 +4893,7 @@
         </is>
       </c>
       <c r="C144" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D144" t="n">
         <v>2</v>
@@ -4919,7 +4929,7 @@
         </is>
       </c>
       <c r="C145" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D145" t="n">
         <v>2</v>
@@ -4949,7 +4959,7 @@
         </is>
       </c>
       <c r="C146" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D146" t="n">
         <v>5</v>
@@ -4982,7 +4992,7 @@
         </is>
       </c>
       <c r="C147" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D147" t="n">
         <v>0</v>
@@ -5014,7 +5024,7 @@
         </is>
       </c>
       <c r="C148" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D148" t="n">
         <v>4</v>
@@ -5048,7 +5058,7 @@
         </is>
       </c>
       <c r="C149" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D149" t="n">
         <v>2</v>
@@ -5078,7 +5088,7 @@
         </is>
       </c>
       <c r="C150" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D150" t="n">
         <v>3</v>
@@ -5110,7 +5120,7 @@
         </is>
       </c>
       <c r="C151" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D151" t="n">
         <v>5</v>
@@ -5143,7 +5153,7 @@
         </is>
       </c>
       <c r="C152" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D152" t="n">
         <v>4</v>
@@ -5176,7 +5186,7 @@
         </is>
       </c>
       <c r="C153" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D153" t="n">
         <v>3</v>
@@ -5207,7 +5217,7 @@
         </is>
       </c>
       <c r="C154" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D154" t="n">
         <v>2</v>
@@ -5239,7 +5249,7 @@
         </is>
       </c>
       <c r="C155" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D155" t="n">
         <v>1</v>
@@ -5271,7 +5281,7 @@
         </is>
       </c>
       <c r="C156" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D156" t="n">
         <v>0</v>
@@ -5302,7 +5312,7 @@
         </is>
       </c>
       <c r="C157" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D157" t="n">
         <v>4</v>
@@ -5334,7 +5344,7 @@
         </is>
       </c>
       <c r="C158" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D158" t="n">
         <v>3</v>
@@ -5365,7 +5375,7 @@
         </is>
       </c>
       <c r="C159" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D159" t="n">
         <v>0</v>
@@ -5399,7 +5409,7 @@
         </is>
       </c>
       <c r="C160" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D160" t="n">
         <v>5</v>
@@ -5432,7 +5442,7 @@
         </is>
       </c>
       <c r="C161" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D161" t="n">
         <v>2</v>
@@ -5463,7 +5473,7 @@
         </is>
       </c>
       <c r="C162" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D162" t="n">
         <v>4</v>
@@ -5495,7 +5505,7 @@
         </is>
       </c>
       <c r="C163" s="2" t="n">
-        <v>45405</v>
+        <v>45406</v>
       </c>
       <c r="D163" t="n">
         <v>2</v>
@@ -5509,7 +5519,7 @@
       <c r="G163" t="n">
         <v>1</v>
       </c>
-      <c r="H163" t="b">
+      <c r="H163" t="n">
         <v>1</v>
       </c>
       <c r="I163" t="inlineStr"/>
@@ -5527,7 +5537,7 @@
         </is>
       </c>
       <c r="C164" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D164" t="n">
         <v>4</v>
@@ -5593,7 +5603,7 @@
         </is>
       </c>
       <c r="C166" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D166" t="n">
         <v>0</v>
@@ -5625,7 +5635,7 @@
         </is>
       </c>
       <c r="C167" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D167" t="n">
         <v>4</v>
@@ -5658,7 +5668,7 @@
         </is>
       </c>
       <c r="C168" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D168" t="n">
         <v>0</v>
@@ -5690,7 +5700,7 @@
         </is>
       </c>
       <c r="C169" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D169" t="n">
         <v>4</v>
@@ -5720,7 +5730,7 @@
         </is>
       </c>
       <c r="C170" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D170" t="n">
         <v>4</v>
@@ -5751,7 +5761,7 @@
         </is>
       </c>
       <c r="C171" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D171" t="n">
         <v>0</v>
@@ -5781,7 +5791,7 @@
         </is>
       </c>
       <c r="C172" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D172" t="n">
         <v>1</v>
@@ -5813,7 +5823,7 @@
         </is>
       </c>
       <c r="C173" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D173" t="n">
         <v>1</v>
@@ -5843,7 +5853,7 @@
         </is>
       </c>
       <c r="C174" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D174" t="n">
         <v>4</v>
@@ -5873,7 +5883,7 @@
         </is>
       </c>
       <c r="C175" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D175" t="n">
         <v>4</v>
@@ -5903,7 +5913,7 @@
         </is>
       </c>
       <c r="C176" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D176" t="n">
         <v>3</v>
@@ -5933,7 +5943,7 @@
         </is>
       </c>
       <c r="C177" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D177" t="n">
         <v>3</v>
@@ -5995,7 +6005,7 @@
         </is>
       </c>
       <c r="C179" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D179" t="n">
         <v>4</v>
@@ -6029,7 +6039,7 @@
         </is>
       </c>
       <c r="C180" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D180" t="n">
         <v>2</v>
@@ -6059,7 +6069,7 @@
         </is>
       </c>
       <c r="C181" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D181" t="n">
         <v>3</v>
@@ -6089,7 +6099,7 @@
         </is>
       </c>
       <c r="C182" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D182" t="n">
         <v>4</v>
@@ -6119,7 +6129,7 @@
         </is>
       </c>
       <c r="C183" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D183" t="n">
         <v>2</v>
@@ -6149,7 +6159,7 @@
         </is>
       </c>
       <c r="C184" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D184" t="n">
         <v>0</v>
@@ -6182,7 +6192,7 @@
         </is>
       </c>
       <c r="C185" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D185" t="n">
         <v>2</v>
@@ -6212,7 +6222,7 @@
         </is>
       </c>
       <c r="C186" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D186" t="n">
         <v>4</v>
@@ -6242,7 +6252,7 @@
         </is>
       </c>
       <c r="C187" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D187" t="n">
         <v>4</v>
@@ -6272,7 +6282,7 @@
         </is>
       </c>
       <c r="C188" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D188" t="n">
         <v>4</v>
@@ -6302,7 +6312,7 @@
         </is>
       </c>
       <c r="C189" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D189" t="n">
         <v>3</v>
@@ -6332,7 +6342,7 @@
         </is>
       </c>
       <c r="C190" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D190" t="n">
         <v>3</v>
@@ -6362,7 +6372,7 @@
         </is>
       </c>
       <c r="C191" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D191" t="n">
         <v>4</v>
@@ -6392,7 +6402,7 @@
         </is>
       </c>
       <c r="C192" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D192" t="n">
         <v>3</v>
@@ -6422,7 +6432,7 @@
         </is>
       </c>
       <c r="C193" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D193" t="n">
         <v>2</v>
@@ -6454,7 +6464,7 @@
         </is>
       </c>
       <c r="C194" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D194" t="n">
         <v>4</v>
@@ -6487,7 +6497,7 @@
         </is>
       </c>
       <c r="C195" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D195" t="n">
         <v>2</v>
@@ -6517,7 +6527,7 @@
         </is>
       </c>
       <c r="C196" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D196" t="n">
         <v>4</v>
@@ -6581,7 +6591,7 @@
         </is>
       </c>
       <c r="C198" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D198" t="n">
         <v>4</v>
@@ -6611,7 +6621,7 @@
         </is>
       </c>
       <c r="C199" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D199" t="n">
         <v>3</v>
@@ -6641,7 +6651,7 @@
         </is>
       </c>
       <c r="C200" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D200" t="n">
         <v>2</v>
@@ -6671,7 +6681,7 @@
         </is>
       </c>
       <c r="C201" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D201" t="n">
         <v>1</v>
@@ -6735,7 +6745,7 @@
         </is>
       </c>
       <c r="C203" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D203" t="n">
         <v>3</v>
@@ -6765,7 +6775,7 @@
         </is>
       </c>
       <c r="C204" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D204" t="n">
         <v>0</v>
@@ -6795,7 +6805,7 @@
         </is>
       </c>
       <c r="C205" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D205" t="n">
         <v>0</v>
@@ -6827,7 +6837,7 @@
         </is>
       </c>
       <c r="C206" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D206" t="n">
         <v>2</v>
@@ -6861,7 +6871,7 @@
         </is>
       </c>
       <c r="C207" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D207" t="n">
         <v>0</v>
@@ -6891,7 +6901,7 @@
         </is>
       </c>
       <c r="C208" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D208" t="n">
         <v>1</v>
@@ -6923,7 +6933,7 @@
         </is>
       </c>
       <c r="C209" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D209" t="n">
         <v>0</v>
@@ -6955,7 +6965,7 @@
         </is>
       </c>
       <c r="C210" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D210" t="n">
         <v>5</v>
@@ -6987,7 +6997,7 @@
         </is>
       </c>
       <c r="C211" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D211" t="n">
         <v>2</v>
@@ -7017,7 +7027,7 @@
         </is>
       </c>
       <c r="C212" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D212" t="n">
         <v>5</v>
@@ -7081,7 +7091,7 @@
         </is>
       </c>
       <c r="C214" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D214" t="n">
         <v>2</v>
@@ -7111,27 +7121,29 @@
         </is>
       </c>
       <c r="C215" s="2" t="n">
-        <v>45405</v>
+        <v>45410</v>
       </c>
       <c r="D215" t="n">
+        <v>3</v>
+      </c>
+      <c r="E215" t="b">
+        <v>1</v>
+      </c>
+      <c r="F215" t="n">
         <v>2</v>
       </c>
-      <c r="E215" t="b">
-        <v>0</v>
-      </c>
-      <c r="F215" t="n">
-        <v>1</v>
-      </c>
       <c r="G215" t="n">
-        <v>2</v>
-      </c>
-      <c r="H215" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="H215" t="b">
+        <v>1</v>
       </c>
       <c r="I215" t="n">
-        <v>1</v>
-      </c>
-      <c r="J215" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="J215" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -7145,7 +7157,7 @@
         </is>
       </c>
       <c r="C216" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D216" t="n">
         <v>2</v>
@@ -7175,7 +7187,7 @@
         </is>
       </c>
       <c r="C217" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D217" t="n">
         <v>1</v>
@@ -7207,7 +7219,7 @@
         </is>
       </c>
       <c r="C218" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D218" t="n">
         <v>1</v>
@@ -7241,7 +7253,7 @@
         </is>
       </c>
       <c r="C219" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D219" t="n">
         <v>5</v>
@@ -7273,7 +7285,7 @@
         </is>
       </c>
       <c r="C220" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D220" t="n">
         <v>5</v>
@@ -7305,7 +7317,7 @@
         </is>
       </c>
       <c r="C221" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D221" t="n">
         <v>1</v>
@@ -7339,7 +7351,7 @@
         </is>
       </c>
       <c r="C222" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D222" t="n">
         <v>3</v>
@@ -7370,7 +7382,7 @@
         </is>
       </c>
       <c r="C223" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D223" t="n">
         <v>1</v>
@@ -7402,7 +7414,7 @@
         </is>
       </c>
       <c r="C224" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D224" t="n">
         <v>0</v>
@@ -7432,7 +7444,7 @@
         </is>
       </c>
       <c r="C225" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D225" t="n">
         <v>2</v>
@@ -7465,7 +7477,7 @@
         </is>
       </c>
       <c r="C226" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D226" t="n">
         <v>2</v>
@@ -7495,7 +7507,7 @@
         </is>
       </c>
       <c r="C227" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D227" t="n">
         <v>4</v>
@@ -7529,10 +7541,10 @@
         </is>
       </c>
       <c r="C228" s="2" t="n">
-        <v>45403</v>
+        <v>45410</v>
       </c>
       <c r="D228" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E228" t="b">
         <v>0</v>
@@ -7541,9 +7553,11 @@
         <v>0</v>
       </c>
       <c r="G228" t="n">
-        <v>0</v>
-      </c>
-      <c r="H228" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H228" t="b">
+        <v>0</v>
+      </c>
       <c r="I228" t="inlineStr"/>
       <c r="J228" t="inlineStr"/>
     </row>
@@ -7559,7 +7573,7 @@
         </is>
       </c>
       <c r="C229" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D229" t="n">
         <v>4</v>
@@ -7589,7 +7603,7 @@
         </is>
       </c>
       <c r="C230" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D230" t="n">
         <v>3</v>
@@ -7633,7 +7647,7 @@
       <c r="G231" t="n">
         <v>1</v>
       </c>
-      <c r="H231" t="b">
+      <c r="H231" t="n">
         <v>1</v>
       </c>
       <c r="I231" t="inlineStr"/>
@@ -7654,7 +7668,7 @@
         </is>
       </c>
       <c r="C232" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D232" t="n">
         <v>0</v>
@@ -7684,7 +7698,7 @@
         </is>
       </c>
       <c r="C233" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D233" t="n">
         <v>2</v>
@@ -7716,7 +7730,7 @@
         </is>
       </c>
       <c r="C234" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D234" t="n">
         <v>3</v>
@@ -7748,7 +7762,7 @@
         </is>
       </c>
       <c r="C235" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D235" t="n">
         <v>2</v>
@@ -7779,7 +7793,7 @@
         </is>
       </c>
       <c r="C236" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D236" t="n">
         <v>3</v>
@@ -7809,7 +7823,7 @@
         </is>
       </c>
       <c r="C237" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D237" t="n">
         <v>4</v>
@@ -7841,7 +7855,7 @@
         </is>
       </c>
       <c r="C238" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D238" t="n">
         <v>1</v>
@@ -7871,7 +7885,7 @@
         </is>
       </c>
       <c r="C239" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D239" t="n">
         <v>2</v>
@@ -7901,7 +7915,7 @@
         </is>
       </c>
       <c r="C240" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D240" t="n">
         <v>1</v>
@@ -7931,7 +7945,7 @@
         </is>
       </c>
       <c r="C241" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D241" t="n">
         <v>3</v>
@@ -7961,7 +7975,7 @@
         </is>
       </c>
       <c r="C242" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D242" t="n">
         <v>2</v>
@@ -7991,7 +8005,7 @@
         </is>
       </c>
       <c r="C243" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D243" t="n">
         <v>2</v>
@@ -8021,7 +8035,7 @@
         </is>
       </c>
       <c r="C244" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D244" t="n">
         <v>4</v>
@@ -8054,7 +8068,7 @@
         </is>
       </c>
       <c r="C245" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D245" t="n">
         <v>1</v>
@@ -8088,7 +8102,7 @@
         </is>
       </c>
       <c r="C246" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D246" t="n">
         <v>0</v>
@@ -8118,7 +8132,7 @@
         </is>
       </c>
       <c r="C247" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D247" t="n">
         <v>3</v>
@@ -8150,7 +8164,7 @@
         </is>
       </c>
       <c r="C248" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D248" t="n">
         <v>0</v>
@@ -8182,7 +8196,7 @@
         </is>
       </c>
       <c r="C249" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D249" t="n">
         <v>3</v>
@@ -8212,7 +8226,7 @@
         </is>
       </c>
       <c r="C250" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D250" t="n">
         <v>0</v>
@@ -8242,7 +8256,7 @@
         </is>
       </c>
       <c r="C251" s="2" t="n">
-        <v>45404</v>
+        <v>45406</v>
       </c>
       <c r="D251" t="n">
         <v>1</v>
@@ -8274,7 +8288,7 @@
         </is>
       </c>
       <c r="C252" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D252" t="n">
         <v>3</v>
@@ -8307,7 +8321,7 @@
         </is>
       </c>
       <c r="C253" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D253" t="n">
         <v>0</v>
@@ -8341,7 +8355,7 @@
         </is>
       </c>
       <c r="C254" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D254" t="n">
         <v>2</v>
@@ -8371,7 +8385,7 @@
         </is>
       </c>
       <c r="C255" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D255" t="n">
         <v>0</v>
@@ -8401,7 +8415,7 @@
         </is>
       </c>
       <c r="C256" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D256" t="n">
         <v>3</v>
@@ -8463,7 +8477,7 @@
         </is>
       </c>
       <c r="C258" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D258" t="n">
         <v>1</v>
@@ -8495,7 +8509,7 @@
         </is>
       </c>
       <c r="C259" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D259" t="n">
         <v>3</v>
@@ -8529,7 +8543,7 @@
         </is>
       </c>
       <c r="C260" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D260" t="n">
         <v>3</v>
@@ -8561,7 +8575,7 @@
         </is>
       </c>
       <c r="C261" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D261" t="n">
         <v>2</v>
@@ -8591,7 +8605,7 @@
         </is>
       </c>
       <c r="C262" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D262" t="n">
         <v>2</v>
@@ -8621,7 +8635,7 @@
         </is>
       </c>
       <c r="C263" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D263" t="n">
         <v>0</v>
@@ -8651,7 +8665,7 @@
         </is>
       </c>
       <c r="C264" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D264" t="n">
         <v>1</v>
@@ -8681,7 +8695,7 @@
         </is>
       </c>
       <c r="C265" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D265" t="n">
         <v>0</v>
@@ -8713,7 +8727,7 @@
         </is>
       </c>
       <c r="C266" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D266" t="n">
         <v>3</v>
@@ -8743,7 +8757,7 @@
         </is>
       </c>
       <c r="C267" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D267" t="n">
         <v>4</v>
@@ -8773,7 +8787,7 @@
         </is>
       </c>
       <c r="C268" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D268" t="n">
         <v>3</v>
@@ -8805,7 +8819,7 @@
         </is>
       </c>
       <c r="C269" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D269" t="n">
         <v>4</v>
@@ -8835,7 +8849,7 @@
         </is>
       </c>
       <c r="C270" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D270" t="n">
         <v>2</v>
@@ -8866,7 +8880,7 @@
         </is>
       </c>
       <c r="C271" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D271" t="n">
         <v>4</v>
@@ -8896,7 +8910,7 @@
         </is>
       </c>
       <c r="C272" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D272" t="n">
         <v>4</v>
@@ -8928,7 +8942,7 @@
         </is>
       </c>
       <c r="C273" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D273" t="n">
         <v>0</v>
@@ -8960,7 +8974,7 @@
         </is>
       </c>
       <c r="C274" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D274" t="n">
         <v>0</v>
@@ -8990,7 +9004,7 @@
         </is>
       </c>
       <c r="C275" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D275" t="n">
         <v>0</v>
@@ -9022,7 +9036,7 @@
         </is>
       </c>
       <c r="C276" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D276" t="n">
         <v>0</v>
@@ -9052,7 +9066,7 @@
         </is>
       </c>
       <c r="C277" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D277" t="n">
         <v>2</v>
@@ -9085,7 +9099,7 @@
         </is>
       </c>
       <c r="C278" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D278" t="n">
         <v>0</v>
@@ -9118,7 +9132,7 @@
         </is>
       </c>
       <c r="C279" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D279" t="n">
         <v>2</v>
@@ -9151,7 +9165,7 @@
         </is>
       </c>
       <c r="C280" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D280" t="n">
         <v>0</v>
@@ -9181,7 +9195,7 @@
         </is>
       </c>
       <c r="C281" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D281" t="n">
         <v>2</v>
@@ -9211,7 +9225,7 @@
         </is>
       </c>
       <c r="C282" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D282" t="n">
         <v>0</v>
@@ -9241,7 +9255,7 @@
         </is>
       </c>
       <c r="C283" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D283" t="n">
         <v>0</v>
@@ -9274,7 +9288,7 @@
         </is>
       </c>
       <c r="C284" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D284" t="n">
         <v>0</v>
@@ -9307,7 +9321,7 @@
         </is>
       </c>
       <c r="C285" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D285" t="n">
         <v>3</v>
@@ -9339,7 +9353,7 @@
         </is>
       </c>
       <c r="C286" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D286" t="n">
         <v>4</v>
@@ -9373,7 +9387,7 @@
         </is>
       </c>
       <c r="C287" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D287" t="n">
         <v>0</v>
@@ -9405,7 +9419,7 @@
         </is>
       </c>
       <c r="C288" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D288" t="n">
         <v>1</v>
@@ -9436,7 +9450,7 @@
         </is>
       </c>
       <c r="C289" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D289" t="n">
         <v>5</v>
@@ -9468,7 +9482,7 @@
         </is>
       </c>
       <c r="C290" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D290" t="n">
         <v>0</v>
@@ -9498,7 +9512,7 @@
         </is>
       </c>
       <c r="C291" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D291" t="n">
         <v>1</v>
@@ -9528,7 +9542,7 @@
         </is>
       </c>
       <c r="C292" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D292" t="n">
         <v>0</v>
@@ -9559,7 +9573,7 @@
         </is>
       </c>
       <c r="C293" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D293" t="n">
         <v>0</v>
@@ -9590,7 +9604,7 @@
         </is>
       </c>
       <c r="C294" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D294" t="n">
         <v>3</v>
@@ -9623,7 +9637,7 @@
         </is>
       </c>
       <c r="C295" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D295" t="n">
         <v>0</v>
@@ -9653,7 +9667,7 @@
         </is>
       </c>
       <c r="C296" s="2" t="n">
-        <v>45404</v>
+        <v>45406</v>
       </c>
       <c r="D296" t="n">
         <v>0</v>
@@ -9687,7 +9701,7 @@
         </is>
       </c>
       <c r="C297" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D297" t="n">
         <v>0</v>
@@ -9719,7 +9733,7 @@
         </is>
       </c>
       <c r="C298" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D298" t="n">
         <v>3</v>
@@ -9749,7 +9763,7 @@
         </is>
       </c>
       <c r="C299" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D299" t="n">
         <v>3</v>
@@ -9780,7 +9794,7 @@
         </is>
       </c>
       <c r="C300" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D300" t="n">
         <v>4</v>
@@ -9813,7 +9827,7 @@
         </is>
       </c>
       <c r="C301" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D301" t="n">
         <v>2</v>
@@ -9847,7 +9861,7 @@
         </is>
       </c>
       <c r="C302" s="2" t="n">
-        <v>45405</v>
+        <v>45406</v>
       </c>
       <c r="D302" t="n">
         <v>2</v>
@@ -9881,7 +9895,7 @@
         </is>
       </c>
       <c r="C303" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D303" t="n">
         <v>1</v>
@@ -9912,7 +9926,7 @@
         </is>
       </c>
       <c r="C304" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D304" t="n">
         <v>4</v>
@@ -9943,7 +9957,7 @@
         </is>
       </c>
       <c r="C305" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D305" t="n">
         <v>0</v>
@@ -9976,7 +9990,7 @@
         </is>
       </c>
       <c r="C306" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D306" t="n">
         <v>0</v>
@@ -10006,10 +10020,10 @@
         </is>
       </c>
       <c r="C307" s="2" t="n">
-        <v>45403</v>
+        <v>45407</v>
       </c>
       <c r="D307" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E307" t="b">
         <v>0</v>
@@ -10018,15 +10032,17 @@
         <v>2</v>
       </c>
       <c r="G307" t="n">
-        <v>2</v>
-      </c>
-      <c r="H307" t="n">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="H307" t="b">
+        <v>0</v>
       </c>
       <c r="I307" t="n">
         <v>1</v>
       </c>
-      <c r="J307" t="inlineStr"/>
+      <c r="J307" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
@@ -10040,7 +10056,7 @@
         </is>
       </c>
       <c r="C308" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D308" t="n">
         <v>0</v>
@@ -10070,7 +10086,7 @@
         </is>
       </c>
       <c r="C309" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D309" t="n">
         <v>1</v>
@@ -10105,7 +10121,7 @@
         </is>
       </c>
       <c r="C310" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D310" t="n">
         <v>4</v>
@@ -10137,7 +10153,7 @@
         </is>
       </c>
       <c r="C311" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D311" t="n">
         <v>1</v>
@@ -10171,7 +10187,7 @@
         </is>
       </c>
       <c r="C312" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D312" t="n">
         <v>0</v>
@@ -10203,7 +10219,7 @@
         </is>
       </c>
       <c r="C313" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D313" t="n">
         <v>3</v>
@@ -10234,7 +10250,7 @@
         </is>
       </c>
       <c r="C314" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D314" t="n">
         <v>2</v>
@@ -10267,7 +10283,7 @@
         </is>
       </c>
       <c r="C315" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D315" t="n">
         <v>4</v>
@@ -10313,7 +10329,7 @@
       <c r="G316" t="n">
         <v>1</v>
       </c>
-      <c r="H316" t="b">
+      <c r="H316" t="n">
         <v>1</v>
       </c>
       <c r="I316" t="inlineStr"/>
@@ -10332,7 +10348,7 @@
         </is>
       </c>
       <c r="C317" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D317" t="n">
         <v>2</v>
@@ -10362,7 +10378,7 @@
         </is>
       </c>
       <c r="C318" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D318" t="n">
         <v>0</v>
@@ -10394,7 +10410,7 @@
         </is>
       </c>
       <c r="C319" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D319" t="n">
         <v>0</v>
@@ -10429,7 +10445,7 @@
         </is>
       </c>
       <c r="C320" s="2" t="n">
-        <v>45404</v>
+        <v>45406</v>
       </c>
       <c r="D320" t="n">
         <v>1</v>
@@ -10465,7 +10481,7 @@
         </is>
       </c>
       <c r="C321" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D321" t="n">
         <v>1</v>
@@ -10499,7 +10515,7 @@
         </is>
       </c>
       <c r="C322" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D322" t="n">
         <v>4</v>
@@ -10530,7 +10546,7 @@
         </is>
       </c>
       <c r="C323" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D323" t="n">
         <v>2</v>
@@ -10566,7 +10582,7 @@
         </is>
       </c>
       <c r="C324" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D324" t="n">
         <v>1</v>
@@ -10614,7 +10630,7 @@
       <c r="G325" t="n">
         <v>1</v>
       </c>
-      <c r="H325" t="b">
+      <c r="H325" t="n">
         <v>1</v>
       </c>
       <c r="I325" t="inlineStr"/>
@@ -10633,7 +10649,7 @@
         </is>
       </c>
       <c r="C326" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D326" t="n">
         <v>1</v>
@@ -10666,7 +10682,7 @@
         </is>
       </c>
       <c r="C327" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D327" t="n">
         <v>3</v>
@@ -10701,7 +10717,7 @@
         </is>
       </c>
       <c r="C328" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D328" t="n">
         <v>0</v>
@@ -10731,7 +10747,7 @@
         </is>
       </c>
       <c r="C329" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D329" t="n">
         <v>0</v>
@@ -10761,7 +10777,7 @@
         </is>
       </c>
       <c r="C330" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D330" t="n">
         <v>2</v>
@@ -10796,7 +10812,7 @@
         </is>
       </c>
       <c r="C331" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D331" t="n">
         <v>0</v>
@@ -10828,7 +10844,7 @@
         </is>
       </c>
       <c r="C332" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D332" t="n">
         <v>2</v>
@@ -10863,7 +10879,7 @@
         </is>
       </c>
       <c r="C333" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D333" t="n">
         <v>0</v>
@@ -10893,7 +10909,7 @@
         </is>
       </c>
       <c r="C334" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D334" t="n">
         <v>3</v>
@@ -10924,7 +10940,7 @@
         </is>
       </c>
       <c r="C335" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D335" t="n">
         <v>0</v>
@@ -10954,7 +10970,7 @@
         </is>
       </c>
       <c r="C336" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D336" t="n">
         <v>0</v>
@@ -10984,7 +11000,7 @@
         </is>
       </c>
       <c r="C337" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D337" t="n">
         <v>2</v>
@@ -11016,7 +11032,7 @@
         </is>
       </c>
       <c r="C338" s="2" t="n">
-        <v>45404</v>
+        <v>45406</v>
       </c>
       <c r="D338" t="n">
         <v>0</v>
@@ -11048,7 +11064,7 @@
         </is>
       </c>
       <c r="C339" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D339" t="n">
         <v>0</v>
@@ -11078,7 +11094,7 @@
         </is>
       </c>
       <c r="C340" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D340" t="n">
         <v>4</v>
@@ -11110,7 +11126,7 @@
         </is>
       </c>
       <c r="C341" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D341" t="n">
         <v>4</v>
@@ -11142,7 +11158,7 @@
         </is>
       </c>
       <c r="C342" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D342" t="n">
         <v>4</v>
@@ -11172,7 +11188,7 @@
         </is>
       </c>
       <c r="C343" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D343" t="n">
         <v>3</v>
@@ -11202,7 +11218,7 @@
         </is>
       </c>
       <c r="C344" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D344" t="n">
         <v>4</v>
@@ -11235,7 +11251,7 @@
         </is>
       </c>
       <c r="C345" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D345" t="n">
         <v>2</v>
@@ -11268,7 +11284,7 @@
         </is>
       </c>
       <c r="C346" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D346" t="n">
         <v>3</v>
@@ -11302,7 +11318,7 @@
         </is>
       </c>
       <c r="C347" s="2" t="n">
-        <v>45404</v>
+        <v>45406</v>
       </c>
       <c r="D347" t="n">
         <v>1</v>
@@ -11316,7 +11332,7 @@
       <c r="G347" t="n">
         <v>2</v>
       </c>
-      <c r="H347" t="b">
+      <c r="H347" t="n">
         <v>1</v>
       </c>
       <c r="I347" t="n">
@@ -11339,7 +11355,7 @@
         </is>
       </c>
       <c r="C348" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D348" t="n">
         <v>0</v>
@@ -11369,7 +11385,7 @@
         </is>
       </c>
       <c r="C349" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D349" t="n">
         <v>2</v>
@@ -11399,7 +11415,7 @@
         </is>
       </c>
       <c r="C350" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D350" t="n">
         <v>0</v>
@@ -11431,7 +11447,7 @@
         </is>
       </c>
       <c r="C351" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D351" t="n">
         <v>5</v>
@@ -11463,24 +11479,26 @@
         </is>
       </c>
       <c r="C352" s="2" t="n">
-        <v>45403</v>
+        <v>45407</v>
       </c>
       <c r="D352" t="n">
         <v>0</v>
       </c>
       <c r="E352" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F352" t="n">
         <v>0</v>
       </c>
       <c r="G352" t="n">
-        <v>1</v>
-      </c>
-      <c r="H352" t="n">
-        <v>0</v>
-      </c>
-      <c r="I352" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="H352" t="b">
+        <v>0</v>
+      </c>
+      <c r="I352" t="n">
+        <v>0</v>
+      </c>
       <c r="J352" t="inlineStr"/>
     </row>
     <row r="353">
@@ -11495,7 +11513,7 @@
         </is>
       </c>
       <c r="C353" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D353" t="n">
         <v>3</v>
@@ -11525,7 +11543,7 @@
         </is>
       </c>
       <c r="C354" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D354" t="n">
         <v>2</v>
@@ -11555,7 +11573,7 @@
         </is>
       </c>
       <c r="C355" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D355" t="n">
         <v>4</v>
@@ -11589,7 +11607,7 @@
         </is>
       </c>
       <c r="C356" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D356" t="n">
         <v>1</v>
@@ -11622,7 +11640,7 @@
         </is>
       </c>
       <c r="C357" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D357" t="n">
         <v>4</v>
@@ -11652,7 +11670,7 @@
         </is>
       </c>
       <c r="C358" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D358" t="n">
         <v>0</v>
@@ -11684,7 +11702,7 @@
         </is>
       </c>
       <c r="C359" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D359" t="n">
         <v>4</v>
@@ -11715,7 +11733,7 @@
         </is>
       </c>
       <c r="C360" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D360" t="n">
         <v>0</v>
@@ -11747,7 +11765,7 @@
         </is>
       </c>
       <c r="C361" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D361" t="n">
         <v>4</v>
@@ -11777,7 +11795,7 @@
         </is>
       </c>
       <c r="C362" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D362" t="n">
         <v>0</v>
@@ -11809,7 +11827,7 @@
         </is>
       </c>
       <c r="C363" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D363" t="n">
         <v>3</v>
@@ -11841,7 +11859,7 @@
         </is>
       </c>
       <c r="C364" s="2" t="n">
-        <v>45404</v>
+        <v>45406</v>
       </c>
       <c r="D364" t="n">
         <v>0</v>
@@ -11876,7 +11894,7 @@
         </is>
       </c>
       <c r="C365" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D365" t="n">
         <v>2</v>
@@ -11908,7 +11926,7 @@
         </is>
       </c>
       <c r="C366" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D366" t="n">
         <v>0</v>
@@ -11940,7 +11958,7 @@
         </is>
       </c>
       <c r="C367" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D367" t="n">
         <v>0</v>
@@ -11971,7 +11989,7 @@
         </is>
       </c>
       <c r="C368" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D368" t="n">
         <v>3</v>
@@ -12001,7 +12019,7 @@
         </is>
       </c>
       <c r="C369" s="2" t="n">
-        <v>45404</v>
+        <v>45406</v>
       </c>
       <c r="D369" t="n">
         <v>1</v>
@@ -12015,7 +12033,7 @@
       <c r="G369" t="n">
         <v>1</v>
       </c>
-      <c r="H369" t="b">
+      <c r="H369" t="n">
         <v>0</v>
       </c>
       <c r="I369" t="inlineStr"/>
@@ -12035,7 +12053,7 @@
         </is>
       </c>
       <c r="C370" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D370" t="n">
         <v>3</v>
@@ -12067,7 +12085,7 @@
         </is>
       </c>
       <c r="C371" s="2" t="n">
-        <v>45404</v>
+        <v>45406</v>
       </c>
       <c r="D371" t="n">
         <v>1</v>
@@ -12081,7 +12099,7 @@
       <c r="G371" t="n">
         <v>1</v>
       </c>
-      <c r="H371" t="b">
+      <c r="H371" t="n">
         <v>1</v>
       </c>
       <c r="I371" t="inlineStr"/>
@@ -12100,7 +12118,7 @@
         </is>
       </c>
       <c r="C372" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D372" t="n">
         <v>0</v>
@@ -12132,7 +12150,7 @@
         </is>
       </c>
       <c r="C373" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D373" t="n">
         <v>1</v>
@@ -12162,7 +12180,7 @@
         </is>
       </c>
       <c r="C374" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D374" t="n">
         <v>3</v>
@@ -12192,7 +12210,7 @@
         </is>
       </c>
       <c r="C375" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D375" t="n">
         <v>3</v>
@@ -12223,7 +12241,7 @@
         </is>
       </c>
       <c r="C376" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D376" t="n">
         <v>0</v>
@@ -12253,7 +12271,7 @@
         </is>
       </c>
       <c r="C377" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D377" t="n">
         <v>1</v>
@@ -12285,7 +12303,7 @@
         </is>
       </c>
       <c r="C378" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D378" t="n">
         <v>0</v>
@@ -12317,21 +12335,23 @@
         </is>
       </c>
       <c r="C379" s="2" t="n">
-        <v>45403</v>
+        <v>45421</v>
       </c>
       <c r="D379" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E379" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F379" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G379" t="n">
-        <v>0</v>
-      </c>
-      <c r="H379" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H379" t="b">
+        <v>1</v>
+      </c>
       <c r="I379" t="inlineStr"/>
       <c r="J379" t="inlineStr"/>
     </row>
@@ -12348,7 +12368,7 @@
         </is>
       </c>
       <c r="C380" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D380" t="n">
         <v>1</v>
@@ -12378,7 +12398,7 @@
         </is>
       </c>
       <c r="C381" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D381" t="n">
         <v>0</v>
@@ -12408,7 +12428,7 @@
         </is>
       </c>
       <c r="C382" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D382" t="n">
         <v>0</v>
@@ -12438,7 +12458,7 @@
         </is>
       </c>
       <c r="C383" s="2" t="n">
-        <v>45403</v>
+        <v>45406</v>
       </c>
       <c r="D383" t="n">
         <v>4</v>

</xml_diff>

<commit_message>
hide start menu at quiz beginning and display series score at the end
</commit_message>
<xml_diff>
--- a/time_spacing/words/words_V1.0.0.xlsx
+++ b/time_spacing/words/words_V1.0.0.xlsx
@@ -501,7 +501,7 @@
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D2" t="n">
         <v>2</v>
@@ -531,7 +531,7 @@
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D3" t="n">
         <v>7</v>
@@ -561,7 +561,7 @@
         </is>
       </c>
       <c r="C4" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D4" t="n">
         <v>8</v>
@@ -593,7 +593,7 @@
         </is>
       </c>
       <c r="C5" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D5" t="n">
         <v>7</v>
@@ -637,7 +637,7 @@
       <c r="G6" t="n">
         <v>1</v>
       </c>
-      <c r="H6" t="b">
+      <c r="H6" t="n">
         <v>1</v>
       </c>
       <c r="I6" t="inlineStr"/>
@@ -655,7 +655,7 @@
         </is>
       </c>
       <c r="C7" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D7" t="n">
         <v>4</v>
@@ -685,7 +685,7 @@
         </is>
       </c>
       <c r="C8" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -715,10 +715,10 @@
         </is>
       </c>
       <c r="C9" s="2" t="n">
-        <v>45406</v>
+        <v>45422</v>
       </c>
       <c r="D9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
@@ -727,9 +727,11 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
     </row>
@@ -745,7 +747,7 @@
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D10" t="n">
         <v>8</v>
@@ -775,7 +777,7 @@
         </is>
       </c>
       <c r="C11" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D11" t="n">
         <v>4</v>
@@ -839,21 +841,23 @@
         </is>
       </c>
       <c r="C13" s="2" t="n">
-        <v>45406</v>
+        <v>45433</v>
       </c>
       <c r="D13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1</v>
+      </c>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
     </row>
@@ -883,7 +887,7 @@
       <c r="G14" t="n">
         <v>1</v>
       </c>
-      <c r="H14" t="b">
+      <c r="H14" t="n">
         <v>1</v>
       </c>
       <c r="I14" t="inlineStr"/>
@@ -901,7 +905,7 @@
         </is>
       </c>
       <c r="C15" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D15" t="n">
         <v>5</v>
@@ -933,7 +937,7 @@
         </is>
       </c>
       <c r="C16" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D16" t="n">
         <v>7</v>
@@ -963,7 +967,7 @@
         </is>
       </c>
       <c r="C17" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D17" t="n">
         <v>8</v>
@@ -995,10 +999,10 @@
         </is>
       </c>
       <c r="C18" s="2" t="n">
-        <v>45406</v>
+        <v>45422</v>
       </c>
       <c r="D18" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
@@ -1007,12 +1011,14 @@
         <v>1</v>
       </c>
       <c r="G18" t="n">
-        <v>1</v>
-      </c>
-      <c r="H18" t="n">
-        <v>1</v>
-      </c>
-      <c r="I18" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="H18" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1</v>
+      </c>
       <c r="J18" t="inlineStr"/>
     </row>
     <row r="19">
@@ -1027,7 +1033,7 @@
         </is>
       </c>
       <c r="C19" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D19" t="n">
         <v>8</v>
@@ -1057,10 +1063,10 @@
         </is>
       </c>
       <c r="C20" s="2" t="n">
-        <v>45406</v>
+        <v>45411</v>
       </c>
       <c r="D20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E20" t="b">
         <v>0</v>
@@ -1069,9 +1075,11 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>0</v>
-      </c>
-      <c r="H20" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H20" t="b">
+        <v>0</v>
+      </c>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
     </row>
@@ -1087,7 +1095,7 @@
         </is>
       </c>
       <c r="C21" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D21" t="n">
         <v>4</v>
@@ -1117,21 +1125,23 @@
         </is>
       </c>
       <c r="C22" s="2" t="n">
-        <v>45406</v>
+        <v>45436</v>
       </c>
       <c r="D22" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E22" t="b">
         <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" t="n">
-        <v>0</v>
-      </c>
-      <c r="H22" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1</v>
+      </c>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
     </row>
@@ -1147,7 +1157,7 @@
         </is>
       </c>
       <c r="C23" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D23" t="n">
         <v>3</v>
@@ -1177,7 +1187,7 @@
         </is>
       </c>
       <c r="C24" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D24" t="n">
         <v>5</v>
@@ -1239,7 +1249,7 @@
         </is>
       </c>
       <c r="C26" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D26" t="n">
         <v>7</v>
@@ -1269,7 +1279,7 @@
         </is>
       </c>
       <c r="C27" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D27" t="n">
         <v>8</v>
@@ -1301,7 +1311,7 @@
         </is>
       </c>
       <c r="C28" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D28" t="n">
         <v>5</v>
@@ -1333,7 +1343,7 @@
         </is>
       </c>
       <c r="C29" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D29" t="n">
         <v>7</v>
@@ -1363,7 +1373,7 @@
         </is>
       </c>
       <c r="C30" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D30" t="n">
         <v>8</v>
@@ -1395,7 +1405,7 @@
         </is>
       </c>
       <c r="C31" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D31" t="n">
         <v>4</v>
@@ -1427,7 +1437,7 @@
         </is>
       </c>
       <c r="C32" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D32" t="n">
         <v>4</v>
@@ -1459,7 +1469,7 @@
         </is>
       </c>
       <c r="C33" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D33" t="n">
         <v>8</v>
@@ -1491,7 +1501,7 @@
         </is>
       </c>
       <c r="C34" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D34" t="n">
         <v>4</v>
@@ -1553,7 +1563,7 @@
         </is>
       </c>
       <c r="C36" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D36" t="n">
         <v>4</v>
@@ -1583,7 +1593,7 @@
         </is>
       </c>
       <c r="C37" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D37" t="n">
         <v>3</v>
@@ -1613,7 +1623,7 @@
         </is>
       </c>
       <c r="C38" s="2" t="n">
-        <v>45406</v>
+        <v>45436</v>
       </c>
       <c r="D38" t="n">
         <v>8</v>
@@ -1622,15 +1632,17 @@
         <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G38" t="n">
-        <v>1</v>
-      </c>
-      <c r="H38" t="n">
-        <v>1</v>
-      </c>
-      <c r="I38" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="H38" t="b">
+        <v>1</v>
+      </c>
+      <c r="I38" t="n">
+        <v>1</v>
+      </c>
       <c r="J38" t="inlineStr"/>
     </row>
     <row r="39">
@@ -1645,7 +1657,7 @@
         </is>
       </c>
       <c r="C39" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D39" t="n">
         <v>7</v>
@@ -1675,21 +1687,23 @@
         </is>
       </c>
       <c r="C40" s="2" t="n">
-        <v>45406</v>
+        <v>45433</v>
       </c>
       <c r="D40" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E40" t="b">
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40" t="n">
-        <v>0</v>
-      </c>
-      <c r="H40" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H40" t="n">
+        <v>1</v>
+      </c>
       <c r="I40" t="inlineStr"/>
       <c r="J40" t="inlineStr"/>
     </row>
@@ -1705,24 +1719,26 @@
         </is>
       </c>
       <c r="C41" s="2" t="n">
-        <v>45406</v>
+        <v>45411</v>
       </c>
       <c r="D41" t="n">
+        <v>3</v>
+      </c>
+      <c r="E41" t="b">
+        <v>0</v>
+      </c>
+      <c r="F41" t="n">
+        <v>1</v>
+      </c>
+      <c r="G41" t="n">
         <v>2</v>
       </c>
-      <c r="E41" t="b">
-        <v>0</v>
-      </c>
-      <c r="F41" t="n">
-        <v>0</v>
-      </c>
-      <c r="G41" t="n">
-        <v>1</v>
-      </c>
       <c r="H41" t="n">
-        <v>0</v>
-      </c>
-      <c r="I41" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0</v>
+      </c>
       <c r="J41" t="inlineStr"/>
     </row>
     <row r="42">
@@ -1769,7 +1785,7 @@
         </is>
       </c>
       <c r="C43" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D43" t="n">
         <v>5</v>
@@ -1801,7 +1817,7 @@
         </is>
       </c>
       <c r="C44" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D44" t="n">
         <v>4</v>
@@ -1831,7 +1847,7 @@
         </is>
       </c>
       <c r="C45" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D45" t="n">
         <v>7</v>
@@ -1893,7 +1909,7 @@
         </is>
       </c>
       <c r="C47" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D47" t="n">
         <v>3</v>
@@ -1923,10 +1939,10 @@
         </is>
       </c>
       <c r="C48" s="2" t="n">
-        <v>45406</v>
+        <v>45409</v>
       </c>
       <c r="D48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E48" t="b">
         <v>0</v>
@@ -1935,9 +1951,11 @@
         <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>0</v>
-      </c>
-      <c r="H48" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H48" t="b">
+        <v>0</v>
+      </c>
       <c r="I48" t="inlineStr"/>
       <c r="J48" t="inlineStr"/>
     </row>
@@ -1953,7 +1971,7 @@
         </is>
       </c>
       <c r="C49" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D49" t="n">
         <v>2</v>
@@ -2017,24 +2035,26 @@
         </is>
       </c>
       <c r="C51" s="2" t="n">
-        <v>45406</v>
+        <v>45435</v>
       </c>
       <c r="D51" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E51" t="b">
         <v>0</v>
       </c>
       <c r="F51" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G51" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H51" t="n">
         <v>1</v>
       </c>
-      <c r="I51" t="inlineStr"/>
+      <c r="I51" t="n">
+        <v>1</v>
+      </c>
       <c r="J51" t="inlineStr"/>
     </row>
     <row r="52">
@@ -2049,7 +2069,7 @@
         </is>
       </c>
       <c r="C52" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D52" t="n">
         <v>3</v>
@@ -2079,7 +2099,7 @@
         </is>
       </c>
       <c r="C53" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D53" t="n">
         <v>3</v>
@@ -2109,7 +2129,7 @@
         </is>
       </c>
       <c r="C54" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D54" t="n">
         <v>5</v>
@@ -2139,7 +2159,7 @@
         </is>
       </c>
       <c r="C55" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D55" t="n">
         <v>7</v>
@@ -2169,7 +2189,7 @@
         </is>
       </c>
       <c r="C56" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D56" t="n">
         <v>4</v>
@@ -2199,7 +2219,7 @@
         </is>
       </c>
       <c r="C57" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D57" t="n">
         <v>8</v>
@@ -2231,21 +2251,23 @@
         </is>
       </c>
       <c r="C58" s="2" t="n">
-        <v>45406</v>
+        <v>45436</v>
       </c>
       <c r="D58" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E58" t="b">
         <v>0</v>
       </c>
       <c r="F58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G58" t="n">
-        <v>0</v>
-      </c>
-      <c r="H58" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H58" t="b">
+        <v>1</v>
+      </c>
       <c r="I58" t="inlineStr"/>
       <c r="J58" t="inlineStr"/>
     </row>
@@ -2261,7 +2283,7 @@
         </is>
       </c>
       <c r="C59" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D59" t="n">
         <v>7</v>
@@ -2291,24 +2313,26 @@
         </is>
       </c>
       <c r="C60" s="2" t="n">
-        <v>45406</v>
+        <v>45433</v>
       </c>
       <c r="D60" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E60" t="b">
         <v>0</v>
       </c>
       <c r="F60" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G60" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H60" t="n">
         <v>1</v>
       </c>
-      <c r="I60" t="inlineStr"/>
+      <c r="I60" t="n">
+        <v>1</v>
+      </c>
       <c r="J60" t="inlineStr"/>
     </row>
     <row r="61">
@@ -2337,7 +2361,7 @@
       <c r="G61" t="n">
         <v>2</v>
       </c>
-      <c r="H61" t="b">
+      <c r="H61" t="n">
         <v>0</v>
       </c>
       <c r="I61" t="n">
@@ -2357,7 +2381,7 @@
         </is>
       </c>
       <c r="C62" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D62" t="n">
         <v>4</v>
@@ -2401,7 +2425,7 @@
       <c r="G63" t="n">
         <v>1</v>
       </c>
-      <c r="H63" t="b">
+      <c r="H63" t="n">
         <v>1</v>
       </c>
       <c r="I63" t="inlineStr"/>
@@ -2419,7 +2443,7 @@
         </is>
       </c>
       <c r="C64" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D64" t="n">
         <v>4</v>
@@ -2449,10 +2473,10 @@
         </is>
       </c>
       <c r="C65" s="2" t="n">
-        <v>45406</v>
+        <v>45435</v>
       </c>
       <c r="D65" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E65" t="b">
         <v>0</v>
@@ -2461,9 +2485,11 @@
         <v>0</v>
       </c>
       <c r="G65" t="n">
-        <v>0</v>
-      </c>
-      <c r="H65" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H65" t="n">
+        <v>0</v>
+      </c>
       <c r="I65" t="inlineStr"/>
       <c r="J65" t="inlineStr"/>
     </row>
@@ -2479,7 +2505,7 @@
         </is>
       </c>
       <c r="C66" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D66" t="n">
         <v>5</v>
@@ -2511,7 +2537,7 @@
         </is>
       </c>
       <c r="C67" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D67" t="n">
         <v>2</v>
@@ -2543,7 +2569,7 @@
         </is>
       </c>
       <c r="C68" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D68" t="n">
         <v>4</v>
@@ -2573,7 +2599,7 @@
         </is>
       </c>
       <c r="C69" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D69" t="n">
         <v>4</v>
@@ -2603,7 +2629,7 @@
         </is>
       </c>
       <c r="C70" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D70" t="n">
         <v>7</v>
@@ -2633,7 +2659,7 @@
         </is>
       </c>
       <c r="C71" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D71" t="n">
         <v>1</v>
@@ -2665,7 +2691,7 @@
         </is>
       </c>
       <c r="C72" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D72" t="n">
         <v>5</v>
@@ -2697,7 +2723,7 @@
         </is>
       </c>
       <c r="C73" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D73" t="n">
         <v>8</v>
@@ -2729,7 +2755,7 @@
         </is>
       </c>
       <c r="C74" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D74" t="n">
         <v>3</v>
@@ -2759,7 +2785,7 @@
         </is>
       </c>
       <c r="C75" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D75" t="n">
         <v>4</v>
@@ -2791,7 +2817,7 @@
         </is>
       </c>
       <c r="C76" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D76" t="n">
         <v>2</v>
@@ -2821,7 +2847,7 @@
         </is>
       </c>
       <c r="C77" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D77" t="n">
         <v>3</v>
@@ -2851,7 +2877,7 @@
         </is>
       </c>
       <c r="C78" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D78" t="n">
         <v>7</v>
@@ -2881,7 +2907,7 @@
         </is>
       </c>
       <c r="C79" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D79" t="n">
         <v>5</v>
@@ -2913,7 +2939,7 @@
         </is>
       </c>
       <c r="C80" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D80" t="n">
         <v>7</v>
@@ -2943,7 +2969,7 @@
         </is>
       </c>
       <c r="C81" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D81" t="n">
         <v>7</v>
@@ -2973,7 +2999,7 @@
         </is>
       </c>
       <c r="C82" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D82" t="n">
         <v>8</v>
@@ -3005,7 +3031,7 @@
         </is>
       </c>
       <c r="C83" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D83" t="n">
         <v>4</v>
@@ -3037,7 +3063,7 @@
         </is>
       </c>
       <c r="C84" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D84" t="n">
         <v>4</v>
@@ -3067,7 +3093,7 @@
         </is>
       </c>
       <c r="C85" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D85" t="n">
         <v>4</v>
@@ -3097,7 +3123,7 @@
         </is>
       </c>
       <c r="C86" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D86" t="n">
         <v>3</v>
@@ -3127,7 +3153,7 @@
         </is>
       </c>
       <c r="C87" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D87" t="n">
         <v>3</v>
@@ -3157,21 +3183,23 @@
         </is>
       </c>
       <c r="C88" s="2" t="n">
-        <v>45406</v>
+        <v>45436</v>
       </c>
       <c r="D88" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E88" t="b">
         <v>0</v>
       </c>
       <c r="F88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G88" t="n">
-        <v>0</v>
-      </c>
-      <c r="H88" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H88" t="n">
+        <v>1</v>
+      </c>
       <c r="I88" t="inlineStr"/>
       <c r="J88" t="inlineStr"/>
     </row>
@@ -3187,7 +3215,7 @@
         </is>
       </c>
       <c r="C89" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D89" t="n">
         <v>7</v>
@@ -3217,7 +3245,7 @@
         </is>
       </c>
       <c r="C90" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D90" t="n">
         <v>4</v>
@@ -3249,7 +3277,7 @@
         </is>
       </c>
       <c r="C91" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D91" t="n">
         <v>4</v>
@@ -3279,7 +3307,7 @@
         </is>
       </c>
       <c r="C92" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D92" t="n">
         <v>7</v>
@@ -3309,7 +3337,7 @@
         </is>
       </c>
       <c r="C93" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D93" t="n">
         <v>4</v>
@@ -3339,7 +3367,7 @@
         </is>
       </c>
       <c r="C94" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D94" t="n">
         <v>4</v>
@@ -3369,7 +3397,7 @@
         </is>
       </c>
       <c r="C95" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D95" t="n">
         <v>3</v>
@@ -3399,7 +3427,7 @@
         </is>
       </c>
       <c r="C96" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D96" t="n">
         <v>3</v>
@@ -3429,7 +3457,7 @@
         </is>
       </c>
       <c r="C97" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D97" t="n">
         <v>0</v>
@@ -3459,10 +3487,10 @@
         </is>
       </c>
       <c r="C98" s="2" t="n">
-        <v>45406</v>
+        <v>45409</v>
       </c>
       <c r="D98" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E98" t="b">
         <v>0</v>
@@ -3471,9 +3499,11 @@
         <v>0</v>
       </c>
       <c r="G98" t="n">
-        <v>0</v>
-      </c>
-      <c r="H98" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H98" t="b">
+        <v>0</v>
+      </c>
       <c r="I98" t="inlineStr"/>
       <c r="J98" t="inlineStr"/>
     </row>
@@ -3489,7 +3519,7 @@
         </is>
       </c>
       <c r="C99" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D99" t="n">
         <v>5</v>
@@ -3519,7 +3549,7 @@
         </is>
       </c>
       <c r="C100" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D100" t="n">
         <v>2</v>
@@ -3551,10 +3581,10 @@
         </is>
       </c>
       <c r="C101" s="2" t="n">
-        <v>45406</v>
+        <v>45422</v>
       </c>
       <c r="D101" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E101" t="b">
         <v>0</v>
@@ -3563,9 +3593,11 @@
         <v>0</v>
       </c>
       <c r="G101" t="n">
-        <v>0</v>
-      </c>
-      <c r="H101" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H101" t="b">
+        <v>0</v>
+      </c>
       <c r="I101" t="inlineStr"/>
       <c r="J101" t="inlineStr"/>
     </row>
@@ -3581,7 +3613,7 @@
         </is>
       </c>
       <c r="C102" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D102" t="n">
         <v>1</v>
@@ -3611,7 +3643,7 @@
         </is>
       </c>
       <c r="C103" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D103" t="n">
         <v>4</v>
@@ -3675,7 +3707,7 @@
         </is>
       </c>
       <c r="C105" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D105" t="n">
         <v>5</v>
@@ -3707,7 +3739,7 @@
         </is>
       </c>
       <c r="C106" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D106" t="n">
         <v>3</v>
@@ -3737,7 +3769,7 @@
         </is>
       </c>
       <c r="C107" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D107" t="n">
         <v>5</v>
@@ -3767,7 +3799,7 @@
         </is>
       </c>
       <c r="C108" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D108" t="n">
         <v>8</v>
@@ -3797,7 +3829,7 @@
         </is>
       </c>
       <c r="C109" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D109" t="n">
         <v>3</v>
@@ -3827,7 +3859,7 @@
         </is>
       </c>
       <c r="C110" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D110" t="n">
         <v>1</v>
@@ -3859,21 +3891,23 @@
         </is>
       </c>
       <c r="C111" s="2" t="n">
-        <v>45406</v>
+        <v>45409</v>
       </c>
       <c r="D111" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E111" t="b">
         <v>0</v>
       </c>
       <c r="F111" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G111" t="n">
-        <v>0</v>
-      </c>
-      <c r="H111" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H111" t="n">
+        <v>1</v>
+      </c>
       <c r="I111" t="inlineStr"/>
       <c r="J111" t="inlineStr"/>
     </row>
@@ -3889,10 +3923,10 @@
         </is>
       </c>
       <c r="C112" s="2" t="n">
-        <v>45406</v>
+        <v>45408</v>
       </c>
       <c r="D112" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E112" t="b">
         <v>0</v>
@@ -3901,9 +3935,11 @@
         <v>0</v>
       </c>
       <c r="G112" t="n">
-        <v>0</v>
-      </c>
-      <c r="H112" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H112" t="b">
+        <v>0</v>
+      </c>
       <c r="I112" t="inlineStr"/>
       <c r="J112" t="inlineStr"/>
     </row>
@@ -3919,7 +3955,7 @@
         </is>
       </c>
       <c r="C113" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D113" t="n">
         <v>5</v>
@@ -3949,7 +3985,7 @@
         </is>
       </c>
       <c r="C114" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D114" t="n">
         <v>3</v>
@@ -3979,7 +4015,7 @@
         </is>
       </c>
       <c r="C115" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D115" t="n">
         <v>4</v>
@@ -4009,7 +4045,7 @@
         </is>
       </c>
       <c r="C116" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D116" t="n">
         <v>4</v>
@@ -4039,24 +4075,26 @@
         </is>
       </c>
       <c r="C117" s="2" t="n">
-        <v>45406</v>
+        <v>45433</v>
       </c>
       <c r="D117" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E117" t="b">
         <v>0</v>
       </c>
       <c r="F117" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G117" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H117" t="n">
         <v>1</v>
       </c>
-      <c r="I117" t="inlineStr"/>
+      <c r="I117" t="n">
+        <v>1</v>
+      </c>
       <c r="J117" t="inlineStr"/>
     </row>
     <row r="118">
@@ -4071,7 +4109,7 @@
         </is>
       </c>
       <c r="C118" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D118" t="n">
         <v>2</v>
@@ -4103,7 +4141,7 @@
         </is>
       </c>
       <c r="C119" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D119" t="n">
         <v>5</v>
@@ -4135,7 +4173,7 @@
         </is>
       </c>
       <c r="C120" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D120" t="n">
         <v>7</v>
@@ -4165,7 +4203,7 @@
         </is>
       </c>
       <c r="C121" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D121" t="n">
         <v>4</v>
@@ -4195,10 +4233,10 @@
         </is>
       </c>
       <c r="C122" s="2" t="n">
-        <v>45406</v>
+        <v>45409</v>
       </c>
       <c r="D122" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E122" t="b">
         <v>0</v>
@@ -4207,9 +4245,11 @@
         <v>0</v>
       </c>
       <c r="G122" t="n">
-        <v>0</v>
-      </c>
-      <c r="H122" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H122" t="b">
+        <v>0</v>
+      </c>
       <c r="I122" t="inlineStr"/>
       <c r="J122" t="inlineStr"/>
     </row>
@@ -4225,10 +4265,10 @@
         </is>
       </c>
       <c r="C123" s="2" t="n">
-        <v>45406</v>
+        <v>45411</v>
       </c>
       <c r="D123" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E123" t="b">
         <v>0</v>
@@ -4237,9 +4277,11 @@
         <v>0</v>
       </c>
       <c r="G123" t="n">
-        <v>0</v>
-      </c>
-      <c r="H123" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H123" t="n">
+        <v>0</v>
+      </c>
       <c r="I123" t="inlineStr"/>
       <c r="J123" t="inlineStr"/>
     </row>
@@ -4255,7 +4297,7 @@
         </is>
       </c>
       <c r="C124" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D124" t="n">
         <v>3</v>
@@ -4285,24 +4327,26 @@
         </is>
       </c>
       <c r="C125" s="2" t="n">
-        <v>45406</v>
+        <v>45411</v>
       </c>
       <c r="D125" t="n">
+        <v>3</v>
+      </c>
+      <c r="E125" t="b">
+        <v>0</v>
+      </c>
+      <c r="F125" t="n">
         <v>2</v>
       </c>
-      <c r="E125" t="b">
-        <v>0</v>
-      </c>
-      <c r="F125" t="n">
-        <v>1</v>
-      </c>
       <c r="G125" t="n">
-        <v>1</v>
-      </c>
-      <c r="H125" t="n">
-        <v>1</v>
-      </c>
-      <c r="I125" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="H125" t="b">
+        <v>1</v>
+      </c>
+      <c r="I125" t="n">
+        <v>1</v>
+      </c>
       <c r="J125" t="inlineStr"/>
     </row>
     <row r="126">
@@ -4317,21 +4361,23 @@
         </is>
       </c>
       <c r="C126" s="2" t="n">
-        <v>45406</v>
+        <v>45422</v>
       </c>
       <c r="D126" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E126" t="b">
         <v>0</v>
       </c>
       <c r="F126" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G126" t="n">
-        <v>0</v>
-      </c>
-      <c r="H126" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H126" t="n">
+        <v>1</v>
+      </c>
       <c r="I126" t="inlineStr"/>
       <c r="J126" t="inlineStr"/>
     </row>
@@ -4347,7 +4393,7 @@
         </is>
       </c>
       <c r="C127" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D127" t="n">
         <v>7</v>
@@ -4377,7 +4423,7 @@
         </is>
       </c>
       <c r="C128" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D128" t="n">
         <v>8</v>
@@ -4409,7 +4455,7 @@
         </is>
       </c>
       <c r="C129" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D129" t="n">
         <v>5</v>
@@ -4441,7 +4487,7 @@
         </is>
       </c>
       <c r="C130" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D130" t="n">
         <v>4</v>
@@ -4473,7 +4519,7 @@
         </is>
       </c>
       <c r="C131" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D131" t="n">
         <v>7</v>
@@ -4503,21 +4549,23 @@
         </is>
       </c>
       <c r="C132" s="2" t="n">
-        <v>45406</v>
+        <v>45433</v>
       </c>
       <c r="D132" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E132" t="b">
         <v>0</v>
       </c>
       <c r="F132" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G132" t="n">
-        <v>0</v>
-      </c>
-      <c r="H132" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H132" t="n">
+        <v>1</v>
+      </c>
       <c r="I132" t="inlineStr"/>
       <c r="J132" t="inlineStr"/>
     </row>
@@ -4533,7 +4581,7 @@
         </is>
       </c>
       <c r="C133" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D133" t="n">
         <v>4</v>
@@ -4577,7 +4625,7 @@
       <c r="G134" t="n">
         <v>3</v>
       </c>
-      <c r="H134" t="b">
+      <c r="H134" t="n">
         <v>1</v>
       </c>
       <c r="I134" t="n">
@@ -4599,7 +4647,7 @@
         </is>
       </c>
       <c r="C135" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D135" t="n">
         <v>3</v>
@@ -4666,7 +4714,7 @@
         </is>
       </c>
       <c r="C137" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D137" t="n">
         <v>0</v>
@@ -4698,7 +4746,7 @@
         </is>
       </c>
       <c r="C138" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D138" t="n">
         <v>4</v>
@@ -4760,7 +4808,7 @@
         </is>
       </c>
       <c r="C140" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D140" t="n">
         <v>0</v>
@@ -4791,24 +4839,26 @@
         </is>
       </c>
       <c r="C141" s="2" t="n">
-        <v>45406</v>
+        <v>45433</v>
       </c>
       <c r="D141" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E141" t="b">
         <v>0</v>
       </c>
       <c r="F141" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G141" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H141" t="n">
         <v>1</v>
       </c>
-      <c r="I141" t="inlineStr"/>
+      <c r="I141" t="n">
+        <v>1</v>
+      </c>
       <c r="J141" t="inlineStr"/>
     </row>
     <row r="142">
@@ -4825,21 +4875,23 @@
         </is>
       </c>
       <c r="C142" s="2" t="n">
-        <v>45406</v>
+        <v>45422</v>
       </c>
       <c r="D142" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E142" t="b">
         <v>0</v>
       </c>
       <c r="F142" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G142" t="n">
-        <v>0</v>
-      </c>
-      <c r="H142" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H142" t="n">
+        <v>1</v>
+      </c>
       <c r="I142" t="inlineStr"/>
       <c r="J142" t="inlineStr"/>
     </row>
@@ -4857,10 +4909,10 @@
         </is>
       </c>
       <c r="C143" s="2" t="n">
-        <v>45406</v>
+        <v>45408</v>
       </c>
       <c r="D143" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E143" t="b">
         <v>0</v>
@@ -4869,15 +4921,17 @@
         <v>1</v>
       </c>
       <c r="G143" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H143" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I143" t="n">
-        <v>0</v>
-      </c>
-      <c r="J143" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="J143" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -4893,10 +4947,10 @@
         </is>
       </c>
       <c r="C144" s="2" t="n">
-        <v>45406</v>
+        <v>45408</v>
       </c>
       <c r="D144" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E144" t="b">
         <v>0</v>
@@ -4905,16 +4959,16 @@
         <v>2</v>
       </c>
       <c r="G144" t="n">
-        <v>3</v>
-      </c>
-      <c r="H144" t="n">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="H144" t="b">
+        <v>0</v>
       </c>
       <c r="I144" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J144" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145">
@@ -4929,7 +4983,7 @@
         </is>
       </c>
       <c r="C145" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D145" t="n">
         <v>2</v>
@@ -4959,7 +5013,7 @@
         </is>
       </c>
       <c r="C146" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D146" t="n">
         <v>5</v>
@@ -4992,7 +5046,7 @@
         </is>
       </c>
       <c r="C147" s="2" t="n">
-        <v>45406</v>
+        <v>45408</v>
       </c>
       <c r="D147" t="n">
         <v>0</v>
@@ -5004,9 +5058,11 @@
         <v>0</v>
       </c>
       <c r="G147" t="n">
-        <v>0</v>
-      </c>
-      <c r="H147" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H147" t="n">
+        <v>0</v>
+      </c>
       <c r="I147" t="inlineStr"/>
       <c r="J147" t="inlineStr"/>
     </row>
@@ -5024,19 +5080,19 @@
         </is>
       </c>
       <c r="C148" s="2" t="n">
-        <v>45406</v>
+        <v>45433</v>
       </c>
       <c r="D148" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E148" t="b">
         <v>0</v>
       </c>
       <c r="F148" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G148" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H148" t="n">
         <v>1</v>
@@ -5044,7 +5100,9 @@
       <c r="I148" t="n">
         <v>1</v>
       </c>
-      <c r="J148" t="inlineStr"/>
+      <c r="J148" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -5058,7 +5116,7 @@
         </is>
       </c>
       <c r="C149" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D149" t="n">
         <v>2</v>
@@ -5088,10 +5146,10 @@
         </is>
       </c>
       <c r="C150" s="2" t="n">
-        <v>45406</v>
+        <v>45409</v>
       </c>
       <c r="D150" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E150" t="b">
         <v>0</v>
@@ -5100,12 +5158,14 @@
         <v>1</v>
       </c>
       <c r="G150" t="n">
-        <v>1</v>
-      </c>
-      <c r="H150" t="n">
-        <v>1</v>
-      </c>
-      <c r="I150" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="H150" t="b">
+        <v>0</v>
+      </c>
+      <c r="I150" t="n">
+        <v>1</v>
+      </c>
       <c r="J150" t="inlineStr"/>
     </row>
     <row r="151">
@@ -5120,7 +5180,7 @@
         </is>
       </c>
       <c r="C151" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D151" t="n">
         <v>5</v>
@@ -5153,7 +5213,7 @@
         </is>
       </c>
       <c r="C152" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D152" t="n">
         <v>4</v>
@@ -5186,7 +5246,7 @@
         </is>
       </c>
       <c r="C153" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D153" t="n">
         <v>3</v>
@@ -5217,7 +5277,7 @@
         </is>
       </c>
       <c r="C154" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D154" t="n">
         <v>2</v>
@@ -5249,7 +5309,7 @@
         </is>
       </c>
       <c r="C155" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D155" t="n">
         <v>1</v>
@@ -5281,7 +5341,7 @@
         </is>
       </c>
       <c r="C156" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D156" t="n">
         <v>0</v>
@@ -5312,7 +5372,7 @@
         </is>
       </c>
       <c r="C157" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D157" t="n">
         <v>4</v>
@@ -5344,7 +5404,7 @@
         </is>
       </c>
       <c r="C158" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D158" t="n">
         <v>3</v>
@@ -5375,7 +5435,7 @@
         </is>
       </c>
       <c r="C159" s="2" t="n">
-        <v>45406</v>
+        <v>45408</v>
       </c>
       <c r="D159" t="n">
         <v>0</v>
@@ -5387,12 +5447,14 @@
         <v>0</v>
       </c>
       <c r="G159" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H159" t="n">
         <v>0</v>
       </c>
-      <c r="I159" t="inlineStr"/>
+      <c r="I159" t="n">
+        <v>0</v>
+      </c>
       <c r="J159" t="inlineStr"/>
     </row>
     <row r="160">
@@ -5409,7 +5471,7 @@
         </is>
       </c>
       <c r="C160" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D160" t="n">
         <v>5</v>
@@ -5442,7 +5504,7 @@
         </is>
       </c>
       <c r="C161" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D161" t="n">
         <v>2</v>
@@ -5473,7 +5535,7 @@
         </is>
       </c>
       <c r="C162" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D162" t="n">
         <v>4</v>
@@ -5505,7 +5567,7 @@
         </is>
       </c>
       <c r="C163" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D163" t="n">
         <v>2</v>
@@ -5537,7 +5599,7 @@
         </is>
       </c>
       <c r="C164" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D164" t="n">
         <v>4</v>
@@ -5603,7 +5665,7 @@
         </is>
       </c>
       <c r="C166" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D166" t="n">
         <v>0</v>
@@ -5635,7 +5697,7 @@
         </is>
       </c>
       <c r="C167" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D167" t="n">
         <v>4</v>
@@ -5668,7 +5730,7 @@
         </is>
       </c>
       <c r="C168" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D168" t="n">
         <v>0</v>
@@ -5700,21 +5762,23 @@
         </is>
       </c>
       <c r="C169" s="2" t="n">
-        <v>45406</v>
+        <v>45433</v>
       </c>
       <c r="D169" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E169" t="b">
         <v>0</v>
       </c>
       <c r="F169" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G169" t="n">
-        <v>0</v>
-      </c>
-      <c r="H169" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H169" t="n">
+        <v>1</v>
+      </c>
       <c r="I169" t="inlineStr"/>
       <c r="J169" t="inlineStr"/>
     </row>
@@ -5730,7 +5794,7 @@
         </is>
       </c>
       <c r="C170" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D170" t="n">
         <v>4</v>
@@ -5761,7 +5825,7 @@
         </is>
       </c>
       <c r="C171" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D171" t="n">
         <v>0</v>
@@ -5791,7 +5855,7 @@
         </is>
       </c>
       <c r="C172" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D172" t="n">
         <v>1</v>
@@ -5823,7 +5887,7 @@
         </is>
       </c>
       <c r="C173" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D173" t="n">
         <v>1</v>
@@ -5853,7 +5917,7 @@
         </is>
       </c>
       <c r="C174" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D174" t="n">
         <v>4</v>
@@ -5883,10 +5947,10 @@
         </is>
       </c>
       <c r="C175" s="2" t="n">
-        <v>45406</v>
+        <v>45411</v>
       </c>
       <c r="D175" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E175" t="b">
         <v>0</v>
@@ -5895,9 +5959,11 @@
         <v>0</v>
       </c>
       <c r="G175" t="n">
-        <v>0</v>
-      </c>
-      <c r="H175" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H175" t="n">
+        <v>0</v>
+      </c>
       <c r="I175" t="inlineStr"/>
       <c r="J175" t="inlineStr"/>
     </row>
@@ -5913,7 +5979,7 @@
         </is>
       </c>
       <c r="C176" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D176" t="n">
         <v>3</v>
@@ -5943,10 +6009,10 @@
         </is>
       </c>
       <c r="C177" s="2" t="n">
-        <v>45406</v>
+        <v>45409</v>
       </c>
       <c r="D177" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E177" t="b">
         <v>0</v>
@@ -5955,9 +6021,11 @@
         <v>0</v>
       </c>
       <c r="G177" t="n">
-        <v>0</v>
-      </c>
-      <c r="H177" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H177" t="n">
+        <v>0</v>
+      </c>
       <c r="I177" t="inlineStr"/>
       <c r="J177" t="inlineStr"/>
     </row>
@@ -6005,10 +6073,10 @@
         </is>
       </c>
       <c r="C179" s="2" t="n">
-        <v>45406</v>
+        <v>45411</v>
       </c>
       <c r="D179" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E179" t="b">
         <v>0</v>
@@ -6017,15 +6085,17 @@
         <v>2</v>
       </c>
       <c r="G179" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H179" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I179" t="n">
         <v>1</v>
       </c>
-      <c r="J179" t="inlineStr"/>
+      <c r="J179" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -6039,7 +6109,7 @@
         </is>
       </c>
       <c r="C180" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D180" t="n">
         <v>2</v>
@@ -6069,7 +6139,7 @@
         </is>
       </c>
       <c r="C181" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D181" t="n">
         <v>3</v>
@@ -6099,7 +6169,7 @@
         </is>
       </c>
       <c r="C182" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D182" t="n">
         <v>4</v>
@@ -6129,7 +6199,7 @@
         </is>
       </c>
       <c r="C183" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D183" t="n">
         <v>2</v>
@@ -6159,7 +6229,7 @@
         </is>
       </c>
       <c r="C184" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D184" t="n">
         <v>0</v>
@@ -6192,7 +6262,7 @@
         </is>
       </c>
       <c r="C185" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D185" t="n">
         <v>2</v>
@@ -6222,7 +6292,7 @@
         </is>
       </c>
       <c r="C186" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D186" t="n">
         <v>4</v>
@@ -6252,21 +6322,23 @@
         </is>
       </c>
       <c r="C187" s="2" t="n">
-        <v>45406</v>
+        <v>45433</v>
       </c>
       <c r="D187" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E187" t="b">
         <v>0</v>
       </c>
       <c r="F187" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G187" t="n">
-        <v>0</v>
-      </c>
-      <c r="H187" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H187" t="b">
+        <v>1</v>
+      </c>
       <c r="I187" t="inlineStr"/>
       <c r="J187" t="inlineStr"/>
     </row>
@@ -6282,7 +6354,7 @@
         </is>
       </c>
       <c r="C188" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D188" t="n">
         <v>4</v>
@@ -6312,7 +6384,7 @@
         </is>
       </c>
       <c r="C189" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D189" t="n">
         <v>3</v>
@@ -6342,7 +6414,7 @@
         </is>
       </c>
       <c r="C190" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D190" t="n">
         <v>3</v>
@@ -6372,7 +6444,7 @@
         </is>
       </c>
       <c r="C191" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D191" t="n">
         <v>4</v>
@@ -6402,7 +6474,7 @@
         </is>
       </c>
       <c r="C192" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D192" t="n">
         <v>3</v>
@@ -6432,7 +6504,7 @@
         </is>
       </c>
       <c r="C193" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D193" t="n">
         <v>2</v>
@@ -6464,7 +6536,7 @@
         </is>
       </c>
       <c r="C194" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D194" t="n">
         <v>4</v>
@@ -6497,7 +6569,7 @@
         </is>
       </c>
       <c r="C195" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D195" t="n">
         <v>2</v>
@@ -6527,7 +6599,7 @@
         </is>
       </c>
       <c r="C196" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D196" t="n">
         <v>4</v>
@@ -6591,21 +6663,23 @@
         </is>
       </c>
       <c r="C198" s="2" t="n">
-        <v>45406</v>
+        <v>45433</v>
       </c>
       <c r="D198" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E198" t="b">
         <v>0</v>
       </c>
       <c r="F198" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G198" t="n">
-        <v>0</v>
-      </c>
-      <c r="H198" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H198" t="b">
+        <v>1</v>
+      </c>
       <c r="I198" t="inlineStr"/>
       <c r="J198" t="inlineStr"/>
     </row>
@@ -6621,7 +6695,7 @@
         </is>
       </c>
       <c r="C199" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D199" t="n">
         <v>3</v>
@@ -6651,7 +6725,7 @@
         </is>
       </c>
       <c r="C200" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D200" t="n">
         <v>2</v>
@@ -6681,7 +6755,7 @@
         </is>
       </c>
       <c r="C201" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D201" t="n">
         <v>1</v>
@@ -6745,7 +6819,7 @@
         </is>
       </c>
       <c r="C203" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D203" t="n">
         <v>3</v>
@@ -6775,7 +6849,7 @@
         </is>
       </c>
       <c r="C204" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D204" t="n">
         <v>0</v>
@@ -6805,7 +6879,7 @@
         </is>
       </c>
       <c r="C205" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D205" t="n">
         <v>0</v>
@@ -6837,7 +6911,7 @@
         </is>
       </c>
       <c r="C206" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D206" t="n">
         <v>2</v>
@@ -6871,7 +6945,7 @@
         </is>
       </c>
       <c r="C207" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D207" t="n">
         <v>0</v>
@@ -6901,7 +6975,7 @@
         </is>
       </c>
       <c r="C208" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D208" t="n">
         <v>1</v>
@@ -6933,24 +7007,26 @@
         </is>
       </c>
       <c r="C209" s="2" t="n">
-        <v>45406</v>
+        <v>45408</v>
       </c>
       <c r="D209" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E209" t="b">
         <v>0</v>
       </c>
       <c r="F209" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G209" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H209" t="n">
-        <v>0</v>
-      </c>
-      <c r="I209" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="I209" t="n">
+        <v>0</v>
+      </c>
       <c r="J209" t="inlineStr"/>
     </row>
     <row r="210">
@@ -6965,10 +7041,10 @@
         </is>
       </c>
       <c r="C210" s="2" t="n">
-        <v>45406</v>
+        <v>45422</v>
       </c>
       <c r="D210" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E210" t="b">
         <v>0</v>
@@ -6977,12 +7053,14 @@
         <v>1</v>
       </c>
       <c r="G210" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H210" t="n">
-        <v>1</v>
-      </c>
-      <c r="I210" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="I210" t="n">
+        <v>1</v>
+      </c>
       <c r="J210" t="inlineStr"/>
     </row>
     <row r="211">
@@ -6997,7 +7075,7 @@
         </is>
       </c>
       <c r="C211" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D211" t="n">
         <v>2</v>
@@ -7027,7 +7105,7 @@
         </is>
       </c>
       <c r="C212" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D212" t="n">
         <v>5</v>
@@ -7091,21 +7169,23 @@
         </is>
       </c>
       <c r="C214" s="2" t="n">
-        <v>45406</v>
+        <v>45411</v>
       </c>
       <c r="D214" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E214" t="b">
         <v>0</v>
       </c>
       <c r="F214" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G214" t="n">
-        <v>0</v>
-      </c>
-      <c r="H214" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H214" t="n">
+        <v>1</v>
+      </c>
       <c r="I214" t="inlineStr"/>
       <c r="J214" t="inlineStr"/>
     </row>
@@ -7135,7 +7215,7 @@
       <c r="G215" t="n">
         <v>3</v>
       </c>
-      <c r="H215" t="b">
+      <c r="H215" t="n">
         <v>1</v>
       </c>
       <c r="I215" t="n">
@@ -7157,7 +7237,7 @@
         </is>
       </c>
       <c r="C216" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D216" t="n">
         <v>2</v>
@@ -7187,21 +7267,23 @@
         </is>
       </c>
       <c r="C217" s="2" t="n">
-        <v>45406</v>
+        <v>45409</v>
       </c>
       <c r="D217" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E217" t="b">
         <v>0</v>
       </c>
       <c r="F217" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G217" t="n">
-        <v>0</v>
-      </c>
-      <c r="H217" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H217" t="b">
+        <v>1</v>
+      </c>
       <c r="I217" t="inlineStr"/>
       <c r="J217" t="inlineStr"/>
     </row>
@@ -7219,7 +7301,7 @@
         </is>
       </c>
       <c r="C218" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D218" t="n">
         <v>1</v>
@@ -7253,7 +7335,7 @@
         </is>
       </c>
       <c r="C219" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D219" t="n">
         <v>5</v>
@@ -7285,7 +7367,7 @@
         </is>
       </c>
       <c r="C220" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D220" t="n">
         <v>5</v>
@@ -7317,7 +7399,7 @@
         </is>
       </c>
       <c r="C221" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D221" t="n">
         <v>1</v>
@@ -7351,7 +7433,7 @@
         </is>
       </c>
       <c r="C222" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D222" t="n">
         <v>3</v>
@@ -7382,7 +7464,7 @@
         </is>
       </c>
       <c r="C223" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D223" t="n">
         <v>1</v>
@@ -7414,7 +7496,7 @@
         </is>
       </c>
       <c r="C224" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D224" t="n">
         <v>0</v>
@@ -7444,7 +7526,7 @@
         </is>
       </c>
       <c r="C225" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D225" t="n">
         <v>2</v>
@@ -7477,7 +7559,7 @@
         </is>
       </c>
       <c r="C226" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D226" t="n">
         <v>2</v>
@@ -7507,7 +7589,7 @@
         </is>
       </c>
       <c r="C227" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D227" t="n">
         <v>4</v>
@@ -7555,7 +7637,7 @@
       <c r="G228" t="n">
         <v>1</v>
       </c>
-      <c r="H228" t="b">
+      <c r="H228" t="n">
         <v>0</v>
       </c>
       <c r="I228" t="inlineStr"/>
@@ -7573,7 +7655,7 @@
         </is>
       </c>
       <c r="C229" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D229" t="n">
         <v>4</v>
@@ -7603,7 +7685,7 @@
         </is>
       </c>
       <c r="C230" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D230" t="n">
         <v>3</v>
@@ -7668,7 +7750,7 @@
         </is>
       </c>
       <c r="C232" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D232" t="n">
         <v>0</v>
@@ -7698,7 +7780,7 @@
         </is>
       </c>
       <c r="C233" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D233" t="n">
         <v>2</v>
@@ -7730,7 +7812,7 @@
         </is>
       </c>
       <c r="C234" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D234" t="n">
         <v>3</v>
@@ -7762,7 +7844,7 @@
         </is>
       </c>
       <c r="C235" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D235" t="n">
         <v>2</v>
@@ -7793,10 +7875,10 @@
         </is>
       </c>
       <c r="C236" s="2" t="n">
-        <v>45406</v>
+        <v>45409</v>
       </c>
       <c r="D236" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E236" t="b">
         <v>0</v>
@@ -7805,9 +7887,11 @@
         <v>0</v>
       </c>
       <c r="G236" t="n">
-        <v>0</v>
-      </c>
-      <c r="H236" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H236" t="b">
+        <v>0</v>
+      </c>
       <c r="I236" t="inlineStr"/>
       <c r="J236" t="inlineStr"/>
     </row>
@@ -7823,7 +7907,7 @@
         </is>
       </c>
       <c r="C237" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D237" t="n">
         <v>4</v>
@@ -7855,7 +7939,7 @@
         </is>
       </c>
       <c r="C238" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D238" t="n">
         <v>1</v>
@@ -7885,7 +7969,7 @@
         </is>
       </c>
       <c r="C239" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D239" t="n">
         <v>2</v>
@@ -7915,7 +7999,7 @@
         </is>
       </c>
       <c r="C240" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D240" t="n">
         <v>1</v>
@@ -7945,21 +8029,23 @@
         </is>
       </c>
       <c r="C241" s="2" t="n">
-        <v>45406</v>
+        <v>45422</v>
       </c>
       <c r="D241" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E241" t="b">
         <v>0</v>
       </c>
       <c r="F241" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G241" t="n">
-        <v>0</v>
-      </c>
-      <c r="H241" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H241" t="n">
+        <v>1</v>
+      </c>
       <c r="I241" t="inlineStr"/>
       <c r="J241" t="inlineStr"/>
     </row>
@@ -7975,7 +8061,7 @@
         </is>
       </c>
       <c r="C242" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D242" t="n">
         <v>2</v>
@@ -8005,7 +8091,7 @@
         </is>
       </c>
       <c r="C243" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D243" t="n">
         <v>2</v>
@@ -8035,7 +8121,7 @@
         </is>
       </c>
       <c r="C244" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D244" t="n">
         <v>4</v>
@@ -8068,7 +8154,7 @@
         </is>
       </c>
       <c r="C245" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D245" t="n">
         <v>1</v>
@@ -8102,7 +8188,7 @@
         </is>
       </c>
       <c r="C246" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D246" t="n">
         <v>0</v>
@@ -8132,7 +8218,7 @@
         </is>
       </c>
       <c r="C247" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D247" t="n">
         <v>3</v>
@@ -8164,7 +8250,7 @@
         </is>
       </c>
       <c r="C248" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D248" t="n">
         <v>0</v>
@@ -8196,10 +8282,10 @@
         </is>
       </c>
       <c r="C249" s="2" t="n">
-        <v>45406</v>
+        <v>45409</v>
       </c>
       <c r="D249" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E249" t="b">
         <v>0</v>
@@ -8208,9 +8294,11 @@
         <v>0</v>
       </c>
       <c r="G249" t="n">
-        <v>0</v>
-      </c>
-      <c r="H249" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H249" t="n">
+        <v>0</v>
+      </c>
       <c r="I249" t="inlineStr"/>
       <c r="J249" t="inlineStr"/>
     </row>
@@ -8226,7 +8314,7 @@
         </is>
       </c>
       <c r="C250" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D250" t="n">
         <v>0</v>
@@ -8256,7 +8344,7 @@
         </is>
       </c>
       <c r="C251" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D251" t="n">
         <v>1</v>
@@ -8288,7 +8376,7 @@
         </is>
       </c>
       <c r="C252" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D252" t="n">
         <v>3</v>
@@ -8321,7 +8409,7 @@
         </is>
       </c>
       <c r="C253" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D253" t="n">
         <v>0</v>
@@ -8355,7 +8443,7 @@
         </is>
       </c>
       <c r="C254" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D254" t="n">
         <v>2</v>
@@ -8385,7 +8473,7 @@
         </is>
       </c>
       <c r="C255" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D255" t="n">
         <v>0</v>
@@ -8415,7 +8503,7 @@
         </is>
       </c>
       <c r="C256" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D256" t="n">
         <v>3</v>
@@ -8445,24 +8533,26 @@
         </is>
       </c>
       <c r="C257" s="2" t="n">
-        <v>45407</v>
+        <v>45422</v>
       </c>
       <c r="D257" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E257" t="b">
         <v>0</v>
       </c>
       <c r="F257" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G257" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H257" t="n">
-        <v>0</v>
-      </c>
-      <c r="I257" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="I257" t="n">
+        <v>0</v>
+      </c>
       <c r="J257" t="inlineStr"/>
     </row>
     <row r="258">
@@ -8477,24 +8567,26 @@
         </is>
       </c>
       <c r="C258" s="2" t="n">
-        <v>45406</v>
+        <v>45409</v>
       </c>
       <c r="D258" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E258" t="b">
         <v>0</v>
       </c>
       <c r="F258" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G258" t="n">
-        <v>1</v>
-      </c>
-      <c r="H258" t="n">
-        <v>1</v>
-      </c>
-      <c r="I258" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="H258" t="b">
+        <v>1</v>
+      </c>
+      <c r="I258" t="n">
+        <v>1</v>
+      </c>
       <c r="J258" t="inlineStr"/>
     </row>
     <row r="259">
@@ -8509,27 +8601,29 @@
         </is>
       </c>
       <c r="C259" s="2" t="n">
-        <v>45406</v>
+        <v>45422</v>
       </c>
       <c r="D259" t="n">
+        <v>4</v>
+      </c>
+      <c r="E259" t="b">
+        <v>0</v>
+      </c>
+      <c r="F259" t="n">
         <v>3</v>
       </c>
-      <c r="E259" t="b">
-        <v>0</v>
-      </c>
-      <c r="F259" t="n">
-        <v>2</v>
-      </c>
       <c r="G259" t="n">
-        <v>2</v>
-      </c>
-      <c r="H259" t="n">
+        <v>3</v>
+      </c>
+      <c r="H259" t="b">
         <v>1</v>
       </c>
       <c r="I259" t="n">
         <v>1</v>
       </c>
-      <c r="J259" t="inlineStr"/>
+      <c r="J259" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
@@ -8543,7 +8637,7 @@
         </is>
       </c>
       <c r="C260" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D260" t="n">
         <v>3</v>
@@ -8575,10 +8669,10 @@
         </is>
       </c>
       <c r="C261" s="2" t="n">
-        <v>45406</v>
+        <v>45408</v>
       </c>
       <c r="D261" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E261" t="b">
         <v>0</v>
@@ -8587,9 +8681,11 @@
         <v>0</v>
       </c>
       <c r="G261" t="n">
-        <v>0</v>
-      </c>
-      <c r="H261" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H261" t="n">
+        <v>0</v>
+      </c>
       <c r="I261" t="inlineStr"/>
       <c r="J261" t="inlineStr"/>
     </row>
@@ -8605,7 +8701,7 @@
         </is>
       </c>
       <c r="C262" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D262" t="n">
         <v>2</v>
@@ -8635,7 +8731,7 @@
         </is>
       </c>
       <c r="C263" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D263" t="n">
         <v>0</v>
@@ -8665,21 +8761,23 @@
         </is>
       </c>
       <c r="C264" s="2" t="n">
-        <v>45406</v>
+        <v>45409</v>
       </c>
       <c r="D264" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E264" t="b">
         <v>0</v>
       </c>
       <c r="F264" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G264" t="n">
-        <v>0</v>
-      </c>
-      <c r="H264" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H264" t="n">
+        <v>1</v>
+      </c>
       <c r="I264" t="inlineStr"/>
       <c r="J264" t="inlineStr"/>
     </row>
@@ -8695,7 +8793,7 @@
         </is>
       </c>
       <c r="C265" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D265" t="n">
         <v>0</v>
@@ -8727,7 +8825,7 @@
         </is>
       </c>
       <c r="C266" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D266" t="n">
         <v>3</v>
@@ -8757,7 +8855,7 @@
         </is>
       </c>
       <c r="C267" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D267" t="n">
         <v>4</v>
@@ -8787,7 +8885,7 @@
         </is>
       </c>
       <c r="C268" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D268" t="n">
         <v>3</v>
@@ -8819,7 +8917,7 @@
         </is>
       </c>
       <c r="C269" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D269" t="n">
         <v>4</v>
@@ -8849,7 +8947,7 @@
         </is>
       </c>
       <c r="C270" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D270" t="n">
         <v>2</v>
@@ -8880,7 +8978,7 @@
         </is>
       </c>
       <c r="C271" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D271" t="n">
         <v>4</v>
@@ -8910,7 +9008,7 @@
         </is>
       </c>
       <c r="C272" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D272" t="n">
         <v>4</v>
@@ -8942,7 +9040,7 @@
         </is>
       </c>
       <c r="C273" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D273" t="n">
         <v>0</v>
@@ -8974,7 +9072,7 @@
         </is>
       </c>
       <c r="C274" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D274" t="n">
         <v>0</v>
@@ -9004,7 +9102,7 @@
         </is>
       </c>
       <c r="C275" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D275" t="n">
         <v>0</v>
@@ -9036,7 +9134,7 @@
         </is>
       </c>
       <c r="C276" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D276" t="n">
         <v>0</v>
@@ -9066,7 +9164,7 @@
         </is>
       </c>
       <c r="C277" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D277" t="n">
         <v>2</v>
@@ -9099,7 +9197,7 @@
         </is>
       </c>
       <c r="C278" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D278" t="n">
         <v>0</v>
@@ -9132,7 +9230,7 @@
         </is>
       </c>
       <c r="C279" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D279" t="n">
         <v>2</v>
@@ -9165,7 +9263,7 @@
         </is>
       </c>
       <c r="C280" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D280" t="n">
         <v>0</v>
@@ -9195,7 +9293,7 @@
         </is>
       </c>
       <c r="C281" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D281" t="n">
         <v>2</v>
@@ -9225,7 +9323,7 @@
         </is>
       </c>
       <c r="C282" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D282" t="n">
         <v>0</v>
@@ -9255,24 +9353,26 @@
         </is>
       </c>
       <c r="C283" s="2" t="n">
-        <v>45406</v>
+        <v>45408</v>
       </c>
       <c r="D283" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E283" t="b">
         <v>0</v>
       </c>
       <c r="F283" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G283" t="n">
-        <v>1</v>
-      </c>
-      <c r="H283" t="n">
-        <v>0</v>
-      </c>
-      <c r="I283" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="H283" t="b">
+        <v>1</v>
+      </c>
+      <c r="I283" t="n">
+        <v>0</v>
+      </c>
       <c r="J283" t="inlineStr"/>
     </row>
     <row r="284">
@@ -9288,24 +9388,26 @@
         </is>
       </c>
       <c r="C284" s="2" t="n">
-        <v>45406</v>
+        <v>45408</v>
       </c>
       <c r="D284" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E284" t="b">
         <v>0</v>
       </c>
       <c r="F284" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G284" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H284" t="n">
-        <v>0</v>
-      </c>
-      <c r="I284" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="I284" t="n">
+        <v>0</v>
+      </c>
       <c r="J284" t="inlineStr"/>
     </row>
     <row r="285">
@@ -9321,7 +9423,7 @@
         </is>
       </c>
       <c r="C285" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D285" t="n">
         <v>3</v>
@@ -9353,7 +9455,7 @@
         </is>
       </c>
       <c r="C286" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D286" t="n">
         <v>4</v>
@@ -9387,7 +9489,7 @@
         </is>
       </c>
       <c r="C287" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D287" t="n">
         <v>0</v>
@@ -9419,7 +9521,7 @@
         </is>
       </c>
       <c r="C288" s="2" t="n">
-        <v>45406</v>
+        <v>45408</v>
       </c>
       <c r="D288" t="n">
         <v>1</v>
@@ -9431,9 +9533,11 @@
         <v>0</v>
       </c>
       <c r="G288" t="n">
-        <v>0</v>
-      </c>
-      <c r="H288" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H288" t="n">
+        <v>0</v>
+      </c>
       <c r="I288" t="inlineStr"/>
       <c r="J288" t="inlineStr"/>
     </row>
@@ -9450,7 +9554,7 @@
         </is>
       </c>
       <c r="C289" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D289" t="n">
         <v>5</v>
@@ -9482,7 +9586,7 @@
         </is>
       </c>
       <c r="C290" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D290" t="n">
         <v>0</v>
@@ -9512,7 +9616,7 @@
         </is>
       </c>
       <c r="C291" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D291" t="n">
         <v>1</v>
@@ -9542,7 +9646,7 @@
         </is>
       </c>
       <c r="C292" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D292" t="n">
         <v>0</v>
@@ -9573,7 +9677,7 @@
         </is>
       </c>
       <c r="C293" s="2" t="n">
-        <v>45406</v>
+        <v>45408</v>
       </c>
       <c r="D293" t="n">
         <v>0</v>
@@ -9585,9 +9689,11 @@
         <v>0</v>
       </c>
       <c r="G293" t="n">
-        <v>0</v>
-      </c>
-      <c r="H293" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H293" t="b">
+        <v>0</v>
+      </c>
       <c r="I293" t="inlineStr"/>
       <c r="J293" t="inlineStr"/>
     </row>
@@ -9604,7 +9710,7 @@
         </is>
       </c>
       <c r="C294" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D294" t="n">
         <v>3</v>
@@ -9637,7 +9743,7 @@
         </is>
       </c>
       <c r="C295" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D295" t="n">
         <v>0</v>
@@ -9667,27 +9773,29 @@
         </is>
       </c>
       <c r="C296" s="2" t="n">
-        <v>45406</v>
+        <v>45408</v>
       </c>
       <c r="D296" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E296" t="b">
         <v>0</v>
       </c>
       <c r="F296" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G296" t="n">
-        <v>2</v>
-      </c>
-      <c r="H296" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="H296" t="b">
+        <v>1</v>
       </c>
       <c r="I296" t="n">
         <v>0</v>
       </c>
-      <c r="J296" t="inlineStr"/>
+      <c r="J296" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
@@ -9701,7 +9809,7 @@
         </is>
       </c>
       <c r="C297" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D297" t="n">
         <v>0</v>
@@ -9733,7 +9841,7 @@
         </is>
       </c>
       <c r="C298" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D298" t="n">
         <v>3</v>
@@ -9763,10 +9871,10 @@
         </is>
       </c>
       <c r="C299" s="2" t="n">
-        <v>45406</v>
+        <v>45409</v>
       </c>
       <c r="D299" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E299" t="b">
         <v>0</v>
@@ -9775,9 +9883,11 @@
         <v>0</v>
       </c>
       <c r="G299" t="n">
-        <v>0</v>
-      </c>
-      <c r="H299" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H299" t="n">
+        <v>0</v>
+      </c>
       <c r="I299" t="inlineStr"/>
       <c r="J299" t="inlineStr"/>
     </row>
@@ -9794,7 +9904,7 @@
         </is>
       </c>
       <c r="C300" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D300" t="n">
         <v>4</v>
@@ -9827,7 +9937,7 @@
         </is>
       </c>
       <c r="C301" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D301" t="n">
         <v>2</v>
@@ -9861,7 +9971,7 @@
         </is>
       </c>
       <c r="C302" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D302" t="n">
         <v>2</v>
@@ -9895,7 +10005,7 @@
         </is>
       </c>
       <c r="C303" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D303" t="n">
         <v>1</v>
@@ -9926,10 +10036,10 @@
         </is>
       </c>
       <c r="C304" s="2" t="n">
-        <v>45406</v>
+        <v>45411</v>
       </c>
       <c r="D304" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E304" t="b">
         <v>0</v>
@@ -9938,9 +10048,11 @@
         <v>0</v>
       </c>
       <c r="G304" t="n">
-        <v>0</v>
-      </c>
-      <c r="H304" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H304" t="n">
+        <v>0</v>
+      </c>
       <c r="I304" t="inlineStr"/>
       <c r="J304" t="inlineStr"/>
     </row>
@@ -9957,7 +10069,7 @@
         </is>
       </c>
       <c r="C305" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D305" t="n">
         <v>0</v>
@@ -9990,7 +10102,7 @@
         </is>
       </c>
       <c r="C306" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D306" t="n">
         <v>0</v>
@@ -10034,7 +10146,7 @@
       <c r="G307" t="n">
         <v>3</v>
       </c>
-      <c r="H307" t="b">
+      <c r="H307" t="n">
         <v>0</v>
       </c>
       <c r="I307" t="n">
@@ -10056,7 +10168,7 @@
         </is>
       </c>
       <c r="C308" s="2" t="n">
-        <v>45406</v>
+        <v>45408</v>
       </c>
       <c r="D308" t="n">
         <v>0</v>
@@ -10068,9 +10180,11 @@
         <v>0</v>
       </c>
       <c r="G308" t="n">
-        <v>0</v>
-      </c>
-      <c r="H308" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H308" t="b">
+        <v>0</v>
+      </c>
       <c r="I308" t="inlineStr"/>
       <c r="J308" t="inlineStr"/>
     </row>
@@ -10086,27 +10200,29 @@
         </is>
       </c>
       <c r="C309" s="2" t="n">
-        <v>45406</v>
+        <v>45409</v>
       </c>
       <c r="D309" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E309" t="b">
         <v>0</v>
       </c>
       <c r="F309" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G309" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H309" t="n">
         <v>1</v>
       </c>
       <c r="I309" t="n">
-        <v>0</v>
-      </c>
-      <c r="J309" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="J309" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
@@ -10121,7 +10237,7 @@
         </is>
       </c>
       <c r="C310" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D310" t="n">
         <v>4</v>
@@ -10153,7 +10269,7 @@
         </is>
       </c>
       <c r="C311" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D311" t="n">
         <v>1</v>
@@ -10187,7 +10303,7 @@
         </is>
       </c>
       <c r="C312" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D312" t="n">
         <v>0</v>
@@ -10219,7 +10335,7 @@
         </is>
       </c>
       <c r="C313" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D313" t="n">
         <v>3</v>
@@ -10250,7 +10366,7 @@
         </is>
       </c>
       <c r="C314" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D314" t="n">
         <v>2</v>
@@ -10283,7 +10399,7 @@
         </is>
       </c>
       <c r="C315" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D315" t="n">
         <v>4</v>
@@ -10348,7 +10464,7 @@
         </is>
       </c>
       <c r="C317" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D317" t="n">
         <v>2</v>
@@ -10378,7 +10494,7 @@
         </is>
       </c>
       <c r="C318" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D318" t="n">
         <v>0</v>
@@ -10410,27 +10526,29 @@
         </is>
       </c>
       <c r="C319" s="2" t="n">
-        <v>45406</v>
+        <v>45408</v>
       </c>
       <c r="D319" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E319" t="b">
         <v>0</v>
       </c>
       <c r="F319" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G319" t="n">
-        <v>2</v>
-      </c>
-      <c r="H319" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="H319" t="b">
+        <v>1</v>
       </c>
       <c r="I319" t="n">
         <v>0</v>
       </c>
-      <c r="J319" t="inlineStr"/>
+      <c r="J319" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
@@ -10445,7 +10563,7 @@
         </is>
       </c>
       <c r="C320" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D320" t="n">
         <v>1</v>
@@ -10481,7 +10599,7 @@
         </is>
       </c>
       <c r="C321" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D321" t="n">
         <v>1</v>
@@ -10515,7 +10633,7 @@
         </is>
       </c>
       <c r="C322" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D322" t="n">
         <v>4</v>
@@ -10546,7 +10664,7 @@
         </is>
       </c>
       <c r="C323" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D323" t="n">
         <v>2</v>
@@ -10582,7 +10700,7 @@
         </is>
       </c>
       <c r="C324" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D324" t="n">
         <v>1</v>
@@ -10649,7 +10767,7 @@
         </is>
       </c>
       <c r="C326" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D326" t="n">
         <v>1</v>
@@ -10682,7 +10800,7 @@
         </is>
       </c>
       <c r="C327" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D327" t="n">
         <v>3</v>
@@ -10717,7 +10835,7 @@
         </is>
       </c>
       <c r="C328" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D328" t="n">
         <v>0</v>
@@ -10747,7 +10865,7 @@
         </is>
       </c>
       <c r="C329" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D329" t="n">
         <v>0</v>
@@ -10777,7 +10895,7 @@
         </is>
       </c>
       <c r="C330" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D330" t="n">
         <v>2</v>
@@ -10812,7 +10930,7 @@
         </is>
       </c>
       <c r="C331" s="2" t="n">
-        <v>45406</v>
+        <v>45408</v>
       </c>
       <c r="D331" t="n">
         <v>0</v>
@@ -10824,12 +10942,14 @@
         <v>0</v>
       </c>
       <c r="G331" t="n">
-        <v>1</v>
-      </c>
-      <c r="H331" t="n">
-        <v>0</v>
-      </c>
-      <c r="I331" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="H331" t="b">
+        <v>0</v>
+      </c>
+      <c r="I331" t="n">
+        <v>0</v>
+      </c>
       <c r="J331" t="inlineStr"/>
     </row>
     <row r="332">
@@ -10844,7 +10964,7 @@
         </is>
       </c>
       <c r="C332" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D332" t="n">
         <v>2</v>
@@ -10879,7 +10999,7 @@
         </is>
       </c>
       <c r="C333" s="2" t="n">
-        <v>45406</v>
+        <v>45408</v>
       </c>
       <c r="D333" t="n">
         <v>0</v>
@@ -10891,9 +11011,11 @@
         <v>0</v>
       </c>
       <c r="G333" t="n">
-        <v>0</v>
-      </c>
-      <c r="H333" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H333" t="n">
+        <v>0</v>
+      </c>
       <c r="I333" t="inlineStr"/>
       <c r="J333" t="inlineStr"/>
     </row>
@@ -10909,7 +11031,7 @@
         </is>
       </c>
       <c r="C334" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D334" t="n">
         <v>3</v>
@@ -10940,7 +11062,7 @@
         </is>
       </c>
       <c r="C335" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D335" t="n">
         <v>0</v>
@@ -10970,21 +11092,23 @@
         </is>
       </c>
       <c r="C336" s="2" t="n">
-        <v>45406</v>
+        <v>45408</v>
       </c>
       <c r="D336" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E336" t="b">
         <v>0</v>
       </c>
       <c r="F336" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G336" t="n">
-        <v>0</v>
-      </c>
-      <c r="H336" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H336" t="b">
+        <v>1</v>
+      </c>
       <c r="I336" t="inlineStr"/>
       <c r="J336" t="inlineStr"/>
     </row>
@@ -11000,7 +11124,7 @@
         </is>
       </c>
       <c r="C337" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D337" t="n">
         <v>2</v>
@@ -11032,7 +11156,7 @@
         </is>
       </c>
       <c r="C338" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D338" t="n">
         <v>0</v>
@@ -11064,7 +11188,7 @@
         </is>
       </c>
       <c r="C339" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D339" t="n">
         <v>0</v>
@@ -11094,10 +11218,10 @@
         </is>
       </c>
       <c r="C340" s="2" t="n">
-        <v>45406</v>
+        <v>45411</v>
       </c>
       <c r="D340" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E340" t="b">
         <v>0</v>
@@ -11106,12 +11230,14 @@
         <v>1</v>
       </c>
       <c r="G340" t="n">
-        <v>1</v>
-      </c>
-      <c r="H340" t="n">
-        <v>1</v>
-      </c>
-      <c r="I340" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="H340" t="b">
+        <v>0</v>
+      </c>
+      <c r="I340" t="n">
+        <v>1</v>
+      </c>
       <c r="J340" t="inlineStr"/>
     </row>
     <row r="341">
@@ -11126,7 +11252,7 @@
         </is>
       </c>
       <c r="C341" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D341" t="n">
         <v>4</v>
@@ -11158,7 +11284,7 @@
         </is>
       </c>
       <c r="C342" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D342" t="n">
         <v>4</v>
@@ -11188,7 +11314,7 @@
         </is>
       </c>
       <c r="C343" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D343" t="n">
         <v>3</v>
@@ -11218,7 +11344,7 @@
         </is>
       </c>
       <c r="C344" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D344" t="n">
         <v>4</v>
@@ -11251,24 +11377,26 @@
         </is>
       </c>
       <c r="C345" s="2" t="n">
-        <v>45406</v>
+        <v>45411</v>
       </c>
       <c r="D345" t="n">
+        <v>3</v>
+      </c>
+      <c r="E345" t="b">
+        <v>0</v>
+      </c>
+      <c r="F345" t="n">
+        <v>1</v>
+      </c>
+      <c r="G345" t="n">
         <v>2</v>
       </c>
-      <c r="E345" t="b">
-        <v>0</v>
-      </c>
-      <c r="F345" t="n">
-        <v>0</v>
-      </c>
-      <c r="G345" t="n">
-        <v>1</v>
-      </c>
-      <c r="H345" t="n">
-        <v>0</v>
-      </c>
-      <c r="I345" t="inlineStr"/>
+      <c r="H345" t="b">
+        <v>1</v>
+      </c>
+      <c r="I345" t="n">
+        <v>0</v>
+      </c>
       <c r="J345" t="inlineStr"/>
     </row>
     <row r="346">
@@ -11284,7 +11412,7 @@
         </is>
       </c>
       <c r="C346" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D346" t="n">
         <v>3</v>
@@ -11318,7 +11446,7 @@
         </is>
       </c>
       <c r="C347" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D347" t="n">
         <v>1</v>
@@ -11355,7 +11483,7 @@
         </is>
       </c>
       <c r="C348" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D348" t="n">
         <v>0</v>
@@ -11385,7 +11513,7 @@
         </is>
       </c>
       <c r="C349" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D349" t="n">
         <v>2</v>
@@ -11415,7 +11543,7 @@
         </is>
       </c>
       <c r="C350" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D350" t="n">
         <v>0</v>
@@ -11447,7 +11575,7 @@
         </is>
       </c>
       <c r="C351" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D351" t="n">
         <v>5</v>
@@ -11493,7 +11621,7 @@
       <c r="G352" t="n">
         <v>2</v>
       </c>
-      <c r="H352" t="b">
+      <c r="H352" t="n">
         <v>0</v>
       </c>
       <c r="I352" t="n">
@@ -11513,7 +11641,7 @@
         </is>
       </c>
       <c r="C353" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D353" t="n">
         <v>3</v>
@@ -11543,10 +11671,10 @@
         </is>
       </c>
       <c r="C354" s="2" t="n">
-        <v>45406</v>
+        <v>45408</v>
       </c>
       <c r="D354" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E354" t="b">
         <v>0</v>
@@ -11555,9 +11683,11 @@
         <v>0</v>
       </c>
       <c r="G354" t="n">
-        <v>0</v>
-      </c>
-      <c r="H354" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H354" t="b">
+        <v>0</v>
+      </c>
       <c r="I354" t="inlineStr"/>
       <c r="J354" t="inlineStr"/>
     </row>
@@ -11573,7 +11703,7 @@
         </is>
       </c>
       <c r="C355" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D355" t="n">
         <v>4</v>
@@ -11607,7 +11737,7 @@
         </is>
       </c>
       <c r="C356" s="2" t="n">
-        <v>45406</v>
+        <v>45408</v>
       </c>
       <c r="D356" t="n">
         <v>1</v>
@@ -11619,12 +11749,14 @@
         <v>1</v>
       </c>
       <c r="G356" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H356" t="n">
-        <v>1</v>
-      </c>
-      <c r="I356" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="I356" t="n">
+        <v>1</v>
+      </c>
       <c r="J356" t="inlineStr"/>
     </row>
     <row r="357">
@@ -11640,7 +11772,7 @@
         </is>
       </c>
       <c r="C357" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D357" t="n">
         <v>4</v>
@@ -11670,7 +11802,7 @@
         </is>
       </c>
       <c r="C358" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D358" t="n">
         <v>0</v>
@@ -11702,21 +11834,23 @@
         </is>
       </c>
       <c r="C359" s="2" t="n">
-        <v>45406</v>
+        <v>45433</v>
       </c>
       <c r="D359" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E359" t="b">
         <v>0</v>
       </c>
       <c r="F359" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G359" t="n">
-        <v>0</v>
-      </c>
-      <c r="H359" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H359" t="n">
+        <v>1</v>
+      </c>
       <c r="I359" t="inlineStr"/>
       <c r="J359" t="inlineStr"/>
     </row>
@@ -11733,7 +11867,7 @@
         </is>
       </c>
       <c r="C360" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D360" t="n">
         <v>0</v>
@@ -11765,7 +11899,7 @@
         </is>
       </c>
       <c r="C361" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D361" t="n">
         <v>4</v>
@@ -11795,7 +11929,7 @@
         </is>
       </c>
       <c r="C362" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D362" t="n">
         <v>0</v>
@@ -11827,7 +11961,7 @@
         </is>
       </c>
       <c r="C363" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D363" t="n">
         <v>3</v>
@@ -11859,24 +11993,26 @@
         </is>
       </c>
       <c r="C364" s="2" t="n">
-        <v>45406</v>
+        <v>45408</v>
       </c>
       <c r="D364" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E364" t="b">
         <v>0</v>
       </c>
       <c r="F364" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G364" t="n">
-        <v>1</v>
-      </c>
-      <c r="H364" t="n">
-        <v>0</v>
-      </c>
-      <c r="I364" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="H364" t="b">
+        <v>1</v>
+      </c>
+      <c r="I364" t="n">
+        <v>0</v>
+      </c>
       <c r="J364" t="inlineStr"/>
     </row>
     <row r="365">
@@ -11894,7 +12030,7 @@
         </is>
       </c>
       <c r="C365" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D365" t="n">
         <v>2</v>
@@ -11926,7 +12062,7 @@
         </is>
       </c>
       <c r="C366" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D366" t="n">
         <v>0</v>
@@ -11958,7 +12094,7 @@
         </is>
       </c>
       <c r="C367" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D367" t="n">
         <v>0</v>
@@ -11989,7 +12125,7 @@
         </is>
       </c>
       <c r="C368" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D368" t="n">
         <v>3</v>
@@ -12019,7 +12155,7 @@
         </is>
       </c>
       <c r="C369" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D369" t="n">
         <v>1</v>
@@ -12053,7 +12189,7 @@
         </is>
       </c>
       <c r="C370" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D370" t="n">
         <v>3</v>
@@ -12085,7 +12221,7 @@
         </is>
       </c>
       <c r="C371" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D371" t="n">
         <v>1</v>
@@ -12118,7 +12254,7 @@
         </is>
       </c>
       <c r="C372" s="2" t="n">
-        <v>45406</v>
+        <v>45408</v>
       </c>
       <c r="D372" t="n">
         <v>0</v>
@@ -12130,12 +12266,14 @@
         <v>0</v>
       </c>
       <c r="G372" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H372" t="n">
         <v>0</v>
       </c>
-      <c r="I372" t="inlineStr"/>
+      <c r="I372" t="n">
+        <v>0</v>
+      </c>
       <c r="J372" t="inlineStr"/>
     </row>
     <row r="373">
@@ -12150,7 +12288,7 @@
         </is>
       </c>
       <c r="C373" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D373" t="n">
         <v>1</v>
@@ -12180,7 +12318,7 @@
         </is>
       </c>
       <c r="C374" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D374" t="n">
         <v>3</v>
@@ -12210,7 +12348,7 @@
         </is>
       </c>
       <c r="C375" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D375" t="n">
         <v>3</v>
@@ -12241,7 +12379,7 @@
         </is>
       </c>
       <c r="C376" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D376" t="n">
         <v>0</v>
@@ -12271,7 +12409,7 @@
         </is>
       </c>
       <c r="C377" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D377" t="n">
         <v>1</v>
@@ -12303,24 +12441,26 @@
         </is>
       </c>
       <c r="C378" s="2" t="n">
-        <v>45406</v>
+        <v>45408</v>
       </c>
       <c r="D378" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E378" t="b">
         <v>0</v>
       </c>
       <c r="F378" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G378" t="n">
-        <v>1</v>
-      </c>
-      <c r="H378" t="n">
-        <v>0</v>
-      </c>
-      <c r="I378" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="H378" t="b">
+        <v>1</v>
+      </c>
+      <c r="I378" t="n">
+        <v>0</v>
+      </c>
       <c r="J378" t="inlineStr"/>
     </row>
     <row r="379">
@@ -12349,7 +12489,7 @@
       <c r="G379" t="n">
         <v>1</v>
       </c>
-      <c r="H379" t="b">
+      <c r="H379" t="n">
         <v>1</v>
       </c>
       <c r="I379" t="inlineStr"/>
@@ -12368,21 +12508,23 @@
         </is>
       </c>
       <c r="C380" s="2" t="n">
-        <v>45406</v>
+        <v>45409</v>
       </c>
       <c r="D380" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E380" t="b">
         <v>0</v>
       </c>
       <c r="F380" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G380" t="n">
-        <v>0</v>
-      </c>
-      <c r="H380" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H380" t="n">
+        <v>1</v>
+      </c>
       <c r="I380" t="inlineStr"/>
       <c r="J380" t="inlineStr"/>
     </row>
@@ -12398,7 +12540,7 @@
         </is>
       </c>
       <c r="C381" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D381" t="n">
         <v>0</v>
@@ -12428,21 +12570,23 @@
         </is>
       </c>
       <c r="C382" s="2" t="n">
-        <v>45406</v>
+        <v>45408</v>
       </c>
       <c r="D382" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E382" t="b">
         <v>0</v>
       </c>
       <c r="F382" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G382" t="n">
-        <v>0</v>
-      </c>
-      <c r="H382" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H382" t="n">
+        <v>1</v>
+      </c>
       <c r="I382" t="inlineStr"/>
       <c r="J382" t="inlineStr"/>
     </row>
@@ -12458,7 +12602,7 @@
         </is>
       </c>
       <c r="C383" s="2" t="n">
-        <v>45406</v>
+        <v>45407</v>
       </c>
       <c r="D383" t="n">
         <v>4</v>

</xml_diff>